<commit_message>
create a class for tecidos
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/TC_02.xlsx
+++ b/EXCEL LIBS/TC_02.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DEV\rexbot_01\EXCEL LIBS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DEV\rexbot_v1.2\rexBot\EXCEL LIBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6550,7 +6550,7 @@
     <t>PARIS TERRACOTA</t>
   </si>
   <si>
-    <t>Lista Produto : 13-12-2019 10:32:27</t>
+    <t>Lista Produto : 03-01-2020 11:23:29</t>
   </si>
 </sst>
 </file>
@@ -7009,8 +7009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S964"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H617" workbookViewId="0">
-      <selection activeCell="Q930" sqref="Q930"/>
+    <sheetView tabSelected="1" topLeftCell="A929" workbookViewId="0">
+      <selection activeCell="C960" sqref="C960"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16926,7 +16926,7 @@
         <v>358</v>
       </c>
       <c r="Q169" s="6">
-        <v>76.5</v>
+        <v>84</v>
       </c>
       <c r="R169" s="6" t="s">
         <v>23</v>
@@ -17221,7 +17221,7 @@
         <v>368</v>
       </c>
       <c r="Q174" s="6">
-        <v>5283.92</v>
+        <v>3210.95</v>
       </c>
       <c r="R174" s="6" t="s">
         <v>23</v>
@@ -17457,7 +17457,7 @@
         <v>376</v>
       </c>
       <c r="Q178" s="6">
-        <v>1376.3936000000001</v>
+        <v>982.05359999999996</v>
       </c>
       <c r="R178" s="6" t="s">
         <v>23</v>
@@ -17516,7 +17516,7 @@
         <v>378</v>
       </c>
       <c r="Q179" s="6">
-        <v>1071.2</v>
+        <v>736.34</v>
       </c>
       <c r="R179" s="6" t="s">
         <v>23</v>
@@ -17988,7 +17988,7 @@
         <v>394</v>
       </c>
       <c r="Q187" s="6">
-        <v>8897.3799999999992</v>
+        <v>8419.09</v>
       </c>
       <c r="R187" s="6" t="s">
         <v>23</v>
@@ -18342,7 +18342,7 @@
         <v>406</v>
       </c>
       <c r="Q193" s="6">
-        <v>960</v>
+        <v>1934</v>
       </c>
       <c r="R193" s="6" t="s">
         <v>23</v>
@@ -19050,7 +19050,7 @@
         <v>430</v>
       </c>
       <c r="Q205" s="6">
-        <v>445.54</v>
+        <v>78.23</v>
       </c>
       <c r="R205" s="6" t="s">
         <v>23</v>
@@ -19109,7 +19109,7 @@
         <v>432</v>
       </c>
       <c r="Q206" s="6">
-        <v>3829.4</v>
+        <v>3661.8</v>
       </c>
       <c r="R206" s="6" t="s">
         <v>23</v>
@@ -19286,7 +19286,7 @@
         <v>438</v>
       </c>
       <c r="Q209" s="6">
-        <v>3529.58</v>
+        <v>3529.36</v>
       </c>
       <c r="R209" s="6" t="s">
         <v>23</v>
@@ -20053,7 +20053,7 @@
         <v>464</v>
       </c>
       <c r="Q222" s="6">
-        <v>6874.2650000000003</v>
+        <v>5236.7622000000001</v>
       </c>
       <c r="R222" s="6" t="s">
         <v>23</v>
@@ -20348,7 +20348,7 @@
         <v>474</v>
       </c>
       <c r="Q227" s="6">
-        <v>11075.2</v>
+        <v>9230.36</v>
       </c>
       <c r="R227" s="6" t="s">
         <v>23</v>
@@ -20407,7 +20407,7 @@
         <v>476</v>
       </c>
       <c r="Q228" s="6">
-        <v>8392.34</v>
+        <v>6435.94</v>
       </c>
       <c r="R228" s="6" t="s">
         <v>23</v>
@@ -21115,7 +21115,7 @@
         <v>500</v>
       </c>
       <c r="Q240" s="6">
-        <v>6086.44</v>
+        <v>6084.82</v>
       </c>
       <c r="R240" s="6" t="s">
         <v>23</v>
@@ -21528,7 +21528,7 @@
         <v>514</v>
       </c>
       <c r="Q247" s="6">
-        <v>1868.33</v>
+        <v>1398.42</v>
       </c>
       <c r="R247" s="6" t="s">
         <v>23</v>
@@ -21587,7 +21587,7 @@
         <v>516</v>
       </c>
       <c r="Q248" s="6">
-        <v>2290.46</v>
+        <v>2740.34</v>
       </c>
       <c r="R248" s="6" t="s">
         <v>23</v>
@@ -21764,7 +21764,7 @@
         <v>522</v>
       </c>
       <c r="Q251" s="6">
-        <v>2591.31</v>
+        <v>2015.91</v>
       </c>
       <c r="R251" s="6" t="s">
         <v>23</v>
@@ -22590,7 +22590,7 @@
         <v>550</v>
       </c>
       <c r="Q265" s="6">
-        <v>2803.55</v>
+        <v>2612.8000000000002</v>
       </c>
       <c r="R265" s="6" t="s">
         <v>23</v>
@@ -22649,7 +22649,7 @@
         <v>552</v>
       </c>
       <c r="Q266" s="6">
-        <v>6414.3</v>
+        <v>6064.63</v>
       </c>
       <c r="R266" s="6" t="s">
         <v>23</v>
@@ -22885,7 +22885,7 @@
         <v>561</v>
       </c>
       <c r="Q270" s="6">
-        <v>479.12</v>
+        <v>478.46</v>
       </c>
       <c r="R270" s="6" t="s">
         <v>23</v>
@@ -23298,7 +23298,7 @@
         <v>575</v>
       </c>
       <c r="Q277" s="6">
-        <v>1861.7</v>
+        <v>1830.38</v>
       </c>
       <c r="R277" s="6" t="s">
         <v>23</v>
@@ -23829,7 +23829,7 @@
         <v>593</v>
       </c>
       <c r="Q286" s="6">
-        <v>1220.8</v>
+        <v>1162.4000000000001</v>
       </c>
       <c r="R286" s="6" t="s">
         <v>23</v>
@@ -23888,7 +23888,7 @@
         <v>595</v>
       </c>
       <c r="Q287" s="6">
-        <v>3901.53</v>
+        <v>3342.69</v>
       </c>
       <c r="R287" s="6" t="s">
         <v>23</v>
@@ -24065,7 +24065,7 @@
         <v>601</v>
       </c>
       <c r="Q290" s="6">
-        <v>4024</v>
+        <v>3997.8</v>
       </c>
       <c r="R290" s="6" t="s">
         <v>23</v>
@@ -24124,7 +24124,7 @@
         <v>603</v>
       </c>
       <c r="Q291" s="6">
-        <v>8003.1549999999997</v>
+        <v>6553.2340000000004</v>
       </c>
       <c r="R291" s="6" t="s">
         <v>23</v>
@@ -24183,7 +24183,7 @@
         <v>605</v>
       </c>
       <c r="Q292" s="6">
-        <v>377.41</v>
+        <v>326.83</v>
       </c>
       <c r="R292" s="6" t="s">
         <v>23</v>
@@ -24478,7 +24478,7 @@
         <v>615</v>
       </c>
       <c r="Q297" s="6">
-        <v>3698.06</v>
+        <v>3604.41</v>
       </c>
       <c r="R297" s="6" t="s">
         <v>23</v>
@@ -24596,7 +24596,7 @@
         <v>619</v>
       </c>
       <c r="Q299" s="6">
-        <v>1273.4000000000001</v>
+        <v>1187.5999999999999</v>
       </c>
       <c r="R299" s="6" t="s">
         <v>23</v>
@@ -24655,7 +24655,7 @@
         <v>621</v>
       </c>
       <c r="Q300" s="6">
-        <v>2175.88</v>
+        <v>2158.0500000000002</v>
       </c>
       <c r="R300" s="6" t="s">
         <v>23</v>
@@ -24714,7 +24714,7 @@
         <v>623</v>
       </c>
       <c r="Q301" s="6">
-        <v>1112.31</v>
+        <v>1100.29</v>
       </c>
       <c r="R301" s="6" t="s">
         <v>23</v>
@@ -24773,7 +24773,7 @@
         <v>625</v>
       </c>
       <c r="Q302" s="6">
-        <v>4583.6000000000004</v>
+        <v>4550.6000000000004</v>
       </c>
       <c r="R302" s="6" t="s">
         <v>23</v>
@@ -24832,7 +24832,7 @@
         <v>627</v>
       </c>
       <c r="Q303" s="6">
-        <v>8697.09</v>
+        <v>7960</v>
       </c>
       <c r="R303" s="6" t="s">
         <v>23</v>
@@ -24891,7 +24891,7 @@
         <v>629</v>
       </c>
       <c r="Q304" s="6">
-        <v>51077.741000000002</v>
+        <v>63033.591</v>
       </c>
       <c r="R304" s="6" t="s">
         <v>23</v>
@@ -24950,7 +24950,7 @@
         <v>631</v>
       </c>
       <c r="Q305" s="6">
-        <v>1274.0999999999999</v>
+        <v>1204.9000000000001</v>
       </c>
       <c r="R305" s="6" t="s">
         <v>23</v>
@@ -25009,7 +25009,7 @@
         <v>633</v>
       </c>
       <c r="Q306" s="6">
-        <v>4640.8100000000004</v>
+        <v>4538.87</v>
       </c>
       <c r="R306" s="6" t="s">
         <v>23</v>
@@ -25304,7 +25304,7 @@
         <v>643</v>
       </c>
       <c r="Q311" s="6">
-        <v>138.6</v>
+        <v>134.32</v>
       </c>
       <c r="R311" s="6" t="s">
         <v>23</v>
@@ -25363,7 +25363,7 @@
         <v>646</v>
       </c>
       <c r="Q312" s="6">
-        <v>4261.95</v>
+        <v>4244.45</v>
       </c>
       <c r="R312" s="6" t="s">
         <v>23</v>
@@ -25422,7 +25422,7 @@
         <v>649</v>
       </c>
       <c r="Q313" s="6">
-        <v>472.04</v>
+        <v>414.44</v>
       </c>
       <c r="R313" s="6" t="s">
         <v>23</v>
@@ -25481,7 +25481,7 @@
         <v>652</v>
       </c>
       <c r="Q314" s="6">
-        <v>2409.98</v>
+        <v>2371.58</v>
       </c>
       <c r="R314" s="6" t="s">
         <v>23</v>
@@ -25599,7 +25599,7 @@
         <v>658</v>
       </c>
       <c r="Q316" s="6">
-        <v>375.58</v>
+        <v>352.54</v>
       </c>
       <c r="R316" s="6" t="s">
         <v>23</v>
@@ -25717,7 +25717,7 @@
         <v>662</v>
       </c>
       <c r="Q318" s="6">
-        <v>4001.49</v>
+        <v>3976.81</v>
       </c>
       <c r="R318" s="6" t="s">
         <v>23</v>
@@ -25776,7 +25776,7 @@
         <v>664</v>
       </c>
       <c r="Q319" s="6">
-        <v>12376.7</v>
+        <v>11007.87</v>
       </c>
       <c r="R319" s="6" t="s">
         <v>23</v>
@@ -25835,7 +25835,7 @@
         <v>666</v>
       </c>
       <c r="Q320" s="6">
-        <v>3311.71</v>
+        <v>3300.87</v>
       </c>
       <c r="R320" s="6" t="s">
         <v>23</v>
@@ -25894,7 +25894,7 @@
         <v>668</v>
       </c>
       <c r="Q321" s="6">
-        <v>8621.08</v>
+        <v>8102.05</v>
       </c>
       <c r="R321" s="6" t="s">
         <v>23</v>
@@ -25953,7 +25953,7 @@
         <v>670</v>
       </c>
       <c r="Q322" s="6">
-        <v>3995</v>
+        <v>3851.7</v>
       </c>
       <c r="R322" s="6" t="s">
         <v>23</v>
@@ -26071,7 +26071,7 @@
         <v>674</v>
       </c>
       <c r="Q324" s="6">
-        <v>3072.63</v>
+        <v>3036.5</v>
       </c>
       <c r="R324" s="6" t="s">
         <v>23</v>
@@ -26130,7 +26130,7 @@
         <v>676</v>
       </c>
       <c r="Q325" s="6">
-        <v>4313.4799999999996</v>
+        <v>4297.7996999999996</v>
       </c>
       <c r="R325" s="6" t="s">
         <v>23</v>
@@ -26189,7 +26189,7 @@
         <v>678</v>
       </c>
       <c r="Q326" s="6">
-        <v>570.18269999999995</v>
+        <v>561.79999999999995</v>
       </c>
       <c r="R326" s="6" t="s">
         <v>23</v>
@@ -26307,7 +26307,7 @@
         <v>683</v>
       </c>
       <c r="Q328" s="6">
-        <v>4086.79</v>
+        <v>3856.6</v>
       </c>
       <c r="R328" s="6" t="s">
         <v>23</v>
@@ -26366,7 +26366,7 @@
         <v>686</v>
       </c>
       <c r="Q329" s="6">
-        <v>2322.17</v>
+        <v>2100.11</v>
       </c>
       <c r="R329" s="6" t="s">
         <v>23</v>
@@ -26484,7 +26484,7 @@
         <v>692</v>
       </c>
       <c r="Q331" s="6">
-        <v>2266.2939999999999</v>
+        <v>2267.1</v>
       </c>
       <c r="R331" s="6" t="s">
         <v>23</v>
@@ -26543,7 +26543,7 @@
         <v>694</v>
       </c>
       <c r="Q332" s="6">
-        <v>2432.7694000000001</v>
+        <v>2398.0693999999999</v>
       </c>
       <c r="R332" s="6" t="s">
         <v>23</v>
@@ -26602,7 +26602,7 @@
         <v>697</v>
       </c>
       <c r="Q333" s="6">
-        <v>2169.6</v>
+        <v>2108.1999999999998</v>
       </c>
       <c r="R333" s="6" t="s">
         <v>23</v>
@@ -26661,7 +26661,7 @@
         <v>700</v>
       </c>
       <c r="Q334" s="6">
-        <v>213.47399999999999</v>
+        <v>179.5</v>
       </c>
       <c r="R334" s="6" t="s">
         <v>23</v>
@@ -26720,7 +26720,7 @@
         <v>703</v>
       </c>
       <c r="Q335" s="6">
-        <v>1443.635</v>
+        <v>1430.845</v>
       </c>
       <c r="R335" s="6" t="s">
         <v>23</v>
@@ -26779,7 +26779,7 @@
         <v>706</v>
       </c>
       <c r="Q336" s="6">
-        <v>2848.15</v>
+        <v>2631.57</v>
       </c>
       <c r="R336" s="6" t="s">
         <v>23</v>
@@ -27015,7 +27015,7 @@
         <v>714</v>
       </c>
       <c r="Q340" s="6">
-        <v>162.6</v>
+        <v>282.76</v>
       </c>
       <c r="R340" s="6" t="s">
         <v>23</v>
@@ -27310,7 +27310,7 @@
         <v>724</v>
       </c>
       <c r="Q345" s="6">
-        <v>8208.56</v>
+        <v>7767.56</v>
       </c>
       <c r="R345" s="6" t="s">
         <v>23</v>
@@ -27369,7 +27369,7 @@
         <v>726</v>
       </c>
       <c r="Q346" s="6">
-        <v>1358.54</v>
+        <v>1237.69</v>
       </c>
       <c r="R346" s="6" t="s">
         <v>23</v>
@@ -27428,7 +27428,7 @@
         <v>728</v>
       </c>
       <c r="Q347" s="6">
-        <v>264.2</v>
+        <v>245.7</v>
       </c>
       <c r="R347" s="6" t="s">
         <v>23</v>
@@ -27487,7 +27487,7 @@
         <v>731</v>
       </c>
       <c r="Q348" s="6">
-        <v>525.70000000000005</v>
+        <v>447</v>
       </c>
       <c r="R348" s="6" t="s">
         <v>23</v>
@@ -27546,7 +27546,7 @@
         <v>734</v>
       </c>
       <c r="Q349" s="6">
-        <v>1462.38</v>
+        <v>1469.88</v>
       </c>
       <c r="R349" s="6" t="s">
         <v>23</v>
@@ -27664,7 +27664,7 @@
         <v>738</v>
       </c>
       <c r="Q351" s="6">
-        <v>29866.78</v>
+        <v>29854.52</v>
       </c>
       <c r="R351" s="6" t="s">
         <v>23</v>
@@ -27723,7 +27723,7 @@
         <v>741</v>
       </c>
       <c r="Q352" s="6">
-        <v>3529.65</v>
+        <v>3533.8</v>
       </c>
       <c r="R352" s="6" t="s">
         <v>23</v>
@@ -27841,7 +27841,7 @@
         <v>747</v>
       </c>
       <c r="Q354" s="6">
-        <v>301.7</v>
+        <v>291.89999999999998</v>
       </c>
       <c r="R354" s="6" t="s">
         <v>23</v>
@@ -27900,7 +27900,7 @@
         <v>749</v>
       </c>
       <c r="Q355" s="6">
-        <v>1661.38</v>
+        <v>1625.83</v>
       </c>
       <c r="R355" s="6" t="s">
         <v>23</v>
@@ -28195,7 +28195,7 @@
         <v>759</v>
       </c>
       <c r="Q360" s="6">
-        <v>1642.28</v>
+        <v>1630.78</v>
       </c>
       <c r="R360" s="6" t="s">
         <v>23</v>
@@ -28844,7 +28844,7 @@
         <v>794</v>
       </c>
       <c r="Q371" s="6">
-        <v>3808.31</v>
+        <v>3806.4</v>
       </c>
       <c r="R371" s="6" t="s">
         <v>23</v>
@@ -34980,7 +34980,7 @@
         <v>1004</v>
       </c>
       <c r="Q475" s="6">
-        <v>2346.15</v>
+        <v>1422.85</v>
       </c>
       <c r="R475" s="6" t="s">
         <v>23</v>
@@ -35039,7 +35039,7 @@
         <v>1006</v>
       </c>
       <c r="Q476" s="6">
-        <v>963.9</v>
+        <v>674.77</v>
       </c>
       <c r="R476" s="6" t="s">
         <v>23</v>
@@ -35098,7 +35098,7 @@
         <v>1008</v>
       </c>
       <c r="Q477" s="6">
-        <v>1300</v>
+        <v>1029.4100000000001</v>
       </c>
       <c r="R477" s="6" t="s">
         <v>23</v>
@@ -35157,7 +35157,7 @@
         <v>1010</v>
       </c>
       <c r="Q478" s="6">
-        <v>2928.95</v>
+        <v>1491.24</v>
       </c>
       <c r="R478" s="6" t="s">
         <v>23</v>
@@ -35216,7 +35216,7 @@
         <v>1012</v>
       </c>
       <c r="Q479" s="6">
-        <v>1752.71</v>
+        <v>1502.1</v>
       </c>
       <c r="R479" s="6" t="s">
         <v>23</v>
@@ -50792,7 +50792,7 @@
         <v>1546</v>
       </c>
       <c r="Q743" s="6">
-        <v>622.4</v>
+        <v>451.4</v>
       </c>
       <c r="R743" s="6" t="s">
         <v>23</v>
@@ -51087,7 +51087,7 @@
         <v>1563</v>
       </c>
       <c r="Q748" s="6">
-        <v>641.54</v>
+        <v>602.12</v>
       </c>
       <c r="R748" s="6" t="s">
         <v>23</v>
@@ -53388,7 +53388,7 @@
         <v>1649</v>
       </c>
       <c r="Q787" s="6">
-        <v>475.41</v>
+        <v>2117.16</v>
       </c>
       <c r="R787" s="6" t="s">
         <v>23</v>
@@ -53565,7 +53565,7 @@
         <v>1655</v>
       </c>
       <c r="Q790" s="6">
-        <v>14171.366</v>
+        <v>14801.396000000001</v>
       </c>
       <c r="R790" s="6" t="s">
         <v>23</v>
@@ -53683,7 +53683,7 @@
         <v>1659</v>
       </c>
       <c r="Q792" s="6">
-        <v>4022.95</v>
+        <v>3788.95</v>
       </c>
       <c r="R792" s="6" t="s">
         <v>23</v>
@@ -53801,7 +53801,7 @@
         <v>1663</v>
       </c>
       <c r="Q794" s="6">
-        <v>3938.47</v>
+        <v>5482.48</v>
       </c>
       <c r="R794" s="6" t="s">
         <v>23</v>
@@ -53860,7 +53860,7 @@
         <v>1665</v>
       </c>
       <c r="Q795" s="6">
-        <v>20814.189999999999</v>
+        <v>28252.49</v>
       </c>
       <c r="R795" s="6" t="s">
         <v>23</v>
@@ -54155,7 +54155,7 @@
         <v>1675</v>
       </c>
       <c r="Q800" s="6">
-        <v>9127.64</v>
+        <v>9778.93</v>
       </c>
       <c r="R800" s="6" t="s">
         <v>23</v>
@@ -54273,7 +54273,7 @@
         <v>1679</v>
       </c>
       <c r="Q802" s="6">
-        <v>1545.1</v>
+        <v>1301.29</v>
       </c>
       <c r="R802" s="6" t="s">
         <v>23</v>
@@ -54317,7 +54317,7 @@
         <v>23</v>
       </c>
       <c r="L803" s="6">
-        <v>4.4800000000000004</v>
+        <v>4.66</v>
       </c>
       <c r="M803" s="6">
         <v>0</v>
@@ -54332,7 +54332,7 @@
         <v>1681</v>
       </c>
       <c r="Q803" s="6">
-        <v>3069.1383000000001</v>
+        <v>27019.134399999999</v>
       </c>
       <c r="R803" s="6" t="s">
         <v>23</v>
@@ -54391,7 +54391,7 @@
         <v>1684</v>
       </c>
       <c r="Q804" s="6">
-        <v>10850.91</v>
+        <v>26536.57</v>
       </c>
       <c r="R804" s="6" t="s">
         <v>23</v>
@@ -54450,7 +54450,7 @@
         <v>1687</v>
       </c>
       <c r="Q805" s="6">
-        <v>64610.153899999998</v>
+        <v>67020.758300000001</v>
       </c>
       <c r="R805" s="6" t="s">
         <v>23</v>
@@ -54509,7 +54509,7 @@
         <v>1690</v>
       </c>
       <c r="Q806" s="6">
-        <v>1486.05</v>
+        <v>1971.89</v>
       </c>
       <c r="R806" s="6" t="s">
         <v>23</v>
@@ -54568,7 +54568,7 @@
         <v>1693</v>
       </c>
       <c r="Q807" s="6">
-        <v>4476.62</v>
+        <v>5598</v>
       </c>
       <c r="R807" s="6" t="s">
         <v>23</v>
@@ -55866,7 +55866,7 @@
         <v>1758</v>
       </c>
       <c r="Q829" s="6">
-        <v>10684.97</v>
+        <v>10822.53</v>
       </c>
       <c r="R829" s="6" t="s">
         <v>23</v>
@@ -55925,7 +55925,7 @@
         <v>1762</v>
       </c>
       <c r="Q830" s="6">
-        <v>2139.3000000000002</v>
+        <v>2983.86</v>
       </c>
       <c r="R830" s="6" t="s">
         <v>23</v>
@@ -56574,7 +56574,7 @@
         <v>1800</v>
       </c>
       <c r="Q841" s="6">
-        <v>441.98</v>
+        <v>423.69</v>
       </c>
       <c r="R841" s="6" t="s">
         <v>23</v>
@@ -56869,7 +56869,7 @@
         <v>1817</v>
       </c>
       <c r="Q846" s="6">
-        <v>261.14</v>
+        <v>241.96</v>
       </c>
       <c r="R846" s="6" t="s">
         <v>23</v>
@@ -56987,7 +56987,7 @@
         <v>1822</v>
       </c>
       <c r="Q848" s="6">
-        <v>1298.48</v>
+        <v>1281.71</v>
       </c>
       <c r="R848" s="6" t="s">
         <v>23</v>
@@ -57636,7 +57636,7 @@
         <v>1855</v>
       </c>
       <c r="Q859" s="6">
-        <v>18423.72</v>
+        <v>16754.75</v>
       </c>
       <c r="R859" s="6" t="s">
         <v>23</v>
@@ -57754,7 +57754,7 @@
         <v>1861</v>
       </c>
       <c r="Q861" s="6">
-        <v>1746.6</v>
+        <v>1617.93</v>
       </c>
       <c r="R861" s="6" t="s">
         <v>23</v>
@@ -57813,7 +57813,7 @@
         <v>1864</v>
       </c>
       <c r="Q862" s="6">
-        <v>1669.66</v>
+        <v>1620.78</v>
       </c>
       <c r="R862" s="6" t="s">
         <v>23</v>
@@ -57872,7 +57872,7 @@
         <v>1868</v>
       </c>
       <c r="Q863" s="6">
-        <v>686.82</v>
+        <v>903.96</v>
       </c>
       <c r="R863" s="6" t="s">
         <v>23</v>
@@ -57931,7 +57931,7 @@
         <v>1871</v>
       </c>
       <c r="Q864" s="6">
-        <v>1617.36</v>
+        <v>1281.3499999999999</v>
       </c>
       <c r="R864" s="6" t="s">
         <v>23</v>
@@ -57990,7 +57990,7 @@
         <v>1874</v>
       </c>
       <c r="Q865" s="6">
-        <v>50374.98</v>
+        <v>50256.38</v>
       </c>
       <c r="R865" s="6" t="s">
         <v>23</v>
@@ -58521,7 +58521,7 @@
         <v>1901</v>
       </c>
       <c r="Q874" s="6">
-        <v>70</v>
+        <v>186</v>
       </c>
       <c r="R874" s="6" t="s">
         <v>23</v>
@@ -58580,7 +58580,7 @@
         <v>1904</v>
       </c>
       <c r="Q875" s="6">
-        <v>208.8</v>
+        <v>426.7</v>
       </c>
       <c r="R875" s="6" t="s">
         <v>23</v>
@@ -58639,7 +58639,7 @@
         <v>1907</v>
       </c>
       <c r="Q876" s="6">
-        <v>60</v>
+        <v>152.80000000000001</v>
       </c>
       <c r="R876" s="6" t="s">
         <v>23</v>
@@ -58698,7 +58698,7 @@
         <v>1910</v>
       </c>
       <c r="Q877" s="6">
-        <v>109.6</v>
+        <v>208.9</v>
       </c>
       <c r="R877" s="6" t="s">
         <v>23</v>
@@ -58993,7 +58993,7 @@
         <v>1925</v>
       </c>
       <c r="Q882" s="6">
-        <v>15207.5</v>
+        <v>12302.9</v>
       </c>
       <c r="R882" s="6" t="s">
         <v>23</v>
@@ -59111,7 +59111,7 @@
         <v>1932</v>
       </c>
       <c r="Q884" s="6">
-        <v>85.8</v>
+        <v>0</v>
       </c>
       <c r="R884" s="6" t="s">
         <v>23</v>
@@ -59347,7 +59347,7 @@
         <v>1944</v>
       </c>
       <c r="Q888" s="6">
-        <v>170.06</v>
+        <v>346.28</v>
       </c>
       <c r="R888" s="6" t="s">
         <v>23</v>
@@ -60568,7 +60568,7 @@
         <v>21</v>
       </c>
       <c r="K909" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L909" s="6">
         <v>0</v>
@@ -61176,7 +61176,7 @@
         <v>2038</v>
       </c>
       <c r="Q919" s="6">
-        <v>89.2</v>
+        <v>815.8</v>
       </c>
       <c r="R919" s="6" t="s">
         <v>23</v>
@@ -61235,7 +61235,7 @@
         <v>2041</v>
       </c>
       <c r="Q920" s="6">
-        <v>20205.490000000002</v>
+        <v>18195.97</v>
       </c>
       <c r="R920" s="6" t="s">
         <v>23</v>
@@ -61353,7 +61353,7 @@
         <v>2047</v>
       </c>
       <c r="Q922" s="6">
-        <v>40014.955000000002</v>
+        <v>36911.995000000003</v>
       </c>
       <c r="R922" s="6" t="s">
         <v>23</v>
@@ -61471,7 +61471,7 @@
         <v>2053</v>
       </c>
       <c r="Q924" s="6">
-        <v>2371</v>
+        <v>2147</v>
       </c>
       <c r="R924" s="6" t="s">
         <v>23</v>
@@ -61648,7 +61648,7 @@
         <v>2062</v>
       </c>
       <c r="Q927" s="6">
-        <v>614.35</v>
+        <v>392.6</v>
       </c>
       <c r="R927" s="6" t="s">
         <v>23</v>
@@ -62061,7 +62061,7 @@
         <v>2083</v>
       </c>
       <c r="Q934" s="6">
-        <v>3662.4</v>
+        <v>4298.12</v>
       </c>
       <c r="R934" s="6" t="s">
         <v>23</v>
@@ -62238,7 +62238,7 @@
         <v>2092</v>
       </c>
       <c r="Q937" s="6">
-        <v>1093.3</v>
+        <v>5437.66</v>
       </c>
       <c r="R937" s="6" t="s">
         <v>23</v>
@@ -62415,7 +62415,7 @@
         <v>2101</v>
       </c>
       <c r="Q940" s="6">
-        <v>362.4</v>
+        <v>156.44</v>
       </c>
       <c r="R940" s="6" t="s">
         <v>23</v>
@@ -62474,7 +62474,7 @@
         <v>2104</v>
       </c>
       <c r="Q941" s="6">
-        <v>1422.77</v>
+        <v>2331.94</v>
       </c>
       <c r="R941" s="6" t="s">
         <v>23</v>
@@ -62533,7 +62533,7 @@
         <v>2107</v>
       </c>
       <c r="Q942" s="6">
-        <v>3000</v>
+        <v>2855.1</v>
       </c>
       <c r="R942" s="6" t="s">
         <v>23</v>
@@ -62592,7 +62592,7 @@
         <v>2110</v>
       </c>
       <c r="Q943" s="6">
-        <v>1000</v>
+        <v>1962.74</v>
       </c>
       <c r="R943" s="6" t="s">
         <v>23</v>
@@ -63282,7 +63282,7 @@
         <v>21</v>
       </c>
       <c r="K955" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L955" s="6">
         <v>0</v>
@@ -63359,7 +63359,7 @@
         <v>2149</v>
       </c>
       <c r="Q956" s="6">
-        <v>1291.3</v>
+        <v>418.9</v>
       </c>
       <c r="R956" s="6" t="s">
         <v>23</v>
@@ -63400,10 +63400,10 @@
         <v>21</v>
       </c>
       <c r="K957" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L957" s="6">
-        <v>0</v>
+        <v>3.29</v>
       </c>
       <c r="M957" s="6">
         <v>0</v>
@@ -63418,7 +63418,7 @@
         <v>2152</v>
       </c>
       <c r="Q957" s="6">
-        <v>0</v>
+        <v>1473.2</v>
       </c>
       <c r="R957" s="6" t="s">
         <v>23</v>
@@ -63518,10 +63518,10 @@
         <v>21</v>
       </c>
       <c r="K959" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L959" s="6">
-        <v>0</v>
+        <v>3.29</v>
       </c>
       <c r="M959" s="6">
         <v>0</v>
@@ -63536,7 +63536,7 @@
         <v>2158</v>
       </c>
       <c r="Q959" s="6">
-        <v>0</v>
+        <v>1171.4000000000001</v>
       </c>
       <c r="R959" s="6" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
act data base 05022020
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/TC_02.xlsx
+++ b/EXCEL LIBS/TC_02.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14706" uniqueCount="2230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14886" uniqueCount="2266">
   <si>
     <t>sqlnav01.aquinos.org : Aquinos, S.A.</t>
   </si>
@@ -6613,18 +6613,12 @@
     <t>QUARTZ - 603 (AZUL MARINHO)</t>
   </si>
   <si>
-    <t>Lista Produto : 14-01-2020 11:13:33</t>
-  </si>
-  <si>
     <t>TC15147</t>
   </si>
   <si>
     <t>G3160</t>
   </si>
   <si>
-    <t>MACAU - CUOIO (AMARELO)</t>
-  </si>
-  <si>
     <t>TC15148</t>
   </si>
   <si>
@@ -6713,6 +6707,120 @@
   </si>
   <si>
     <t>BOLSHOI 01 | YANODA 22 (BRANCO)</t>
+  </si>
+  <si>
+    <t>Lista Produto : 04-02-2020 15:43:21</t>
+  </si>
+  <si>
+    <t>MACAU - CUOIO (AMARELO TORRADO)</t>
+  </si>
+  <si>
+    <t>TC15158</t>
+  </si>
+  <si>
+    <t>G2842</t>
+  </si>
+  <si>
+    <t>TEXAS 480 C.95 (TAUPE)</t>
+  </si>
+  <si>
+    <t>TC15159</t>
+  </si>
+  <si>
+    <t>G2112</t>
+  </si>
+  <si>
+    <t>SAWANA 21 LIGHT GREY</t>
+  </si>
+  <si>
+    <t>TC15160</t>
+  </si>
+  <si>
+    <t>G3510</t>
+  </si>
+  <si>
+    <t>PEGASUS STAR - LIGHT GREY</t>
+  </si>
+  <si>
+    <t>TC15161</t>
+  </si>
+  <si>
+    <t>G3511</t>
+  </si>
+  <si>
+    <t>PEGASUS STAR - MEDIUM GREY</t>
+  </si>
+  <si>
+    <t>TC15162</t>
+  </si>
+  <si>
+    <t>G3550</t>
+  </si>
+  <si>
+    <t>PEGASUS STAR - VERMELHO</t>
+  </si>
+  <si>
+    <t>TC15163</t>
+  </si>
+  <si>
+    <t>G3540</t>
+  </si>
+  <si>
+    <t>PEGASUS STAR - EXPRESS (CHOCOLATE)</t>
+  </si>
+  <si>
+    <t>TC15164</t>
+  </si>
+  <si>
+    <t>G3130</t>
+  </si>
+  <si>
+    <t>MACAU - MOSS 10 (VERDE)</t>
+  </si>
+  <si>
+    <t>TC15165</t>
+  </si>
+  <si>
+    <t>G3120</t>
+  </si>
+  <si>
+    <t>MACAU - PETROL 15 (AZUL)</t>
+  </si>
+  <si>
+    <t>TC15166</t>
+  </si>
+  <si>
+    <t>G3110</t>
+  </si>
+  <si>
+    <t>MACAU - CEMENT 09 (CINZENTO)</t>
+  </si>
+  <si>
+    <t>TC15167</t>
+  </si>
+  <si>
+    <t>G2212</t>
+  </si>
+  <si>
+    <t>QUEENS DARK GREY</t>
+  </si>
+  <si>
+    <t>TC15168</t>
+  </si>
+  <si>
+    <t>G3610</t>
+  </si>
+  <si>
+    <t>VISSLE DARK GREY</t>
+  </si>
+  <si>
+    <t>TC15169</t>
+  </si>
+  <si>
+    <t>G3710</t>
+  </si>
+  <si>
+    <t>PERSA ASH 12</t>
   </si>
 </sst>
 </file>
@@ -6879,8 +6987,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NavDataRegion" displayName="NavDataRegion" ref="A3:S982" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A3:S982"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NavDataRegion" displayName="NavDataRegion" ref="A3:S994" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A3:S994"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Nº" dataDxfId="16"/>
     <tableColumn id="2" name="Cód. Barras Efacec" dataDxfId="15"/>
@@ -7169,7 +7277,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S982"/>
+  <dimension ref="A1:S994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F977" sqref="F977"/>
@@ -7180,7 +7288,7 @@
     <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
@@ -7223,7 +7331,7 @@
     </row>
     <row r="2" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2196</v>
+        <v>2228</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -17383,7 +17491,7 @@
         <v>368</v>
       </c>
       <c r="Q174" s="6">
-        <v>3210.95</v>
+        <v>3173.8</v>
       </c>
       <c r="R174" s="6" t="s">
         <v>23</v>
@@ -17619,7 +17727,7 @@
         <v>376</v>
       </c>
       <c r="Q178" s="6">
-        <v>452.73860000000002</v>
+        <v>339.65359999999998</v>
       </c>
       <c r="R178" s="6" t="s">
         <v>23</v>
@@ -17678,7 +17786,7 @@
         <v>378</v>
       </c>
       <c r="Q179" s="6">
-        <v>377.4</v>
+        <v>279.19</v>
       </c>
       <c r="R179" s="6" t="s">
         <v>23</v>
@@ -18150,7 +18258,7 @@
         <v>394</v>
       </c>
       <c r="Q187" s="6">
-        <v>8026.58</v>
+        <v>6058.41</v>
       </c>
       <c r="R187" s="6" t="s">
         <v>23</v>
@@ -18504,7 +18612,7 @@
         <v>406</v>
       </c>
       <c r="Q193" s="6">
-        <v>1934</v>
+        <v>1849.7</v>
       </c>
       <c r="R193" s="6" t="s">
         <v>23</v>
@@ -18799,7 +18907,7 @@
         <v>416</v>
       </c>
       <c r="Q198" s="6">
-        <v>1633.1</v>
+        <v>1327.2</v>
       </c>
       <c r="R198" s="6" t="s">
         <v>23</v>
@@ -19212,7 +19320,7 @@
         <v>430</v>
       </c>
       <c r="Q205" s="6">
-        <v>77.44</v>
+        <v>91.66</v>
       </c>
       <c r="R205" s="6" t="s">
         <v>23</v>
@@ -19271,7 +19379,7 @@
         <v>432</v>
       </c>
       <c r="Q206" s="6">
-        <v>3023.45</v>
+        <v>2646.35</v>
       </c>
       <c r="R206" s="6" t="s">
         <v>23</v>
@@ -19448,7 +19556,7 @@
         <v>438</v>
       </c>
       <c r="Q209" s="6">
-        <v>3525.42</v>
+        <v>3516.86</v>
       </c>
       <c r="R209" s="6" t="s">
         <v>23</v>
@@ -20156,7 +20264,7 @@
         <v>462</v>
       </c>
       <c r="Q221" s="6">
-        <v>0</v>
+        <v>-0.59</v>
       </c>
       <c r="R221" s="6" t="s">
         <v>23</v>
@@ -20215,7 +20323,7 @@
         <v>464</v>
       </c>
       <c r="Q222" s="6">
-        <v>3911.0472</v>
+        <v>4153.2572</v>
       </c>
       <c r="R222" s="6" t="s">
         <v>23</v>
@@ -20274,7 +20382,7 @@
         <v>466</v>
       </c>
       <c r="Q223" s="6">
-        <v>1962.65</v>
+        <v>1963.01</v>
       </c>
       <c r="R223" s="6" t="s">
         <v>23</v>
@@ -20510,7 +20618,7 @@
         <v>474</v>
       </c>
       <c r="Q227" s="6">
-        <v>7940.38</v>
+        <v>9288.5300000000007</v>
       </c>
       <c r="R227" s="6" t="s">
         <v>23</v>
@@ -20569,7 +20677,7 @@
         <v>476</v>
       </c>
       <c r="Q228" s="6">
-        <v>5796.52</v>
+        <v>7317.78</v>
       </c>
       <c r="R228" s="6" t="s">
         <v>23</v>
@@ -21277,7 +21385,7 @@
         <v>500</v>
       </c>
       <c r="Q240" s="6">
-        <v>6359.2</v>
+        <v>4772.0690000000004</v>
       </c>
       <c r="R240" s="6" t="s">
         <v>23</v>
@@ -21572,7 +21680,7 @@
         <v>510</v>
       </c>
       <c r="Q245" s="6">
-        <v>696.1</v>
+        <v>784</v>
       </c>
       <c r="R245" s="6" t="s">
         <v>23</v>
@@ -21631,7 +21739,7 @@
         <v>512</v>
       </c>
       <c r="Q246" s="6">
-        <v>1366.5</v>
+        <v>1276</v>
       </c>
       <c r="R246" s="6" t="s">
         <v>23</v>
@@ -21690,7 +21798,7 @@
         <v>514</v>
       </c>
       <c r="Q247" s="6">
-        <v>449.01</v>
+        <v>64</v>
       </c>
       <c r="R247" s="6" t="s">
         <v>23</v>
@@ -21749,7 +21857,7 @@
         <v>516</v>
       </c>
       <c r="Q248" s="6">
-        <v>1223.72</v>
+        <v>3069.59</v>
       </c>
       <c r="R248" s="6" t="s">
         <v>23</v>
@@ -21867,7 +21975,7 @@
         <v>520</v>
       </c>
       <c r="Q250" s="6">
-        <v>1045.8800000000001</v>
+        <v>333.04</v>
       </c>
       <c r="R250" s="6" t="s">
         <v>23</v>
@@ -21926,7 +22034,7 @@
         <v>522</v>
       </c>
       <c r="Q251" s="6">
-        <v>787.59</v>
+        <v>1293.48</v>
       </c>
       <c r="R251" s="6" t="s">
         <v>23</v>
@@ -21985,7 +22093,7 @@
         <v>524</v>
       </c>
       <c r="Q252" s="6">
-        <v>3352.5</v>
+        <v>3182.7</v>
       </c>
       <c r="R252" s="6" t="s">
         <v>23</v>
@@ -22752,7 +22860,7 @@
         <v>550</v>
       </c>
       <c r="Q265" s="6">
-        <v>2431.1999999999998</v>
+        <v>1890.9</v>
       </c>
       <c r="R265" s="6" t="s">
         <v>23</v>
@@ -22811,7 +22919,7 @@
         <v>552</v>
       </c>
       <c r="Q266" s="6">
-        <v>5339.63</v>
+        <v>4161.79</v>
       </c>
       <c r="R266" s="6" t="s">
         <v>23</v>
@@ -22929,7 +23037,7 @@
         <v>556</v>
       </c>
       <c r="Q268" s="6">
-        <v>86.93</v>
+        <v>931.76</v>
       </c>
       <c r="R268" s="6" t="s">
         <v>23</v>
@@ -23165,7 +23273,7 @@
         <v>565</v>
       </c>
       <c r="Q272" s="6">
-        <v>2315.4</v>
+        <v>2207.4</v>
       </c>
       <c r="R272" s="6" t="s">
         <v>23</v>
@@ -23991,7 +24099,7 @@
         <v>593</v>
       </c>
       <c r="Q286" s="6">
-        <v>1154.6199999999999</v>
+        <v>1122.78</v>
       </c>
       <c r="R286" s="6" t="s">
         <v>23</v>
@@ -24050,7 +24158,7 @@
         <v>595</v>
       </c>
       <c r="Q287" s="6">
-        <v>2823.3150000000001</v>
+        <v>2365.7150000000001</v>
       </c>
       <c r="R287" s="6" t="s">
         <v>23</v>
@@ -24109,7 +24217,7 @@
         <v>597</v>
       </c>
       <c r="Q288" s="6">
-        <v>3368.1</v>
+        <v>2699.67</v>
       </c>
       <c r="R288" s="6" t="s">
         <v>23</v>
@@ -24168,7 +24276,7 @@
         <v>599</v>
       </c>
       <c r="Q289" s="6">
-        <v>1283.6199999999999</v>
+        <v>1252.1400000000001</v>
       </c>
       <c r="R289" s="6" t="s">
         <v>23</v>
@@ -24227,7 +24335,7 @@
         <v>601</v>
       </c>
       <c r="Q290" s="6">
-        <v>3929.9450000000002</v>
+        <v>3743.3249999999998</v>
       </c>
       <c r="R290" s="6" t="s">
         <v>23</v>
@@ -24286,7 +24394,7 @@
         <v>603</v>
       </c>
       <c r="Q291" s="6">
-        <v>4981.7240000000002</v>
+        <v>4768.4189999999999</v>
       </c>
       <c r="R291" s="6" t="s">
         <v>23</v>
@@ -24345,7 +24453,7 @@
         <v>605</v>
       </c>
       <c r="Q292" s="6">
-        <v>1365.33</v>
+        <v>1271.73</v>
       </c>
       <c r="R292" s="6" t="s">
         <v>23</v>
@@ -24640,7 +24748,7 @@
         <v>615</v>
       </c>
       <c r="Q297" s="6">
-        <v>3604.41</v>
+        <v>3591.31</v>
       </c>
       <c r="R297" s="6" t="s">
         <v>23</v>
@@ -24758,7 +24866,7 @@
         <v>619</v>
       </c>
       <c r="Q299" s="6">
-        <v>1185.23</v>
+        <v>1127.95</v>
       </c>
       <c r="R299" s="6" t="s">
         <v>23</v>
@@ -24817,7 +24925,7 @@
         <v>621</v>
       </c>
       <c r="Q300" s="6">
-        <v>3822.94</v>
+        <v>2887.72</v>
       </c>
       <c r="R300" s="6" t="s">
         <v>23</v>
@@ -24876,7 +24984,7 @@
         <v>623</v>
       </c>
       <c r="Q301" s="6">
-        <v>956.14</v>
+        <v>1483.26</v>
       </c>
       <c r="R301" s="6" t="s">
         <v>23</v>
@@ -24935,7 +25043,7 @@
         <v>625</v>
       </c>
       <c r="Q302" s="6">
-        <v>4335.59</v>
+        <v>3926.13</v>
       </c>
       <c r="R302" s="6" t="s">
         <v>23</v>
@@ -24994,7 +25102,7 @@
         <v>627</v>
       </c>
       <c r="Q303" s="6">
-        <v>6846.77</v>
+        <v>46778.952400000002</v>
       </c>
       <c r="R303" s="6" t="s">
         <v>23</v>
@@ -25053,7 +25161,7 @@
         <v>629</v>
       </c>
       <c r="Q304" s="6">
-        <v>73445.891000000003</v>
+        <v>76105.731</v>
       </c>
       <c r="R304" s="6" t="s">
         <v>23</v>
@@ -25112,7 +25220,7 @@
         <v>631</v>
       </c>
       <c r="Q305" s="6">
-        <v>3136.51</v>
+        <v>2796.04</v>
       </c>
       <c r="R305" s="6" t="s">
         <v>23</v>
@@ -25171,7 +25279,7 @@
         <v>633</v>
       </c>
       <c r="Q306" s="6">
-        <v>3855.395</v>
+        <v>3474.1950000000002</v>
       </c>
       <c r="R306" s="6" t="s">
         <v>23</v>
@@ -25230,7 +25338,7 @@
         <v>635</v>
       </c>
       <c r="Q307" s="6">
-        <v>935.2</v>
+        <v>971.2</v>
       </c>
       <c r="R307" s="6" t="s">
         <v>23</v>
@@ -25407,7 +25515,7 @@
         <v>641</v>
       </c>
       <c r="Q310" s="6">
-        <v>3871.22</v>
+        <v>3685.07</v>
       </c>
       <c r="R310" s="6" t="s">
         <v>23</v>
@@ -25510,7 +25618,7 @@
         <v>23</v>
       </c>
       <c r="L312" s="6">
-        <v>3.75</v>
+        <v>3.02</v>
       </c>
       <c r="M312" s="6">
         <v>0</v>
@@ -25525,7 +25633,7 @@
         <v>646</v>
       </c>
       <c r="Q312" s="6">
-        <v>2667.31</v>
+        <v>1396.76</v>
       </c>
       <c r="R312" s="6" t="s">
         <v>23</v>
@@ -25584,7 +25692,7 @@
         <v>649</v>
       </c>
       <c r="Q313" s="6">
-        <v>414.44</v>
+        <v>283.95999999999998</v>
       </c>
       <c r="R313" s="6" t="s">
         <v>23</v>
@@ -25643,7 +25751,7 @@
         <v>652</v>
       </c>
       <c r="Q314" s="6">
-        <v>2371.58</v>
+        <v>2321</v>
       </c>
       <c r="R314" s="6" t="s">
         <v>23</v>
@@ -25761,7 +25869,7 @@
         <v>658</v>
       </c>
       <c r="Q316" s="6">
-        <v>344.24</v>
+        <v>305.83999999999997</v>
       </c>
       <c r="R316" s="6" t="s">
         <v>23</v>
@@ -25820,7 +25928,7 @@
         <v>660</v>
       </c>
       <c r="Q317" s="6">
-        <v>8733.14</v>
+        <v>8751.7000000000007</v>
       </c>
       <c r="R317" s="6" t="s">
         <v>23</v>
@@ -25879,7 +25987,7 @@
         <v>662</v>
       </c>
       <c r="Q318" s="6">
-        <v>3976.81</v>
+        <v>3795.2</v>
       </c>
       <c r="R318" s="6" t="s">
         <v>23</v>
@@ -25938,7 +26046,7 @@
         <v>664</v>
       </c>
       <c r="Q319" s="6">
-        <v>9277.42</v>
+        <v>8771.09</v>
       </c>
       <c r="R319" s="6" t="s">
         <v>23</v>
@@ -25997,7 +26105,7 @@
         <v>666</v>
       </c>
       <c r="Q320" s="6">
-        <v>3288.83</v>
+        <v>3007.34</v>
       </c>
       <c r="R320" s="6" t="s">
         <v>23</v>
@@ -26056,7 +26164,7 @@
         <v>668</v>
       </c>
       <c r="Q321" s="6">
-        <v>9199.9</v>
+        <v>6248.95</v>
       </c>
       <c r="R321" s="6" t="s">
         <v>23</v>
@@ -26115,7 +26223,7 @@
         <v>670</v>
       </c>
       <c r="Q322" s="6">
-        <v>3685.83</v>
+        <v>3356.5704000000001</v>
       </c>
       <c r="R322" s="6" t="s">
         <v>23</v>
@@ -26174,7 +26282,7 @@
         <v>672</v>
       </c>
       <c r="Q323" s="6">
-        <v>1704.29</v>
+        <v>1639.43</v>
       </c>
       <c r="R323" s="6" t="s">
         <v>23</v>
@@ -26233,7 +26341,7 @@
         <v>674</v>
       </c>
       <c r="Q324" s="6">
-        <v>2989.5</v>
+        <v>2991.1</v>
       </c>
       <c r="R324" s="6" t="s">
         <v>23</v>
@@ -26292,7 +26400,7 @@
         <v>676</v>
       </c>
       <c r="Q325" s="6">
-        <v>4251.2996999999996</v>
+        <v>4146.0697</v>
       </c>
       <c r="R325" s="6" t="s">
         <v>23</v>
@@ -26351,7 +26459,7 @@
         <v>678</v>
       </c>
       <c r="Q326" s="6">
-        <v>925.16</v>
+        <v>794.18</v>
       </c>
       <c r="R326" s="6" t="s">
         <v>23</v>
@@ -26410,7 +26518,7 @@
         <v>680</v>
       </c>
       <c r="Q327" s="6">
-        <v>20.55</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="R327" s="6" t="s">
         <v>23</v>
@@ -26469,7 +26577,7 @@
         <v>683</v>
       </c>
       <c r="Q328" s="6">
-        <v>3794.12</v>
+        <v>3423.5909999999999</v>
       </c>
       <c r="R328" s="6" t="s">
         <v>23</v>
@@ -26528,7 +26636,7 @@
         <v>686</v>
       </c>
       <c r="Q329" s="6">
-        <v>2092.6999999999998</v>
+        <v>2073.1999999999998</v>
       </c>
       <c r="R329" s="6" t="s">
         <v>23</v>
@@ -26587,7 +26695,7 @@
         <v>689</v>
       </c>
       <c r="Q330" s="6">
-        <v>431.7</v>
+        <v>606.12</v>
       </c>
       <c r="R330" s="6" t="s">
         <v>23</v>
@@ -26646,7 +26754,7 @@
         <v>692</v>
       </c>
       <c r="Q331" s="6">
-        <v>1953.32</v>
+        <v>1333.65</v>
       </c>
       <c r="R331" s="6" t="s">
         <v>23</v>
@@ -26705,7 +26813,7 @@
         <v>694</v>
       </c>
       <c r="Q332" s="6">
-        <v>2385.4</v>
+        <v>2716.39</v>
       </c>
       <c r="R332" s="6" t="s">
         <v>23</v>
@@ -26764,7 +26872,7 @@
         <v>697</v>
       </c>
       <c r="Q333" s="6">
-        <v>2107.77</v>
+        <v>2038.32</v>
       </c>
       <c r="R333" s="6" t="s">
         <v>23</v>
@@ -26823,7 +26931,7 @@
         <v>700</v>
       </c>
       <c r="Q334" s="6">
-        <v>179.5</v>
+        <v>141.1</v>
       </c>
       <c r="R334" s="6" t="s">
         <v>23</v>
@@ -26882,7 +26990,7 @@
         <v>703</v>
       </c>
       <c r="Q335" s="6">
-        <v>1430.845</v>
+        <v>1412.825</v>
       </c>
       <c r="R335" s="6" t="s">
         <v>23</v>
@@ -26941,7 +27049,7 @@
         <v>706</v>
       </c>
       <c r="Q336" s="6">
-        <v>2630.1</v>
+        <v>2375.34</v>
       </c>
       <c r="R336" s="6" t="s">
         <v>23</v>
@@ -27177,7 +27285,7 @@
         <v>714</v>
       </c>
       <c r="Q340" s="6">
-        <v>252.215</v>
+        <v>164.20500000000001</v>
       </c>
       <c r="R340" s="6" t="s">
         <v>23</v>
@@ -27472,7 +27580,7 @@
         <v>724</v>
       </c>
       <c r="Q345" s="6">
-        <v>7767.56</v>
+        <v>5801.68</v>
       </c>
       <c r="R345" s="6" t="s">
         <v>23</v>
@@ -27531,7 +27639,7 @@
         <v>726</v>
       </c>
       <c r="Q346" s="6">
-        <v>1219.19</v>
+        <v>915.69</v>
       </c>
       <c r="R346" s="6" t="s">
         <v>23</v>
@@ -27590,7 +27698,7 @@
         <v>728</v>
       </c>
       <c r="Q347" s="6">
-        <v>226.48</v>
+        <v>207.98</v>
       </c>
       <c r="R347" s="6" t="s">
         <v>23</v>
@@ -27649,7 +27757,7 @@
         <v>731</v>
       </c>
       <c r="Q348" s="6">
-        <v>447</v>
+        <v>412.14</v>
       </c>
       <c r="R348" s="6" t="s">
         <v>23</v>
@@ -27708,7 +27816,7 @@
         <v>734</v>
       </c>
       <c r="Q349" s="6">
-        <v>1469.88</v>
+        <v>830.23</v>
       </c>
       <c r="R349" s="6" t="s">
         <v>23</v>
@@ -27767,7 +27875,7 @@
         <v>736</v>
       </c>
       <c r="Q350" s="6">
-        <v>5285.3950000000004</v>
+        <v>5063.4449999999997</v>
       </c>
       <c r="R350" s="6" t="s">
         <v>23</v>
@@ -27826,7 +27934,7 @@
         <v>738</v>
       </c>
       <c r="Q351" s="6">
-        <v>29854.52</v>
+        <v>29433.56</v>
       </c>
       <c r="R351" s="6" t="s">
         <v>23</v>
@@ -27885,7 +27993,7 @@
         <v>741</v>
       </c>
       <c r="Q352" s="6">
-        <v>3533.8</v>
+        <v>3553.8</v>
       </c>
       <c r="R352" s="6" t="s">
         <v>23</v>
@@ -28003,7 +28111,7 @@
         <v>747</v>
       </c>
       <c r="Q354" s="6">
-        <v>286</v>
+        <v>258.7</v>
       </c>
       <c r="R354" s="6" t="s">
         <v>23</v>
@@ -28062,7 +28170,7 @@
         <v>749</v>
       </c>
       <c r="Q355" s="6">
-        <v>1625.83</v>
+        <v>1533.11</v>
       </c>
       <c r="R355" s="6" t="s">
         <v>23</v>
@@ -28298,7 +28406,7 @@
         <v>757</v>
       </c>
       <c r="Q359" s="6">
-        <v>1059.0999999999999</v>
+        <v>988</v>
       </c>
       <c r="R359" s="6" t="s">
         <v>23</v>
@@ -28357,7 +28465,7 @@
         <v>759</v>
       </c>
       <c r="Q360" s="6">
-        <v>1616.2</v>
+        <v>1579.3</v>
       </c>
       <c r="R360" s="6" t="s">
         <v>23</v>
@@ -28888,7 +28996,7 @@
         <v>787</v>
       </c>
       <c r="Q369" s="6">
-        <v>68.400000000000006</v>
+        <v>60.9</v>
       </c>
       <c r="R369" s="6" t="s">
         <v>23</v>
@@ -28947,7 +29055,7 @@
         <v>791</v>
       </c>
       <c r="Q370" s="6">
-        <v>160.4</v>
+        <v>156.65</v>
       </c>
       <c r="R370" s="6" t="s">
         <v>23</v>
@@ -29006,7 +29114,7 @@
         <v>794</v>
       </c>
       <c r="Q371" s="6">
-        <v>3806.4</v>
+        <v>3506.83</v>
       </c>
       <c r="R371" s="6" t="s">
         <v>23</v>
@@ -29124,7 +29232,7 @@
         <v>800</v>
       </c>
       <c r="Q373" s="6">
-        <v>568.28</v>
+        <v>566.76</v>
       </c>
       <c r="R373" s="6" t="s">
         <v>23</v>
@@ -35142,7 +35250,7 @@
         <v>1004</v>
       </c>
       <c r="Q475" s="6">
-        <v>895.25</v>
+        <v>1141.47</v>
       </c>
       <c r="R475" s="6" t="s">
         <v>23</v>
@@ -35186,7 +35294,7 @@
         <v>23</v>
       </c>
       <c r="L476" s="6">
-        <v>3.25</v>
+        <v>3.99</v>
       </c>
       <c r="M476" s="6">
         <v>0</v>
@@ -35201,7 +35309,7 @@
         <v>1006</v>
       </c>
       <c r="Q476" s="6">
-        <v>345.02</v>
+        <v>460.22</v>
       </c>
       <c r="R476" s="6" t="s">
         <v>23</v>
@@ -35245,7 +35353,7 @@
         <v>23</v>
       </c>
       <c r="L477" s="6">
-        <v>3.42</v>
+        <v>3.99</v>
       </c>
       <c r="M477" s="6">
         <v>0</v>
@@ -35260,7 +35368,7 @@
         <v>1008</v>
       </c>
       <c r="Q477" s="6">
-        <v>194.13</v>
+        <v>329.85</v>
       </c>
       <c r="R477" s="6" t="s">
         <v>23</v>
@@ -35319,7 +35427,7 @@
         <v>1010</v>
       </c>
       <c r="Q478" s="6">
-        <v>1438.48</v>
+        <v>1196.3</v>
       </c>
       <c r="R478" s="6" t="s">
         <v>23</v>
@@ -35378,7 +35486,7 @@
         <v>1012</v>
       </c>
       <c r="Q479" s="6">
-        <v>1106.4000000000001</v>
+        <v>412.94</v>
       </c>
       <c r="R479" s="6" t="s">
         <v>23</v>
@@ -51249,7 +51357,7 @@
         <v>1563</v>
       </c>
       <c r="Q748" s="6">
-        <v>602.12</v>
+        <v>501.64</v>
       </c>
       <c r="R748" s="6" t="s">
         <v>23</v>
@@ -53550,7 +53658,7 @@
         <v>1649</v>
       </c>
       <c r="Q787" s="6">
-        <v>2117.16</v>
+        <v>3440.86</v>
       </c>
       <c r="R787" s="6" t="s">
         <v>23</v>
@@ -53727,7 +53835,7 @@
         <v>1655</v>
       </c>
       <c r="Q790" s="6">
-        <v>13100.130999999999</v>
+        <v>10188.260679999999</v>
       </c>
       <c r="R790" s="6" t="s">
         <v>23</v>
@@ -53845,7 +53953,7 @@
         <v>1659</v>
       </c>
       <c r="Q792" s="6">
-        <v>3788.95</v>
+        <v>2525.35</v>
       </c>
       <c r="R792" s="6" t="s">
         <v>23</v>
@@ -53963,7 +54071,7 @@
         <v>1663</v>
       </c>
       <c r="Q794" s="6">
-        <v>5479.85</v>
+        <v>3746.9549999999999</v>
       </c>
       <c r="R794" s="6" t="s">
         <v>23</v>
@@ -54022,7 +54130,7 @@
         <v>1665</v>
       </c>
       <c r="Q795" s="6">
-        <v>26480</v>
+        <v>21211.67</v>
       </c>
       <c r="R795" s="6" t="s">
         <v>23</v>
@@ -54317,7 +54425,7 @@
         <v>1675</v>
       </c>
       <c r="Q800" s="6">
-        <v>8624.9240000000009</v>
+        <v>7942.9</v>
       </c>
       <c r="R800" s="6" t="s">
         <v>23</v>
@@ -54435,7 +54543,7 @@
         <v>1679</v>
       </c>
       <c r="Q802" s="6">
-        <v>1297.6679999999999</v>
+        <v>1062.6400000000001</v>
       </c>
       <c r="R802" s="6" t="s">
         <v>23</v>
@@ -54494,7 +54602,7 @@
         <v>1681</v>
       </c>
       <c r="Q803" s="6">
-        <v>23151.234400000001</v>
+        <v>22169.932000000001</v>
       </c>
       <c r="R803" s="6" t="s">
         <v>23</v>
@@ -54553,7 +54661,7 @@
         <v>1684</v>
       </c>
       <c r="Q804" s="6">
-        <v>24734.240000000002</v>
+        <v>23273.98</v>
       </c>
       <c r="R804" s="6" t="s">
         <v>23</v>
@@ -54612,7 +54720,7 @@
         <v>1687</v>
       </c>
       <c r="Q805" s="6">
-        <v>62476.988299999997</v>
+        <v>48419.4683</v>
       </c>
       <c r="R805" s="6" t="s">
         <v>23</v>
@@ -54671,7 +54779,7 @@
         <v>1690</v>
       </c>
       <c r="Q806" s="6">
-        <v>2792.39</v>
+        <v>2247.4899999999998</v>
       </c>
       <c r="R806" s="6" t="s">
         <v>23</v>
@@ -54730,7 +54838,7 @@
         <v>1693</v>
       </c>
       <c r="Q807" s="6">
-        <v>5188.3100000000004</v>
+        <v>5187.8100000000004</v>
       </c>
       <c r="R807" s="6" t="s">
         <v>23</v>
@@ -55674,7 +55782,7 @@
         <v>1735</v>
       </c>
       <c r="Q823" s="6">
-        <v>3212.8</v>
+        <v>3081.14</v>
       </c>
       <c r="R823" s="6" t="s">
         <v>23</v>
@@ -56146,7 +56254,7 @@
         <v>1758</v>
       </c>
       <c r="Q831" s="6">
-        <v>20921.96</v>
+        <v>14308.84</v>
       </c>
       <c r="R831" s="6" t="s">
         <v>23</v>
@@ -56205,7 +56313,7 @@
         <v>1762</v>
       </c>
       <c r="Q832" s="6">
-        <v>12375.45</v>
+        <v>10123.129999999999</v>
       </c>
       <c r="R832" s="6" t="s">
         <v>23</v>
@@ -56382,7 +56490,7 @@
         <v>1771</v>
       </c>
       <c r="Q835" s="6">
-        <v>2987.5</v>
+        <v>1184.58</v>
       </c>
       <c r="R835" s="6" t="s">
         <v>23</v>
@@ -56500,7 +56608,7 @@
         <v>1777</v>
       </c>
       <c r="Q837" s="6">
-        <v>542.84</v>
+        <v>562.20000000000005</v>
       </c>
       <c r="R837" s="6" t="s">
         <v>23</v>
@@ -56559,7 +56667,7 @@
         <v>1782</v>
       </c>
       <c r="Q838" s="6">
-        <v>184.8</v>
+        <v>178.32</v>
       </c>
       <c r="R838" s="6" t="s">
         <v>23</v>
@@ -56677,7 +56785,7 @@
         <v>1790</v>
       </c>
       <c r="Q840" s="6">
-        <v>4711.5649999999996</v>
+        <v>4694.0950000000003</v>
       </c>
       <c r="R840" s="6" t="s">
         <v>23</v>
@@ -56736,7 +56844,7 @@
         <v>747</v>
       </c>
       <c r="Q841" s="6">
-        <v>732.5</v>
+        <v>721.73</v>
       </c>
       <c r="R841" s="6" t="s">
         <v>23</v>
@@ -56795,7 +56903,7 @@
         <v>1797</v>
       </c>
       <c r="Q842" s="6">
-        <v>48.5</v>
+        <v>147.5</v>
       </c>
       <c r="R842" s="6" t="s">
         <v>23</v>
@@ -56854,7 +56962,7 @@
         <v>1800</v>
       </c>
       <c r="Q843" s="6">
-        <v>391.01</v>
+        <v>382.66</v>
       </c>
       <c r="R843" s="6" t="s">
         <v>23</v>
@@ -56972,7 +57080,7 @@
         <v>1806</v>
       </c>
       <c r="Q845" s="6">
-        <v>412.8</v>
+        <v>311.12</v>
       </c>
       <c r="R845" s="6" t="s">
         <v>23</v>
@@ -57031,7 +57139,7 @@
         <v>1809</v>
       </c>
       <c r="Q846" s="6">
-        <v>169.3</v>
+        <v>189.3</v>
       </c>
       <c r="R846" s="6" t="s">
         <v>23</v>
@@ -57267,7 +57375,7 @@
         <v>1822</v>
       </c>
       <c r="Q850" s="6">
-        <v>1259.9000000000001</v>
+        <v>-134.6</v>
       </c>
       <c r="R850" s="6" t="s">
         <v>23</v>
@@ -57562,7 +57670,7 @@
         <v>1837</v>
       </c>
       <c r="Q855" s="6">
-        <v>84.5</v>
+        <v>395.27</v>
       </c>
       <c r="R855" s="6" t="s">
         <v>23</v>
@@ -57621,7 +57729,7 @@
         <v>1840</v>
       </c>
       <c r="Q856" s="6">
-        <v>176.9</v>
+        <v>137.69999999999999</v>
       </c>
       <c r="R856" s="6" t="s">
         <v>23</v>
@@ -57916,7 +58024,7 @@
         <v>1855</v>
       </c>
       <c r="Q861" s="6">
-        <v>16744.29</v>
+        <v>11819.3</v>
       </c>
       <c r="R861" s="6" t="s">
         <v>23</v>
@@ -58034,7 +58142,7 @@
         <v>1861</v>
       </c>
       <c r="Q863" s="6">
-        <v>1617.93</v>
+        <v>1528.57</v>
       </c>
       <c r="R863" s="6" t="s">
         <v>23</v>
@@ -58093,7 +58201,7 @@
         <v>1864</v>
       </c>
       <c r="Q864" s="6">
-        <v>1620.78</v>
+        <v>1333.01</v>
       </c>
       <c r="R864" s="6" t="s">
         <v>23</v>
@@ -58152,7 +58260,7 @@
         <v>1868</v>
       </c>
       <c r="Q865" s="6">
-        <v>706.34</v>
+        <v>547.54999999999995</v>
       </c>
       <c r="R865" s="6" t="s">
         <v>23</v>
@@ -58211,7 +58319,7 @@
         <v>1871</v>
       </c>
       <c r="Q866" s="6">
-        <v>2106.0500000000002</v>
+        <v>1839.5</v>
       </c>
       <c r="R866" s="6" t="s">
         <v>23</v>
@@ -58270,7 +58378,7 @@
         <v>1874</v>
       </c>
       <c r="Q867" s="6">
-        <v>46437.62</v>
+        <v>15515.98</v>
       </c>
       <c r="R867" s="6" t="s">
         <v>23</v>
@@ -58388,7 +58496,7 @@
         <v>1880</v>
       </c>
       <c r="Q869" s="6">
-        <v>134.19999999999999</v>
+        <v>0</v>
       </c>
       <c r="R869" s="6" t="s">
         <v>23</v>
@@ -58565,7 +58673,7 @@
         <v>1889</v>
       </c>
       <c r="Q872" s="6">
-        <v>309.85000000000002</v>
+        <v>268</v>
       </c>
       <c r="R872" s="6" t="s">
         <v>23</v>
@@ -58624,7 +58732,7 @@
         <v>1892</v>
       </c>
       <c r="Q873" s="6">
-        <v>346.82</v>
+        <v>322.52</v>
       </c>
       <c r="R873" s="6" t="s">
         <v>23</v>
@@ -58683,7 +58791,7 @@
         <v>1895</v>
       </c>
       <c r="Q874" s="6">
-        <v>701.02</v>
+        <v>676.72</v>
       </c>
       <c r="R874" s="6" t="s">
         <v>23</v>
@@ -58742,7 +58850,7 @@
         <v>1898</v>
       </c>
       <c r="Q875" s="6">
-        <v>109</v>
+        <v>101.19</v>
       </c>
       <c r="R875" s="6" t="s">
         <v>23</v>
@@ -58860,7 +58968,7 @@
         <v>1904</v>
       </c>
       <c r="Q877" s="6">
-        <v>341.26</v>
+        <v>378.4</v>
       </c>
       <c r="R877" s="6" t="s">
         <v>23</v>
@@ -58919,7 +59027,7 @@
         <v>1907</v>
       </c>
       <c r="Q878" s="6">
-        <v>110.08</v>
+        <v>88.72</v>
       </c>
       <c r="R878" s="6" t="s">
         <v>23</v>
@@ -59037,7 +59145,7 @@
         <v>1913</v>
       </c>
       <c r="Q880" s="6">
-        <v>147.18</v>
+        <v>125.82</v>
       </c>
       <c r="R880" s="6" t="s">
         <v>23</v>
@@ -59214,7 +59322,7 @@
         <v>1922</v>
       </c>
       <c r="Q883" s="6">
-        <v>36160</v>
+        <v>26305.74</v>
       </c>
       <c r="R883" s="6" t="s">
         <v>23</v>
@@ -59273,7 +59381,7 @@
         <v>1925</v>
       </c>
       <c r="Q884" s="6">
-        <v>8397.2000000000007</v>
+        <v>4999.1000000000004</v>
       </c>
       <c r="R884" s="6" t="s">
         <v>23</v>
@@ -59450,7 +59558,7 @@
         <v>1935</v>
       </c>
       <c r="Q887" s="6">
-        <v>152.63</v>
+        <v>120.53</v>
       </c>
       <c r="R887" s="6" t="s">
         <v>23</v>
@@ -59627,7 +59735,7 @@
         <v>1944</v>
       </c>
       <c r="Q890" s="6">
-        <v>279.88499999999999</v>
+        <v>237.13499999999999</v>
       </c>
       <c r="R890" s="6" t="s">
         <v>23</v>
@@ -61456,7 +61564,7 @@
         <v>2038</v>
       </c>
       <c r="Q921" s="6">
-        <v>3728.2</v>
+        <v>1465.78</v>
       </c>
       <c r="R921" s="6" t="s">
         <v>23</v>
@@ -61515,7 +61623,7 @@
         <v>2041</v>
       </c>
       <c r="Q922" s="6">
-        <v>22235.64</v>
+        <v>10057.42</v>
       </c>
       <c r="R922" s="6" t="s">
         <v>23</v>
@@ -61633,7 +61741,7 @@
         <v>2047</v>
       </c>
       <c r="Q924" s="6">
-        <v>19364.835800000001</v>
+        <v>7276.0630000000001</v>
       </c>
       <c r="R924" s="6" t="s">
         <v>23</v>
@@ -61751,7 +61859,7 @@
         <v>2053</v>
       </c>
       <c r="Q926" s="6">
-        <v>1864.355</v>
+        <v>1529.5</v>
       </c>
       <c r="R926" s="6" t="s">
         <v>23</v>
@@ -61928,7 +62036,7 @@
         <v>2062</v>
       </c>
       <c r="Q929" s="6">
-        <v>373.86</v>
+        <v>92.63</v>
       </c>
       <c r="R929" s="6" t="s">
         <v>23</v>
@@ -62105,7 +62213,7 @@
         <v>2071</v>
       </c>
       <c r="Q932" s="6">
-        <v>3789.86</v>
+        <v>3245.18</v>
       </c>
       <c r="R932" s="6" t="s">
         <v>23</v>
@@ -62282,7 +62390,7 @@
         <v>2080</v>
       </c>
       <c r="Q935" s="6">
-        <v>2658.89</v>
+        <v>1635.98</v>
       </c>
       <c r="R935" s="6" t="s">
         <v>23</v>
@@ -62341,7 +62449,7 @@
         <v>2083</v>
       </c>
       <c r="Q936" s="6">
-        <v>4298.12</v>
+        <v>3917.6</v>
       </c>
       <c r="R936" s="6" t="s">
         <v>23</v>
@@ -62400,7 +62508,7 @@
         <v>2086</v>
       </c>
       <c r="Q937" s="6">
-        <v>554.79999999999995</v>
+        <v>539.24</v>
       </c>
       <c r="R937" s="6" t="s">
         <v>23</v>
@@ -62518,7 +62626,7 @@
         <v>2092</v>
       </c>
       <c r="Q939" s="6">
-        <v>4620.66</v>
+        <v>4371.99</v>
       </c>
       <c r="R939" s="6" t="s">
         <v>23</v>
@@ -62577,7 +62685,7 @@
         <v>2095</v>
       </c>
       <c r="Q940" s="6">
-        <v>1051.8</v>
+        <v>780.8</v>
       </c>
       <c r="R940" s="6" t="s">
         <v>23</v>
@@ -62636,7 +62744,7 @@
         <v>2098</v>
       </c>
       <c r="Q941" s="6">
-        <v>954.23</v>
+        <v>427.71</v>
       </c>
       <c r="R941" s="6" t="s">
         <v>23</v>
@@ -62695,7 +62803,7 @@
         <v>2101</v>
       </c>
       <c r="Q942" s="6">
-        <v>1936.44</v>
+        <v>940.41</v>
       </c>
       <c r="R942" s="6" t="s">
         <v>23</v>
@@ -62754,7 +62862,7 @@
         <v>2104</v>
       </c>
       <c r="Q943" s="6">
-        <v>2202.91</v>
+        <v>1960.62</v>
       </c>
       <c r="R943" s="6" t="s">
         <v>23</v>
@@ -62813,7 +62921,7 @@
         <v>2107</v>
       </c>
       <c r="Q944" s="6">
-        <v>2726.3</v>
+        <v>3132.35</v>
       </c>
       <c r="R944" s="6" t="s">
         <v>23</v>
@@ -62872,7 +62980,7 @@
         <v>2110</v>
       </c>
       <c r="Q945" s="6">
-        <v>1726.3</v>
+        <v>1566</v>
       </c>
       <c r="R945" s="6" t="s">
         <v>23</v>
@@ -62972,10 +63080,10 @@
         <v>21</v>
       </c>
       <c r="K947" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L947" s="6">
-        <v>0</v>
+        <v>2.71</v>
       </c>
       <c r="M947" s="6">
         <v>0</v>
@@ -62990,7 +63098,7 @@
         <v>2116</v>
       </c>
       <c r="Q947" s="6">
-        <v>0</v>
+        <v>922.3</v>
       </c>
       <c r="R947" s="6" t="s">
         <v>23</v>
@@ -63108,7 +63216,7 @@
         <v>2122</v>
       </c>
       <c r="Q949" s="6">
-        <v>329.3</v>
+        <v>208.58</v>
       </c>
       <c r="R949" s="6" t="s">
         <v>23</v>
@@ -63167,7 +63275,7 @@
         <v>2125</v>
       </c>
       <c r="Q950" s="6">
-        <v>502.02499999999998</v>
+        <v>45.305</v>
       </c>
       <c r="R950" s="6" t="s">
         <v>23</v>
@@ -63226,7 +63334,7 @@
         <v>2128</v>
       </c>
       <c r="Q951" s="6">
-        <v>552.1</v>
+        <v>401.2</v>
       </c>
       <c r="R951" s="6" t="s">
         <v>23</v>
@@ -63285,7 +63393,7 @@
         <v>2131</v>
       </c>
       <c r="Q952" s="6">
-        <v>312.10000000000002</v>
+        <v>251.74</v>
       </c>
       <c r="R952" s="6" t="s">
         <v>23</v>
@@ -63344,7 +63452,7 @@
         <v>2134</v>
       </c>
       <c r="Q953" s="6">
-        <v>229.9</v>
+        <v>292.18</v>
       </c>
       <c r="R953" s="6" t="s">
         <v>23</v>
@@ -63403,7 +63511,7 @@
         <v>2137</v>
       </c>
       <c r="Q954" s="6">
-        <v>251.4</v>
+        <v>201.1</v>
       </c>
       <c r="R954" s="6" t="s">
         <v>23</v>
@@ -63462,7 +63570,7 @@
         <v>2140</v>
       </c>
       <c r="Q955" s="6">
-        <v>241.7</v>
+        <v>191.4</v>
       </c>
       <c r="R955" s="6" t="s">
         <v>23</v>
@@ -63639,7 +63747,7 @@
         <v>2149</v>
       </c>
       <c r="Q958" s="6">
-        <v>1352.6904</v>
+        <v>5698.4903999999997</v>
       </c>
       <c r="R958" s="6" t="s">
         <v>23</v>
@@ -63739,10 +63847,10 @@
         <v>21</v>
       </c>
       <c r="K960" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L960" s="6">
-        <v>0</v>
+        <v>3.29</v>
       </c>
       <c r="M960" s="6">
         <v>0</v>
@@ -63757,7 +63865,7 @@
         <v>2155</v>
       </c>
       <c r="Q960" s="6">
-        <v>0</v>
+        <v>590.20000000000005</v>
       </c>
       <c r="R960" s="6" t="s">
         <v>23</v>
@@ -64122,16 +64230,16 @@
     </row>
     <row r="967" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A967" s="5" t="s">
+        <v>2196</v>
+      </c>
+      <c r="B967" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C967" s="5" t="s">
         <v>2197</v>
       </c>
-      <c r="B967" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C967" s="5" t="s">
-        <v>2198</v>
-      </c>
       <c r="D967" s="5" t="s">
-        <v>2199</v>
+        <v>2229</v>
       </c>
       <c r="E967" s="6" t="s">
         <v>23</v>
@@ -64167,7 +64275,7 @@
         <v>21</v>
       </c>
       <c r="P967" s="5" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="Q967" s="6">
         <v>0</v>
@@ -64181,16 +64289,16 @@
     </row>
     <row r="968" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A968" s="5" t="s">
+        <v>2198</v>
+      </c>
+      <c r="B968" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C968" s="5" t="s">
+        <v>2199</v>
+      </c>
+      <c r="D968" s="5" t="s">
         <v>2200</v>
-      </c>
-      <c r="B968" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C968" s="5" t="s">
-        <v>2201</v>
-      </c>
-      <c r="D968" s="5" t="s">
-        <v>2202</v>
       </c>
       <c r="E968" s="6" t="s">
         <v>23</v>
@@ -64226,7 +64334,7 @@
         <v>21</v>
       </c>
       <c r="P968" s="5" t="s">
-        <v>2201</v>
+        <v>2199</v>
       </c>
       <c r="Q968" s="6">
         <v>0</v>
@@ -64240,16 +64348,16 @@
     </row>
     <row r="969" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A969" s="5" t="s">
+        <v>2201</v>
+      </c>
+      <c r="B969" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C969" s="5" t="s">
+        <v>2202</v>
+      </c>
+      <c r="D969" s="5" t="s">
         <v>2203</v>
-      </c>
-      <c r="B969" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C969" s="5" t="s">
-        <v>2204</v>
-      </c>
-      <c r="D969" s="5" t="s">
-        <v>2205</v>
       </c>
       <c r="E969" s="6" t="s">
         <v>23</v>
@@ -64285,7 +64393,7 @@
         <v>21</v>
       </c>
       <c r="P969" s="5" t="s">
-        <v>2204</v>
+        <v>2202</v>
       </c>
       <c r="Q969" s="6">
         <v>0</v>
@@ -64299,16 +64407,16 @@
     </row>
     <row r="970" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A970" s="5" t="s">
+        <v>2204</v>
+      </c>
+      <c r="B970" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C970" s="5" t="s">
+        <v>2205</v>
+      </c>
+      <c r="D970" s="5" t="s">
         <v>2206</v>
-      </c>
-      <c r="B970" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C970" s="5" t="s">
-        <v>2207</v>
-      </c>
-      <c r="D970" s="5" t="s">
-        <v>2208</v>
       </c>
       <c r="E970" s="6" t="s">
         <v>23</v>
@@ -64344,7 +64452,7 @@
         <v>21</v>
       </c>
       <c r="P970" s="5" t="s">
-        <v>2207</v>
+        <v>2205</v>
       </c>
       <c r="Q970" s="6">
         <v>0</v>
@@ -64358,16 +64466,16 @@
     </row>
     <row r="971" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A971" s="5" t="s">
+        <v>2207</v>
+      </c>
+      <c r="B971" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C971" s="5" t="s">
+        <v>2208</v>
+      </c>
+      <c r="D971" s="5" t="s">
         <v>2209</v>
-      </c>
-      <c r="B971" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C971" s="5" t="s">
-        <v>2210</v>
-      </c>
-      <c r="D971" s="5" t="s">
-        <v>2211</v>
       </c>
       <c r="E971" s="6" t="s">
         <v>23</v>
@@ -64403,7 +64511,7 @@
         <v>21</v>
       </c>
       <c r="P971" s="5" t="s">
-        <v>2210</v>
+        <v>2208</v>
       </c>
       <c r="Q971" s="6">
         <v>0</v>
@@ -64417,16 +64525,16 @@
     </row>
     <row r="972" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A972" s="5" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B972" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C972" s="5" t="s">
+        <v>2211</v>
+      </c>
+      <c r="D972" s="5" t="s">
         <v>2212</v>
-      </c>
-      <c r="B972" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C972" s="5" t="s">
-        <v>2213</v>
-      </c>
-      <c r="D972" s="5" t="s">
-        <v>2214</v>
       </c>
       <c r="E972" s="6" t="s">
         <v>23</v>
@@ -64462,7 +64570,7 @@
         <v>21</v>
       </c>
       <c r="P972" s="5" t="s">
-        <v>2213</v>
+        <v>2211</v>
       </c>
       <c r="Q972" s="6">
         <v>0</v>
@@ -64476,16 +64584,16 @@
     </row>
     <row r="973" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A973" s="5" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B973" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C973" s="5" t="s">
+        <v>2214</v>
+      </c>
+      <c r="D973" s="5" t="s">
         <v>2215</v>
-      </c>
-      <c r="B973" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C973" s="5" t="s">
-        <v>2216</v>
-      </c>
-      <c r="D973" s="5" t="s">
-        <v>2217</v>
       </c>
       <c r="E973" s="6" t="s">
         <v>23</v>
@@ -64521,7 +64629,7 @@
         <v>21</v>
       </c>
       <c r="P973" s="5" t="s">
-        <v>2216</v>
+        <v>2214</v>
       </c>
       <c r="Q973" s="6">
         <v>0</v>
@@ -64535,16 +64643,16 @@
     </row>
     <row r="974" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A974" s="5" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B974" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C974" s="5" t="s">
+        <v>2217</v>
+      </c>
+      <c r="D974" s="5" t="s">
         <v>2218</v>
-      </c>
-      <c r="B974" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C974" s="5" t="s">
-        <v>2219</v>
-      </c>
-      <c r="D974" s="5" t="s">
-        <v>2220</v>
       </c>
       <c r="E974" s="6" t="s">
         <v>23</v>
@@ -64580,7 +64688,7 @@
         <v>21</v>
       </c>
       <c r="P974" s="5" t="s">
-        <v>2219</v>
+        <v>2217</v>
       </c>
       <c r="Q974" s="6">
         <v>0</v>
@@ -64594,16 +64702,16 @@
     </row>
     <row r="975" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A975" s="5" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B975" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C975" s="5" t="s">
+        <v>2220</v>
+      </c>
+      <c r="D975" s="5" t="s">
         <v>2221</v>
-      </c>
-      <c r="B975" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C975" s="5" t="s">
-        <v>2222</v>
-      </c>
-      <c r="D975" s="5" t="s">
-        <v>2223</v>
       </c>
       <c r="E975" s="6" t="s">
         <v>23</v>
@@ -64639,7 +64747,7 @@
         <v>21</v>
       </c>
       <c r="P975" s="5" t="s">
-        <v>2222</v>
+        <v>2220</v>
       </c>
       <c r="Q975" s="6">
         <v>0</v>
@@ -64653,16 +64761,16 @@
     </row>
     <row r="976" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A976" s="5" t="s">
+        <v>2222</v>
+      </c>
+      <c r="B976" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C976" s="5" t="s">
+        <v>2223</v>
+      </c>
+      <c r="D976" s="5" t="s">
         <v>2224</v>
-      </c>
-      <c r="B976" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C976" s="5" t="s">
-        <v>2225</v>
-      </c>
-      <c r="D976" s="5" t="s">
-        <v>2226</v>
       </c>
       <c r="E976" s="6" t="s">
         <v>23</v>
@@ -64698,7 +64806,7 @@
         <v>21</v>
       </c>
       <c r="P976" s="5" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
       <c r="Q976" s="6">
         <v>0</v>
@@ -64712,16 +64820,16 @@
     </row>
     <row r="977" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A977" s="5" t="s">
+        <v>2225</v>
+      </c>
+      <c r="B977" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C977" s="5" t="s">
+        <v>2226</v>
+      </c>
+      <c r="D977" s="5" t="s">
         <v>2227</v>
-      </c>
-      <c r="B977" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C977" s="5" t="s">
-        <v>2228</v>
-      </c>
-      <c r="D977" s="5" t="s">
-        <v>2229</v>
       </c>
       <c r="E977" s="6" t="s">
         <v>23</v>
@@ -64757,7 +64865,7 @@
         <v>21</v>
       </c>
       <c r="P977" s="5" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="Q977" s="6">
         <v>0</v>
@@ -64771,16 +64879,16 @@
     </row>
     <row r="978" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A978" s="5" t="s">
-        <v>2166</v>
+        <v>2230</v>
       </c>
       <c r="B978" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C978" s="5" t="s">
-        <v>2167</v>
+        <v>2231</v>
       </c>
       <c r="D978" s="5" t="s">
-        <v>2168</v>
+        <v>2232</v>
       </c>
       <c r="E978" s="6" t="s">
         <v>23</v>
@@ -64801,10 +64909,10 @@
         <v>21</v>
       </c>
       <c r="K978" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L978" s="6">
-        <v>1.98</v>
+        <v>0</v>
       </c>
       <c r="M978" s="6">
         <v>0</v>
@@ -64816,10 +64924,10 @@
         <v>21</v>
       </c>
       <c r="P978" s="5" t="s">
-        <v>2167</v>
+        <v>2231</v>
       </c>
       <c r="Q978" s="6">
-        <v>589.70000000000005</v>
+        <v>0</v>
       </c>
       <c r="R978" s="6" t="s">
         <v>23</v>
@@ -64830,16 +64938,16 @@
     </row>
     <row r="979" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A979" s="5" t="s">
-        <v>2169</v>
+        <v>2233</v>
       </c>
       <c r="B979" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C979" s="5" t="s">
-        <v>2170</v>
+        <v>2234</v>
       </c>
       <c r="D979" s="5" t="s">
-        <v>2171</v>
+        <v>2235</v>
       </c>
       <c r="E979" s="6" t="s">
         <v>23</v>
@@ -64860,10 +64968,10 @@
         <v>21</v>
       </c>
       <c r="K979" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L979" s="6">
-        <v>3.75</v>
+        <v>0</v>
       </c>
       <c r="M979" s="6">
         <v>0</v>
@@ -64875,10 +64983,10 @@
         <v>21</v>
       </c>
       <c r="P979" s="5" t="s">
-        <v>2170</v>
+        <v>2234</v>
       </c>
       <c r="Q979" s="6">
-        <v>102.8</v>
+        <v>0</v>
       </c>
       <c r="R979" s="6" t="s">
         <v>23</v>
@@ -64889,16 +64997,16 @@
     </row>
     <row r="980" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A980" s="5" t="s">
-        <v>2172</v>
+        <v>2236</v>
       </c>
       <c r="B980" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C980" s="5" t="s">
-        <v>2173</v>
+        <v>2237</v>
       </c>
       <c r="D980" s="5" t="s">
-        <v>2174</v>
+        <v>2238</v>
       </c>
       <c r="E980" s="6" t="s">
         <v>23</v>
@@ -64919,10 +65027,10 @@
         <v>21</v>
       </c>
       <c r="K980" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L980" s="6">
-        <v>2.65</v>
+        <v>0</v>
       </c>
       <c r="M980" s="6">
         <v>0</v>
@@ -64934,10 +65042,10 @@
         <v>21</v>
       </c>
       <c r="P980" s="5" t="s">
-        <v>2173</v>
+        <v>2237</v>
       </c>
       <c r="Q980" s="6">
-        <v>1757.67</v>
+        <v>0</v>
       </c>
       <c r="R980" s="6" t="s">
         <v>23</v>
@@ -64948,16 +65056,16 @@
     </row>
     <row r="981" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A981" s="5" t="s">
-        <v>2190</v>
+        <v>2239</v>
       </c>
       <c r="B981" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C981" s="5" t="s">
-        <v>2191</v>
+        <v>2240</v>
       </c>
       <c r="D981" s="5" t="s">
-        <v>2192</v>
+        <v>2241</v>
       </c>
       <c r="E981" s="6" t="s">
         <v>23</v>
@@ -64993,7 +65101,7 @@
         <v>21</v>
       </c>
       <c r="P981" s="5" t="s">
-        <v>2191</v>
+        <v>2240</v>
       </c>
       <c r="Q981" s="6">
         <v>0</v>
@@ -65007,16 +65115,16 @@
     </row>
     <row r="982" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A982" s="5" t="s">
-        <v>2193</v>
+        <v>2242</v>
       </c>
       <c r="B982" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C982" s="5" t="s">
-        <v>2194</v>
+        <v>2243</v>
       </c>
       <c r="D982" s="5" t="s">
-        <v>2195</v>
+        <v>2244</v>
       </c>
       <c r="E982" s="6" t="s">
         <v>23</v>
@@ -65052,15 +65160,723 @@
         <v>21</v>
       </c>
       <c r="P982" s="5" t="s">
+        <v>2243</v>
+      </c>
+      <c r="Q982" s="6">
+        <v>0</v>
+      </c>
+      <c r="R982" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S982" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="983" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A983" s="5" t="s">
+        <v>2245</v>
+      </c>
+      <c r="B983" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C983" s="5" t="s">
+        <v>2246</v>
+      </c>
+      <c r="D983" s="5" t="s">
+        <v>2247</v>
+      </c>
+      <c r="E983" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F983" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G983" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H983" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I983" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J983" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K983" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L983" s="6">
+        <v>0</v>
+      </c>
+      <c r="M983" s="6">
+        <v>0</v>
+      </c>
+      <c r="N983" s="6">
+        <v>0</v>
+      </c>
+      <c r="O983" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P983" s="5" t="s">
+        <v>2246</v>
+      </c>
+      <c r="Q983" s="6">
+        <v>0</v>
+      </c>
+      <c r="R983" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S983" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="984" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A984" s="5" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B984" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C984" s="5" t="s">
+        <v>2249</v>
+      </c>
+      <c r="D984" s="5" t="s">
+        <v>2250</v>
+      </c>
+      <c r="E984" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F984" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G984" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H984" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I984" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J984" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K984" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L984" s="6">
+        <v>0</v>
+      </c>
+      <c r="M984" s="6">
+        <v>0</v>
+      </c>
+      <c r="N984" s="6">
+        <v>0</v>
+      </c>
+      <c r="O984" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P984" s="5" t="s">
+        <v>2249</v>
+      </c>
+      <c r="Q984" s="6">
+        <v>0</v>
+      </c>
+      <c r="R984" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S984" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="985" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A985" s="5" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B985" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C985" s="5" t="s">
+        <v>2252</v>
+      </c>
+      <c r="D985" s="5" t="s">
+        <v>2253</v>
+      </c>
+      <c r="E985" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F985" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G985" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H985" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I985" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J985" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K985" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L985" s="6">
+        <v>0</v>
+      </c>
+      <c r="M985" s="6">
+        <v>0</v>
+      </c>
+      <c r="N985" s="6">
+        <v>0</v>
+      </c>
+      <c r="O985" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P985" s="5" t="s">
+        <v>2252</v>
+      </c>
+      <c r="Q985" s="6">
+        <v>0</v>
+      </c>
+      <c r="R985" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S985" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="986" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A986" s="5" t="s">
+        <v>2254</v>
+      </c>
+      <c r="B986" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C986" s="5" t="s">
+        <v>2255</v>
+      </c>
+      <c r="D986" s="5" t="s">
+        <v>2256</v>
+      </c>
+      <c r="E986" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F986" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G986" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H986" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I986" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J986" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K986" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L986" s="6">
+        <v>0</v>
+      </c>
+      <c r="M986" s="6">
+        <v>0</v>
+      </c>
+      <c r="N986" s="6">
+        <v>0</v>
+      </c>
+      <c r="O986" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P986" s="5" t="s">
+        <v>2255</v>
+      </c>
+      <c r="Q986" s="6">
+        <v>0</v>
+      </c>
+      <c r="R986" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S986" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="987" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A987" s="5" t="s">
+        <v>2257</v>
+      </c>
+      <c r="B987" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C987" s="5" t="s">
+        <v>2258</v>
+      </c>
+      <c r="D987" s="5" t="s">
+        <v>2259</v>
+      </c>
+      <c r="E987" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F987" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G987" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H987" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I987" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J987" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K987" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L987" s="6">
+        <v>0</v>
+      </c>
+      <c r="M987" s="6">
+        <v>0</v>
+      </c>
+      <c r="N987" s="6">
+        <v>0</v>
+      </c>
+      <c r="O987" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P987" s="5" t="s">
+        <v>2258</v>
+      </c>
+      <c r="Q987" s="6">
+        <v>0</v>
+      </c>
+      <c r="R987" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S987" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="988" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A988" s="5" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B988" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C988" s="5" t="s">
+        <v>2261</v>
+      </c>
+      <c r="D988" s="5" t="s">
+        <v>2262</v>
+      </c>
+      <c r="E988" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F988" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G988" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H988" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I988" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J988" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K988" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L988" s="6">
+        <v>0</v>
+      </c>
+      <c r="M988" s="6">
+        <v>0</v>
+      </c>
+      <c r="N988" s="6">
+        <v>0</v>
+      </c>
+      <c r="O988" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P988" s="5" t="s">
+        <v>2261</v>
+      </c>
+      <c r="Q988" s="6">
+        <v>0</v>
+      </c>
+      <c r="R988" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S988" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="989" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A989" s="5" t="s">
+        <v>2263</v>
+      </c>
+      <c r="B989" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C989" s="5" t="s">
+        <v>2264</v>
+      </c>
+      <c r="D989" s="5" t="s">
+        <v>2265</v>
+      </c>
+      <c r="E989" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F989" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G989" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H989" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I989" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J989" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K989" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L989" s="6">
+        <v>0</v>
+      </c>
+      <c r="M989" s="6">
+        <v>0</v>
+      </c>
+      <c r="N989" s="6">
+        <v>0</v>
+      </c>
+      <c r="O989" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P989" s="5" t="s">
+        <v>2264</v>
+      </c>
+      <c r="Q989" s="6">
+        <v>0</v>
+      </c>
+      <c r="R989" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S989" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="990" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A990" s="5" t="s">
+        <v>2166</v>
+      </c>
+      <c r="B990" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C990" s="5" t="s">
+        <v>2167</v>
+      </c>
+      <c r="D990" s="5" t="s">
+        <v>2168</v>
+      </c>
+      <c r="E990" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F990" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G990" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H990" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I990" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J990" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K990" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L990" s="6">
+        <v>1.98</v>
+      </c>
+      <c r="M990" s="6">
+        <v>0</v>
+      </c>
+      <c r="N990" s="6">
+        <v>0</v>
+      </c>
+      <c r="O990" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P990" s="5" t="s">
+        <v>2167</v>
+      </c>
+      <c r="Q990" s="6">
+        <v>589.70000000000005</v>
+      </c>
+      <c r="R990" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S990" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="991" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A991" s="5" t="s">
+        <v>2169</v>
+      </c>
+      <c r="B991" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C991" s="5" t="s">
+        <v>2170</v>
+      </c>
+      <c r="D991" s="5" t="s">
+        <v>2171</v>
+      </c>
+      <c r="E991" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F991" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G991" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H991" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I991" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J991" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K991" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L991" s="6">
+        <v>3.75</v>
+      </c>
+      <c r="M991" s="6">
+        <v>0</v>
+      </c>
+      <c r="N991" s="6">
+        <v>0</v>
+      </c>
+      <c r="O991" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P991" s="5" t="s">
+        <v>2170</v>
+      </c>
+      <c r="Q991" s="6">
+        <v>503.7</v>
+      </c>
+      <c r="R991" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S991" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="992" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A992" s="5" t="s">
+        <v>2172</v>
+      </c>
+      <c r="B992" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C992" s="5" t="s">
+        <v>2173</v>
+      </c>
+      <c r="D992" s="5" t="s">
+        <v>2174</v>
+      </c>
+      <c r="E992" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F992" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G992" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H992" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I992" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J992" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K992" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L992" s="6">
+        <v>2.65</v>
+      </c>
+      <c r="M992" s="6">
+        <v>0</v>
+      </c>
+      <c r="N992" s="6">
+        <v>0</v>
+      </c>
+      <c r="O992" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P992" s="5" t="s">
+        <v>2173</v>
+      </c>
+      <c r="Q992" s="6">
+        <v>1479.87</v>
+      </c>
+      <c r="R992" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S992" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="993" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A993" s="5" t="s">
+        <v>2190</v>
+      </c>
+      <c r="B993" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C993" s="5" t="s">
+        <v>2191</v>
+      </c>
+      <c r="D993" s="5" t="s">
+        <v>2192</v>
+      </c>
+      <c r="E993" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F993" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G993" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H993" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I993" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J993" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K993" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L993" s="6">
+        <v>0</v>
+      </c>
+      <c r="M993" s="6">
+        <v>0</v>
+      </c>
+      <c r="N993" s="6">
+        <v>0</v>
+      </c>
+      <c r="O993" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P993" s="5" t="s">
+        <v>2191</v>
+      </c>
+      <c r="Q993" s="6">
+        <v>0</v>
+      </c>
+      <c r="R993" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S993" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="994" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A994" s="5" t="s">
+        <v>2193</v>
+      </c>
+      <c r="B994" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C994" s="5" t="s">
         <v>2194</v>
       </c>
-      <c r="Q982" s="6">
-        <v>0</v>
-      </c>
-      <c r="R982" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="S982" s="5" t="s">
+      <c r="D994" s="5" t="s">
+        <v>2195</v>
+      </c>
+      <c r="E994" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F994" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G994" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H994" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I994" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J994" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K994" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L994" s="6">
+        <v>0</v>
+      </c>
+      <c r="M994" s="6">
+        <v>0</v>
+      </c>
+      <c r="N994" s="6">
+        <v>0</v>
+      </c>
+      <c r="O994" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P994" s="5" t="s">
+        <v>2194</v>
+      </c>
+      <c r="Q994" s="6">
+        <v>0</v>
+      </c>
+      <c r="R994" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S994" s="5" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
act db excell 21022020
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/TC_02.xlsx
+++ b/EXCEL LIBS/TC_02.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14931" uniqueCount="2275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15081" uniqueCount="2305">
   <si>
     <t>sqlnav01.aquinos.org : Aquinos, S.A.</t>
   </si>
@@ -6475,9 +6475,6 @@
     <t>G2810</t>
   </si>
   <si>
-    <t>TEXAS 480 C.91 (ELEFANT)</t>
-  </si>
-  <si>
     <t>TC15139</t>
   </si>
   <si>
@@ -6709,18 +6706,12 @@
     <t>BOLSHOI 01 | YANODA 22 (BRANCO)</t>
   </si>
   <si>
-    <t>MACAU - CUOIO (AMARELO TORRADO)</t>
-  </si>
-  <si>
     <t>TC15158</t>
   </si>
   <si>
     <t>G2842</t>
   </si>
   <si>
-    <t>TEXAS 480 C.95 (TAUPE)</t>
-  </si>
-  <si>
     <t>TC15159</t>
   </si>
   <si>
@@ -6820,9 +6811,6 @@
     <t>PERSA ASH 12</t>
   </si>
   <si>
-    <t>Lista Produto : 11-02-2020 10:36:43</t>
-  </si>
-  <si>
     <t>TC15170</t>
   </si>
   <si>
@@ -6848,6 +6836,108 @@
   </si>
   <si>
     <t>MACAU - BLACK (PRETO)</t>
+  </si>
+  <si>
+    <t>Lista Produto : 21-02-2020 11:18:22</t>
+  </si>
+  <si>
+    <t>TEXAS 480 C.91 (ANTRACITE)</t>
+  </si>
+  <si>
+    <t>MACAU -CUOIO (AMARELO TORRADO)</t>
+  </si>
+  <si>
+    <t>TEXAS 480 C.95 (ELEFANT)</t>
+  </si>
+  <si>
+    <t>TC15173</t>
+  </si>
+  <si>
+    <t>G3840</t>
+  </si>
+  <si>
+    <t>QUEENS STAR - CAMEL</t>
+  </si>
+  <si>
+    <t>TC15174</t>
+  </si>
+  <si>
+    <t>G3820</t>
+  </si>
+  <si>
+    <t>QUEENS STAR - TURQUOISE</t>
+  </si>
+  <si>
+    <t>TC15175</t>
+  </si>
+  <si>
+    <t>G3850</t>
+  </si>
+  <si>
+    <t>QUEENS STAR - BORDEAUX</t>
+  </si>
+  <si>
+    <t>TC15176</t>
+  </si>
+  <si>
+    <t>G3810</t>
+  </si>
+  <si>
+    <t>QUEENS STAR - LIGHT GREY</t>
+  </si>
+  <si>
+    <t>TC15177</t>
+  </si>
+  <si>
+    <t>G3811</t>
+  </si>
+  <si>
+    <t>QUEENS STAR - ASH</t>
+  </si>
+  <si>
+    <t>TC15178</t>
+  </si>
+  <si>
+    <t>G3841</t>
+  </si>
+  <si>
+    <t>QUEENS STAR - BROWN</t>
+  </si>
+  <si>
+    <t>TC15179</t>
+  </si>
+  <si>
+    <t>G3801</t>
+  </si>
+  <si>
+    <t>QUEENS STAR - BLACK</t>
+  </si>
+  <si>
+    <t>TC15180</t>
+  </si>
+  <si>
+    <t>G3860</t>
+  </si>
+  <si>
+    <t>QUEENS STAR - YELLOW</t>
+  </si>
+  <si>
+    <t>TC15181</t>
+  </si>
+  <si>
+    <t>G3910</t>
+  </si>
+  <si>
+    <t>LUX 05 - LIGHT GREY</t>
+  </si>
+  <si>
+    <t>TC15182</t>
+  </si>
+  <si>
+    <t>G3911</t>
+  </si>
+  <si>
+    <t>LUX 06 - DARK GREY</t>
   </si>
 </sst>
 </file>
@@ -7014,8 +7104,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NavDataRegion" displayName="NavDataRegion" ref="A3:S997" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A3:S997"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NavDataRegion" displayName="NavDataRegion" ref="A3:S1007" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A3:S1007"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Nº" dataDxfId="16"/>
     <tableColumn id="2" name="Cód. Barras Efacec" dataDxfId="15"/>
@@ -7304,7 +7394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S997"/>
+  <dimension ref="A1:S1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F977" sqref="F977"/>
@@ -7358,7 +7448,7 @@
     </row>
     <row r="2" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2265</v>
+        <v>2271</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -7473,7 +7563,7 @@
         <v>23</v>
       </c>
       <c r="L4" s="6">
-        <v>2.8</v>
+        <v>2.78</v>
       </c>
       <c r="M4" s="6">
         <v>0</v>
@@ -7488,7 +7578,7 @@
         <v>22</v>
       </c>
       <c r="Q4" s="6">
-        <v>0</v>
+        <v>8782</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>23</v>
@@ -7532,7 +7622,7 @@
         <v>23</v>
       </c>
       <c r="L5" s="6">
-        <v>5.1100000000000003</v>
+        <v>3.42</v>
       </c>
       <c r="M5" s="6">
         <v>0</v>
@@ -7547,7 +7637,7 @@
         <v>26</v>
       </c>
       <c r="Q5" s="6">
-        <v>0</v>
+        <v>8559</v>
       </c>
       <c r="R5" s="6" t="s">
         <v>23</v>
@@ -7591,7 +7681,7 @@
         <v>23</v>
       </c>
       <c r="L6" s="6">
-        <v>5.1100000000000003</v>
+        <v>2.95</v>
       </c>
       <c r="M6" s="6">
         <v>0</v>
@@ -7606,7 +7696,7 @@
         <v>28</v>
       </c>
       <c r="Q6" s="6">
-        <v>0</v>
+        <v>6102</v>
       </c>
       <c r="R6" s="6" t="s">
         <v>23</v>
@@ -17105,7 +17195,7 @@
         <v>353</v>
       </c>
       <c r="Q167" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R167" s="6" t="s">
         <v>23</v>
@@ -17754,7 +17844,7 @@
         <v>376</v>
       </c>
       <c r="Q178" s="6">
-        <v>835.65359999999998</v>
+        <v>627.7636</v>
       </c>
       <c r="R178" s="6" t="s">
         <v>23</v>
@@ -17813,7 +17903,7 @@
         <v>378</v>
       </c>
       <c r="Q179" s="6">
-        <v>785.19</v>
+        <v>559.69000000000005</v>
       </c>
       <c r="R179" s="6" t="s">
         <v>23</v>
@@ -18285,7 +18375,7 @@
         <v>394</v>
       </c>
       <c r="Q187" s="6">
-        <v>4884.9799999999996</v>
+        <v>3099.66</v>
       </c>
       <c r="R187" s="6" t="s">
         <v>23</v>
@@ -18639,7 +18729,7 @@
         <v>406</v>
       </c>
       <c r="Q193" s="6">
-        <v>1849.7</v>
+        <v>1470.35</v>
       </c>
       <c r="R193" s="6" t="s">
         <v>23</v>
@@ -18934,7 +19024,7 @@
         <v>416</v>
       </c>
       <c r="Q198" s="6">
-        <v>1180.2</v>
+        <v>680.4</v>
       </c>
       <c r="R198" s="6" t="s">
         <v>23</v>
@@ -19583,7 +19673,7 @@
         <v>438</v>
       </c>
       <c r="Q209" s="6">
-        <v>3502.46</v>
+        <v>2459.65</v>
       </c>
       <c r="R209" s="6" t="s">
         <v>23</v>
@@ -20350,7 +20440,7 @@
         <v>464</v>
       </c>
       <c r="Q222" s="6">
-        <v>3667.4472000000001</v>
+        <v>2940.9011999999998</v>
       </c>
       <c r="R222" s="6" t="s">
         <v>23</v>
@@ -20409,7 +20499,7 @@
         <v>466</v>
       </c>
       <c r="Q223" s="6">
-        <v>1908.11</v>
+        <v>1894.99</v>
       </c>
       <c r="R223" s="6" t="s">
         <v>23</v>
@@ -20645,7 +20735,7 @@
         <v>474</v>
       </c>
       <c r="Q227" s="6">
-        <v>9093.2800000000007</v>
+        <v>6918.28</v>
       </c>
       <c r="R227" s="6" t="s">
         <v>23</v>
@@ -20704,7 +20794,7 @@
         <v>476</v>
       </c>
       <c r="Q228" s="6">
-        <v>6891.23</v>
+        <v>5523.73</v>
       </c>
       <c r="R228" s="6" t="s">
         <v>23</v>
@@ -21412,7 +21502,7 @@
         <v>500</v>
       </c>
       <c r="Q240" s="6">
-        <v>3176.4690000000001</v>
+        <v>3151.8389999999999</v>
       </c>
       <c r="R240" s="6" t="s">
         <v>23</v>
@@ -21471,7 +21561,7 @@
         <v>502</v>
       </c>
       <c r="Q241" s="6">
-        <v>2385.15</v>
+        <v>2590.5500000000002</v>
       </c>
       <c r="R241" s="6" t="s">
         <v>23</v>
@@ -21589,7 +21679,7 @@
         <v>506</v>
       </c>
       <c r="Q243" s="6">
-        <v>617.20000000000005</v>
+        <v>608.91999999999996</v>
       </c>
       <c r="R243" s="6" t="s">
         <v>23</v>
@@ -21825,7 +21915,7 @@
         <v>514</v>
       </c>
       <c r="Q247" s="6">
-        <v>51.52</v>
+        <v>202.59</v>
       </c>
       <c r="R247" s="6" t="s">
         <v>23</v>
@@ -21884,7 +21974,7 @@
         <v>516</v>
       </c>
       <c r="Q248" s="6">
-        <v>2465.42</v>
+        <v>877.86</v>
       </c>
       <c r="R248" s="6" t="s">
         <v>23</v>
@@ -22002,7 +22092,7 @@
         <v>520</v>
       </c>
       <c r="Q250" s="6">
-        <v>283.12</v>
+        <v>-2450.36</v>
       </c>
       <c r="R250" s="6" t="s">
         <v>23</v>
@@ -22046,7 +22136,7 @@
         <v>23</v>
       </c>
       <c r="L251" s="6">
-        <v>2.17</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="M251" s="6">
         <v>0</v>
@@ -22061,7 +22151,7 @@
         <v>522</v>
       </c>
       <c r="Q251" s="6">
-        <v>490.56</v>
+        <v>587.05999999999995</v>
       </c>
       <c r="R251" s="6" t="s">
         <v>23</v>
@@ -22887,7 +22977,7 @@
         <v>550</v>
       </c>
       <c r="Q265" s="6">
-        <v>1716.9</v>
+        <v>1426.9</v>
       </c>
       <c r="R265" s="6" t="s">
         <v>23</v>
@@ -22946,7 +23036,7 @@
         <v>552</v>
       </c>
       <c r="Q266" s="6">
-        <v>3675.69</v>
+        <v>2805.69</v>
       </c>
       <c r="R266" s="6" t="s">
         <v>23</v>
@@ -23064,7 +23154,7 @@
         <v>556</v>
       </c>
       <c r="Q268" s="6">
-        <v>924.33</v>
+        <v>1384.43</v>
       </c>
       <c r="R268" s="6" t="s">
         <v>23</v>
@@ -23713,7 +23803,7 @@
         <v>579</v>
       </c>
       <c r="Q279" s="6">
-        <v>108.23180000000001</v>
+        <v>107.4618</v>
       </c>
       <c r="R279" s="6" t="s">
         <v>23</v>
@@ -23772,7 +23862,7 @@
         <v>581</v>
       </c>
       <c r="Q280" s="6">
-        <v>609.6</v>
+        <v>554.98</v>
       </c>
       <c r="R280" s="6" t="s">
         <v>23</v>
@@ -24067,7 +24157,7 @@
         <v>591</v>
       </c>
       <c r="Q285" s="6">
-        <v>344.2</v>
+        <v>843.9</v>
       </c>
       <c r="R285" s="6" t="s">
         <v>23</v>
@@ -24126,7 +24216,7 @@
         <v>593</v>
       </c>
       <c r="Q286" s="6">
-        <v>1104.52</v>
+        <v>1028.98</v>
       </c>
       <c r="R286" s="6" t="s">
         <v>23</v>
@@ -24185,7 +24275,7 @@
         <v>595</v>
       </c>
       <c r="Q287" s="6">
-        <v>2554.4949999999999</v>
+        <v>2385.9650000000001</v>
       </c>
       <c r="R287" s="6" t="s">
         <v>23</v>
@@ -24244,7 +24334,7 @@
         <v>597</v>
       </c>
       <c r="Q288" s="6">
-        <v>1869.01</v>
+        <v>1814.77</v>
       </c>
       <c r="R288" s="6" t="s">
         <v>23</v>
@@ -24362,7 +24452,7 @@
         <v>601</v>
       </c>
       <c r="Q290" s="6">
-        <v>3681.8649999999998</v>
+        <v>3569.3049999999998</v>
       </c>
       <c r="R290" s="6" t="s">
         <v>23</v>
@@ -24421,7 +24511,7 @@
         <v>603</v>
       </c>
       <c r="Q291" s="6">
-        <v>3905.8890000000001</v>
+        <v>2595.569</v>
       </c>
       <c r="R291" s="6" t="s">
         <v>23</v>
@@ -24480,7 +24570,7 @@
         <v>605</v>
       </c>
       <c r="Q292" s="6">
-        <v>1239.31</v>
+        <v>1151.1199999999999</v>
       </c>
       <c r="R292" s="6" t="s">
         <v>23</v>
@@ -24716,7 +24806,7 @@
         <v>613</v>
       </c>
       <c r="Q296" s="6">
-        <v>1255.2</v>
+        <v>1244.93</v>
       </c>
       <c r="R296" s="6" t="s">
         <v>23</v>
@@ -24775,7 +24865,7 @@
         <v>615</v>
       </c>
       <c r="Q297" s="6">
-        <v>3513.98</v>
+        <v>3419.41</v>
       </c>
       <c r="R297" s="6" t="s">
         <v>23</v>
@@ -24893,7 +24983,7 @@
         <v>619</v>
       </c>
       <c r="Q299" s="6">
-        <v>1113</v>
+        <v>908.45</v>
       </c>
       <c r="R299" s="6" t="s">
         <v>23</v>
@@ -24952,7 +25042,7 @@
         <v>621</v>
       </c>
       <c r="Q300" s="6">
-        <v>2321.06</v>
+        <v>1753.88</v>
       </c>
       <c r="R300" s="6" t="s">
         <v>23</v>
@@ -25011,7 +25101,7 @@
         <v>623</v>
       </c>
       <c r="Q301" s="6">
-        <v>1482.5</v>
+        <v>1171.18</v>
       </c>
       <c r="R301" s="6" t="s">
         <v>23</v>
@@ -25070,7 +25160,7 @@
         <v>625</v>
       </c>
       <c r="Q302" s="6">
-        <v>3897.36</v>
+        <v>1418.87</v>
       </c>
       <c r="R302" s="6" t="s">
         <v>23</v>
@@ -25129,7 +25219,7 @@
         <v>627</v>
       </c>
       <c r="Q303" s="6">
-        <v>46097.3024</v>
+        <v>42658.202400000002</v>
       </c>
       <c r="R303" s="6" t="s">
         <v>23</v>
@@ -25188,7 +25278,7 @@
         <v>629</v>
       </c>
       <c r="Q304" s="6">
-        <v>73689.790999999997</v>
+        <v>36441.870999999999</v>
       </c>
       <c r="R304" s="6" t="s">
         <v>23</v>
@@ -25247,7 +25337,7 @@
         <v>631</v>
       </c>
       <c r="Q305" s="6">
-        <v>2604.2399999999998</v>
+        <v>2408.59</v>
       </c>
       <c r="R305" s="6" t="s">
         <v>23</v>
@@ -25306,7 +25396,7 @@
         <v>633</v>
       </c>
       <c r="Q306" s="6">
-        <v>2680.4949999999999</v>
+        <v>24.585000000000001</v>
       </c>
       <c r="R306" s="6" t="s">
         <v>23</v>
@@ -25660,7 +25750,7 @@
         <v>646</v>
       </c>
       <c r="Q312" s="6">
-        <v>2947.67</v>
+        <v>2868.68</v>
       </c>
       <c r="R312" s="6" t="s">
         <v>23</v>
@@ -25719,7 +25809,7 @@
         <v>649</v>
       </c>
       <c r="Q313" s="6">
-        <v>230.2</v>
+        <v>178.88</v>
       </c>
       <c r="R313" s="6" t="s">
         <v>23</v>
@@ -25778,7 +25868,7 @@
         <v>652</v>
       </c>
       <c r="Q314" s="6">
-        <v>2272.08</v>
+        <v>2268.33</v>
       </c>
       <c r="R314" s="6" t="s">
         <v>23</v>
@@ -25896,7 +25986,7 @@
         <v>658</v>
       </c>
       <c r="Q316" s="6">
-        <v>254.84</v>
+        <v>254.19</v>
       </c>
       <c r="R316" s="6" t="s">
         <v>23</v>
@@ -25955,7 +26045,7 @@
         <v>660</v>
       </c>
       <c r="Q317" s="6">
-        <v>8751.7000000000007</v>
+        <v>8737.5650000000005</v>
       </c>
       <c r="R317" s="6" t="s">
         <v>23</v>
@@ -26014,7 +26104,7 @@
         <v>662</v>
       </c>
       <c r="Q318" s="6">
-        <v>3587.9</v>
+        <v>3547.14</v>
       </c>
       <c r="R318" s="6" t="s">
         <v>23</v>
@@ -26073,7 +26163,7 @@
         <v>664</v>
       </c>
       <c r="Q319" s="6">
-        <v>7311.8</v>
+        <v>7132.64</v>
       </c>
       <c r="R319" s="6" t="s">
         <v>23</v>
@@ -26132,7 +26222,7 @@
         <v>666</v>
       </c>
       <c r="Q320" s="6">
-        <v>2950.22</v>
+        <v>2879.79</v>
       </c>
       <c r="R320" s="6" t="s">
         <v>23</v>
@@ -26191,7 +26281,7 @@
         <v>668</v>
       </c>
       <c r="Q321" s="6">
-        <v>5185.33</v>
+        <v>6430.21</v>
       </c>
       <c r="R321" s="6" t="s">
         <v>23</v>
@@ -26250,7 +26340,7 @@
         <v>670</v>
       </c>
       <c r="Q322" s="6">
-        <v>2426.4603999999999</v>
+        <v>2011.1004</v>
       </c>
       <c r="R322" s="6" t="s">
         <v>23</v>
@@ -26309,7 +26399,7 @@
         <v>672</v>
       </c>
       <c r="Q323" s="6">
-        <v>1247.9749999999999</v>
+        <v>1404.345</v>
       </c>
       <c r="R323" s="6" t="s">
         <v>23</v>
@@ -26368,7 +26458,7 @@
         <v>674</v>
       </c>
       <c r="Q324" s="6">
-        <v>2787.86</v>
+        <v>2708.52</v>
       </c>
       <c r="R324" s="6" t="s">
         <v>23</v>
@@ -26427,7 +26517,7 @@
         <v>676</v>
       </c>
       <c r="Q325" s="6">
-        <v>3894.5126</v>
+        <v>3878.4025999999999</v>
       </c>
       <c r="R325" s="6" t="s">
         <v>23</v>
@@ -26486,7 +26576,7 @@
         <v>678</v>
       </c>
       <c r="Q326" s="6">
-        <v>773.66</v>
+        <v>1880.9</v>
       </c>
       <c r="R326" s="6" t="s">
         <v>23</v>
@@ -26545,7 +26635,7 @@
         <v>680</v>
       </c>
       <c r="Q327" s="6">
-        <v>19.670000000000002</v>
+        <v>16.84</v>
       </c>
       <c r="R327" s="6" t="s">
         <v>23</v>
@@ -26604,7 +26694,7 @@
         <v>683</v>
       </c>
       <c r="Q328" s="6">
-        <v>3382.7809999999999</v>
+        <v>3359.681</v>
       </c>
       <c r="R328" s="6" t="s">
         <v>23</v>
@@ -26663,7 +26753,7 @@
         <v>686</v>
       </c>
       <c r="Q329" s="6">
-        <v>2061.86</v>
+        <v>2052.11</v>
       </c>
       <c r="R329" s="6" t="s">
         <v>23</v>
@@ -26722,7 +26812,7 @@
         <v>689</v>
       </c>
       <c r="Q330" s="6">
-        <v>279.20999999999998</v>
+        <v>716.53</v>
       </c>
       <c r="R330" s="6" t="s">
         <v>23</v>
@@ -26781,7 +26871,7 @@
         <v>692</v>
       </c>
       <c r="Q331" s="6">
-        <v>1179.03</v>
+        <v>1126.93</v>
       </c>
       <c r="R331" s="6" t="s">
         <v>23</v>
@@ -26840,7 +26930,7 @@
         <v>694</v>
       </c>
       <c r="Q332" s="6">
-        <v>3484.01</v>
+        <v>2995</v>
       </c>
       <c r="R332" s="6" t="s">
         <v>23</v>
@@ -26899,7 +26989,7 @@
         <v>697</v>
       </c>
       <c r="Q333" s="6">
-        <v>1974.93</v>
+        <v>1910.09</v>
       </c>
       <c r="R333" s="6" t="s">
         <v>23</v>
@@ -26958,7 +27048,7 @@
         <v>700</v>
       </c>
       <c r="Q334" s="6">
-        <v>125.74</v>
+        <v>106.54</v>
       </c>
       <c r="R334" s="6" t="s">
         <v>23</v>
@@ -27017,7 +27107,7 @@
         <v>703</v>
       </c>
       <c r="Q335" s="6">
-        <v>1363.0350000000001</v>
+        <v>1315.7950000000001</v>
       </c>
       <c r="R335" s="6" t="s">
         <v>23</v>
@@ -27076,7 +27166,7 @@
         <v>706</v>
       </c>
       <c r="Q336" s="6">
-        <v>2352.3000000000002</v>
+        <v>2300.25</v>
       </c>
       <c r="R336" s="6" t="s">
         <v>23</v>
@@ -27607,7 +27697,7 @@
         <v>724</v>
       </c>
       <c r="Q345" s="6">
-        <v>4611.96</v>
+        <v>1951.7</v>
       </c>
       <c r="R345" s="6" t="s">
         <v>23</v>
@@ -27666,7 +27756,7 @@
         <v>726</v>
       </c>
       <c r="Q346" s="6">
-        <v>895.88</v>
+        <v>197.22</v>
       </c>
       <c r="R346" s="6" t="s">
         <v>23</v>
@@ -27725,7 +27815,7 @@
         <v>728</v>
       </c>
       <c r="Q347" s="6">
-        <v>207.98</v>
+        <v>177.6</v>
       </c>
       <c r="R347" s="6" t="s">
         <v>23</v>
@@ -27784,7 +27874,7 @@
         <v>731</v>
       </c>
       <c r="Q348" s="6">
-        <v>412.14</v>
+        <v>401.49</v>
       </c>
       <c r="R348" s="6" t="s">
         <v>23</v>
@@ -27843,7 +27933,7 @@
         <v>734</v>
       </c>
       <c r="Q349" s="6">
-        <v>777.43</v>
+        <v>1245.28</v>
       </c>
       <c r="R349" s="6" t="s">
         <v>23</v>
@@ -27902,7 +27992,7 @@
         <v>736</v>
       </c>
       <c r="Q350" s="6">
-        <v>4957.9250000000002</v>
+        <v>4857.5550000000003</v>
       </c>
       <c r="R350" s="6" t="s">
         <v>23</v>
@@ -27961,7 +28051,7 @@
         <v>738</v>
       </c>
       <c r="Q351" s="6">
-        <v>29359.31</v>
+        <v>28336.23</v>
       </c>
       <c r="R351" s="6" t="s">
         <v>23</v>
@@ -28020,7 +28110,7 @@
         <v>741</v>
       </c>
       <c r="Q352" s="6">
-        <v>3549.65</v>
+        <v>3544.45</v>
       </c>
       <c r="R352" s="6" t="s">
         <v>23</v>
@@ -28138,7 +28228,7 @@
         <v>747</v>
       </c>
       <c r="Q354" s="6">
-        <v>232.7</v>
+        <v>169.83</v>
       </c>
       <c r="R354" s="6" t="s">
         <v>23</v>
@@ -28197,7 +28287,7 @@
         <v>749</v>
       </c>
       <c r="Q355" s="6">
-        <v>1533.11</v>
+        <v>1458.98</v>
       </c>
       <c r="R355" s="6" t="s">
         <v>23</v>
@@ -28433,7 +28523,7 @@
         <v>757</v>
       </c>
       <c r="Q359" s="6">
-        <v>965</v>
+        <v>921.47</v>
       </c>
       <c r="R359" s="6" t="s">
         <v>23</v>
@@ -28492,7 +28582,7 @@
         <v>759</v>
       </c>
       <c r="Q360" s="6">
-        <v>1579.3</v>
+        <v>1531.57</v>
       </c>
       <c r="R360" s="6" t="s">
         <v>23</v>
@@ -29023,7 +29113,7 @@
         <v>787</v>
       </c>
       <c r="Q369" s="6">
-        <v>60.9</v>
+        <v>57.15</v>
       </c>
       <c r="R369" s="6" t="s">
         <v>23</v>
@@ -29082,7 +29172,7 @@
         <v>791</v>
       </c>
       <c r="Q370" s="6">
-        <v>156.65</v>
+        <v>155.9</v>
       </c>
       <c r="R370" s="6" t="s">
         <v>23</v>
@@ -29141,7 +29231,7 @@
         <v>794</v>
       </c>
       <c r="Q371" s="6">
-        <v>3506.83</v>
+        <v>3525.83</v>
       </c>
       <c r="R371" s="6" t="s">
         <v>23</v>
@@ -35277,7 +35367,7 @@
         <v>1004</v>
       </c>
       <c r="Q475" s="6">
-        <v>344.21</v>
+        <v>208.84</v>
       </c>
       <c r="R475" s="6" t="s">
         <v>23</v>
@@ -35395,7 +35485,7 @@
         <v>1008</v>
       </c>
       <c r="Q477" s="6">
-        <v>290.27999999999997</v>
+        <v>289.45</v>
       </c>
       <c r="R477" s="6" t="s">
         <v>23</v>
@@ -35454,7 +35544,7 @@
         <v>1010</v>
       </c>
       <c r="Q478" s="6">
-        <v>1196.3</v>
+        <v>1193.33</v>
       </c>
       <c r="R478" s="6" t="s">
         <v>23</v>
@@ -51384,7 +51474,7 @@
         <v>1563</v>
       </c>
       <c r="Q748" s="6">
-        <v>500.14</v>
+        <v>444.22</v>
       </c>
       <c r="R748" s="6" t="s">
         <v>23</v>
@@ -53685,7 +53775,7 @@
         <v>1649</v>
       </c>
       <c r="Q787" s="6">
-        <v>3440.86</v>
+        <v>3125.09</v>
       </c>
       <c r="R787" s="6" t="s">
         <v>23</v>
@@ -53862,7 +53952,7 @@
         <v>1655</v>
       </c>
       <c r="Q790" s="6">
-        <v>9584.8406799999993</v>
+        <v>7418.4906799999999</v>
       </c>
       <c r="R790" s="6" t="s">
         <v>23</v>
@@ -53980,7 +54070,7 @@
         <v>1659</v>
       </c>
       <c r="Q792" s="6">
-        <v>2056.69</v>
+        <v>933.49</v>
       </c>
       <c r="R792" s="6" t="s">
         <v>23</v>
@@ -54098,7 +54188,7 @@
         <v>1663</v>
       </c>
       <c r="Q794" s="6">
-        <v>3421.5949999999998</v>
+        <v>2521.585</v>
       </c>
       <c r="R794" s="6" t="s">
         <v>23</v>
@@ -54157,7 +54247,7 @@
         <v>1665</v>
       </c>
       <c r="Q795" s="6">
-        <v>21018.51</v>
+        <v>18926.71</v>
       </c>
       <c r="R795" s="6" t="s">
         <v>23</v>
@@ -54452,7 +54542,7 @@
         <v>1675</v>
       </c>
       <c r="Q800" s="6">
-        <v>7845.46</v>
+        <v>6565.2</v>
       </c>
       <c r="R800" s="6" t="s">
         <v>23</v>
@@ -54570,7 +54660,7 @@
         <v>1679</v>
       </c>
       <c r="Q802" s="6">
-        <v>970.95</v>
+        <v>636.15</v>
       </c>
       <c r="R802" s="6" t="s">
         <v>23</v>
@@ -54629,7 +54719,7 @@
         <v>1681</v>
       </c>
       <c r="Q803" s="6">
-        <v>19500.651999999998</v>
+        <v>12206.531999999999</v>
       </c>
       <c r="R803" s="6" t="s">
         <v>23</v>
@@ -54688,7 +54778,7 @@
         <v>1684</v>
       </c>
       <c r="Q804" s="6">
-        <v>21706.080000000002</v>
+        <v>19351.34</v>
       </c>
       <c r="R804" s="6" t="s">
         <v>23</v>
@@ -54747,7 +54837,7 @@
         <v>1687</v>
       </c>
       <c r="Q805" s="6">
-        <v>41485.018300000003</v>
+        <v>33535.568299999999</v>
       </c>
       <c r="R805" s="6" t="s">
         <v>23</v>
@@ -54806,7 +54896,7 @@
         <v>1690</v>
       </c>
       <c r="Q806" s="6">
-        <v>1976.29</v>
+        <v>1289.9000000000001</v>
       </c>
       <c r="R806" s="6" t="s">
         <v>23</v>
@@ -55525,16 +55615,16 @@
     </row>
     <row r="819" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A819" s="5" t="s">
+        <v>2174</v>
+      </c>
+      <c r="B819" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C819" s="5" t="s">
         <v>2175</v>
       </c>
-      <c r="B819" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C819" s="5" t="s">
+      <c r="D819" s="5" t="s">
         <v>2176</v>
-      </c>
-      <c r="D819" s="5" t="s">
-        <v>2177</v>
       </c>
       <c r="E819" s="6" t="s">
         <v>23</v>
@@ -55570,7 +55660,7 @@
         <v>21</v>
       </c>
       <c r="P819" s="5" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="Q819" s="6">
         <v>0</v>
@@ -55584,16 +55674,16 @@
     </row>
     <row r="820" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A820" s="5" t="s">
+        <v>2177</v>
+      </c>
+      <c r="B820" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C820" s="5" t="s">
         <v>2178</v>
       </c>
-      <c r="B820" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C820" s="5" t="s">
+      <c r="D820" s="5" t="s">
         <v>2179</v>
-      </c>
-      <c r="D820" s="5" t="s">
-        <v>2180</v>
       </c>
       <c r="E820" s="6" t="s">
         <v>23</v>
@@ -55629,7 +55719,7 @@
         <v>21</v>
       </c>
       <c r="P820" s="5" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="Q820" s="6">
         <v>0</v>
@@ -55809,7 +55899,7 @@
         <v>1735</v>
       </c>
       <c r="Q823" s="6">
-        <v>3041.46</v>
+        <v>3073.08</v>
       </c>
       <c r="R823" s="6" t="s">
         <v>23</v>
@@ -56281,7 +56371,7 @@
         <v>1758</v>
       </c>
       <c r="Q831" s="6">
-        <v>9837.82</v>
+        <v>14383.02</v>
       </c>
       <c r="R831" s="6" t="s">
         <v>23</v>
@@ -56340,7 +56430,7 @@
         <v>1762</v>
       </c>
       <c r="Q832" s="6">
-        <v>7023.86</v>
+        <v>9814.9699999999993</v>
       </c>
       <c r="R832" s="6" t="s">
         <v>23</v>
@@ -56517,7 +56607,7 @@
         <v>1771</v>
       </c>
       <c r="Q835" s="6">
-        <v>331.07</v>
+        <v>2180.38</v>
       </c>
       <c r="R835" s="6" t="s">
         <v>23</v>
@@ -56635,7 +56725,7 @@
         <v>1777</v>
       </c>
       <c r="Q837" s="6">
-        <v>562.20000000000005</v>
+        <v>543.02</v>
       </c>
       <c r="R837" s="6" t="s">
         <v>23</v>
@@ -56812,7 +56902,7 @@
         <v>1790</v>
       </c>
       <c r="Q840" s="6">
-        <v>4694.0950000000003</v>
+        <v>4662.1149999999998</v>
       </c>
       <c r="R840" s="6" t="s">
         <v>23</v>
@@ -56871,7 +56961,7 @@
         <v>747</v>
       </c>
       <c r="Q841" s="6">
-        <v>721.73</v>
+        <v>663.49</v>
       </c>
       <c r="R841" s="6" t="s">
         <v>23</v>
@@ -56930,7 +57020,7 @@
         <v>1797</v>
       </c>
       <c r="Q842" s="6">
-        <v>139.44</v>
+        <v>117.21</v>
       </c>
       <c r="R842" s="6" t="s">
         <v>23</v>
@@ -56989,7 +57079,7 @@
         <v>1800</v>
       </c>
       <c r="Q843" s="6">
-        <v>382.66</v>
+        <v>278.67</v>
       </c>
       <c r="R843" s="6" t="s">
         <v>23</v>
@@ -57107,7 +57197,7 @@
         <v>1806</v>
       </c>
       <c r="Q845" s="6">
-        <v>311.12</v>
+        <v>308.62</v>
       </c>
       <c r="R845" s="6" t="s">
         <v>23</v>
@@ -57284,7 +57374,7 @@
         <v>1817</v>
       </c>
       <c r="Q848" s="6">
-        <v>199.09</v>
+        <v>161.55000000000001</v>
       </c>
       <c r="R848" s="6" t="s">
         <v>23</v>
@@ -57402,7 +57492,7 @@
         <v>1822</v>
       </c>
       <c r="Q850" s="6">
-        <v>-134.6</v>
+        <v>0</v>
       </c>
       <c r="R850" s="6" t="s">
         <v>23</v>
@@ -57682,7 +57772,7 @@
         <v>23</v>
       </c>
       <c r="L855" s="6">
-        <v>2.52</v>
+        <v>2.27</v>
       </c>
       <c r="M855" s="6">
         <v>0</v>
@@ -57697,7 +57787,7 @@
         <v>1837</v>
       </c>
       <c r="Q855" s="6">
-        <v>153.18</v>
+        <v>148.88999999999999</v>
       </c>
       <c r="R855" s="6" t="s">
         <v>23</v>
@@ -57756,7 +57846,7 @@
         <v>1840</v>
       </c>
       <c r="Q856" s="6">
-        <v>137.69999999999999</v>
+        <v>129.12</v>
       </c>
       <c r="R856" s="6" t="s">
         <v>23</v>
@@ -58051,7 +58141,7 @@
         <v>1855</v>
       </c>
       <c r="Q861" s="6">
-        <v>11819.3</v>
+        <v>11316.8</v>
       </c>
       <c r="R861" s="6" t="s">
         <v>23</v>
@@ -58346,7 +58436,7 @@
         <v>1871</v>
       </c>
       <c r="Q866" s="6">
-        <v>1839.5</v>
+        <v>1799.69</v>
       </c>
       <c r="R866" s="6" t="s">
         <v>23</v>
@@ -58508,7 +58598,7 @@
         <v>23</v>
       </c>
       <c r="L869" s="6">
-        <v>2.4</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="M869" s="6">
         <v>0</v>
@@ -58523,7 +58613,7 @@
         <v>1880</v>
       </c>
       <c r="Q869" s="6">
-        <v>0</v>
+        <v>175.9</v>
       </c>
       <c r="R869" s="6" t="s">
         <v>23</v>
@@ -58700,7 +58790,7 @@
         <v>1889</v>
       </c>
       <c r="Q872" s="6">
-        <v>255.85</v>
+        <v>185.69</v>
       </c>
       <c r="R872" s="6" t="s">
         <v>23</v>
@@ -58759,7 +58849,7 @@
         <v>1892</v>
       </c>
       <c r="Q873" s="6">
-        <v>298.22000000000003</v>
+        <v>276.83</v>
       </c>
       <c r="R873" s="6" t="s">
         <v>23</v>
@@ -58818,7 +58908,7 @@
         <v>1895</v>
       </c>
       <c r="Q874" s="6">
-        <v>676.72</v>
+        <v>664.17</v>
       </c>
       <c r="R874" s="6" t="s">
         <v>23</v>
@@ -59054,7 +59144,7 @@
         <v>1907</v>
       </c>
       <c r="Q878" s="6">
-        <v>152.32</v>
+        <v>207.82</v>
       </c>
       <c r="R878" s="6" t="s">
         <v>23</v>
@@ -59231,7 +59321,7 @@
         <v>1916</v>
       </c>
       <c r="Q881" s="6">
-        <v>326.54000000000002</v>
+        <v>325.13</v>
       </c>
       <c r="R881" s="6" t="s">
         <v>23</v>
@@ -59290,7 +59380,7 @@
         <v>1919</v>
       </c>
       <c r="Q882" s="6">
-        <v>496.7</v>
+        <v>379.61</v>
       </c>
       <c r="R882" s="6" t="s">
         <v>23</v>
@@ -59349,7 +59439,7 @@
         <v>1922</v>
       </c>
       <c r="Q883" s="6">
-        <v>20884.14</v>
+        <v>10940.86</v>
       </c>
       <c r="R883" s="6" t="s">
         <v>23</v>
@@ -59408,7 +59498,7 @@
         <v>1925</v>
       </c>
       <c r="Q884" s="6">
-        <v>3979</v>
+        <v>3848.9</v>
       </c>
       <c r="R884" s="6" t="s">
         <v>23</v>
@@ -59585,7 +59675,7 @@
         <v>1935</v>
       </c>
       <c r="Q887" s="6">
-        <v>120.53</v>
+        <v>88.46</v>
       </c>
       <c r="R887" s="6" t="s">
         <v>23</v>
@@ -59644,7 +59734,7 @@
         <v>1938</v>
       </c>
       <c r="Q888" s="6">
-        <v>160.06</v>
+        <v>138.63999999999999</v>
       </c>
       <c r="R888" s="6" t="s">
         <v>23</v>
@@ -59703,7 +59793,7 @@
         <v>1941</v>
       </c>
       <c r="Q889" s="6">
-        <v>124.87</v>
+        <v>114.19</v>
       </c>
       <c r="R889" s="6" t="s">
         <v>23</v>
@@ -59762,7 +59852,7 @@
         <v>1944</v>
       </c>
       <c r="Q890" s="6">
-        <v>444.53500000000003</v>
+        <v>246.05500000000001</v>
       </c>
       <c r="R890" s="6" t="s">
         <v>23</v>
@@ -61576,7 +61666,7 @@
         <v>23</v>
       </c>
       <c r="L921" s="6">
-        <v>1.8</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="M921" s="6">
         <v>0</v>
@@ -61591,7 +61681,7 @@
         <v>2038</v>
       </c>
       <c r="Q921" s="6">
-        <v>1465.78</v>
+        <v>2256.6799999999998</v>
       </c>
       <c r="R921" s="6" t="s">
         <v>23</v>
@@ -61650,7 +61740,7 @@
         <v>2041</v>
       </c>
       <c r="Q922" s="6">
-        <v>6958.81</v>
+        <v>14639.15</v>
       </c>
       <c r="R922" s="6" t="s">
         <v>23</v>
@@ -61768,7 +61858,7 @@
         <v>2047</v>
       </c>
       <c r="Q924" s="6">
-        <v>6921.4629999999997</v>
+        <v>6058.6030000000001</v>
       </c>
       <c r="R924" s="6" t="s">
         <v>23</v>
@@ -62063,7 +62153,7 @@
         <v>2062</v>
       </c>
       <c r="Q929" s="6">
-        <v>84.63</v>
+        <v>540.07000000000005</v>
       </c>
       <c r="R929" s="6" t="s">
         <v>23</v>
@@ -62122,7 +62212,7 @@
         <v>2065</v>
       </c>
       <c r="Q930" s="6">
-        <v>491.11</v>
+        <v>2303.9899999999998</v>
       </c>
       <c r="R930" s="6" t="s">
         <v>23</v>
@@ -62240,7 +62330,7 @@
         <v>2071</v>
       </c>
       <c r="Q932" s="6">
-        <v>3245.18</v>
+        <v>2924.78</v>
       </c>
       <c r="R932" s="6" t="s">
         <v>23</v>
@@ -62417,7 +62507,7 @@
         <v>2080</v>
       </c>
       <c r="Q935" s="6">
-        <v>1635.98</v>
+        <v>1088.8</v>
       </c>
       <c r="R935" s="6" t="s">
         <v>23</v>
@@ -62653,7 +62743,7 @@
         <v>2092</v>
       </c>
       <c r="Q939" s="6">
-        <v>4091.1</v>
+        <v>3749.72</v>
       </c>
       <c r="R939" s="6" t="s">
         <v>23</v>
@@ -62712,7 +62802,7 @@
         <v>2095</v>
       </c>
       <c r="Q940" s="6">
-        <v>699.59</v>
+        <v>1734.42</v>
       </c>
       <c r="R940" s="6" t="s">
         <v>23</v>
@@ -62771,7 +62861,7 @@
         <v>2098</v>
       </c>
       <c r="Q941" s="6">
-        <v>343.91</v>
+        <v>220.05</v>
       </c>
       <c r="R941" s="6" t="s">
         <v>23</v>
@@ -62830,7 +62920,7 @@
         <v>2101</v>
       </c>
       <c r="Q942" s="6">
-        <v>771.35500000000002</v>
+        <v>670.755</v>
       </c>
       <c r="R942" s="6" t="s">
         <v>23</v>
@@ -62889,7 +62979,7 @@
         <v>2104</v>
       </c>
       <c r="Q943" s="6">
-        <v>1572.17</v>
+        <v>1507.77</v>
       </c>
       <c r="R943" s="6" t="s">
         <v>23</v>
@@ -62948,7 +63038,7 @@
         <v>2107</v>
       </c>
       <c r="Q944" s="6">
-        <v>2684.32</v>
+        <v>2491.12</v>
       </c>
       <c r="R944" s="6" t="s">
         <v>23</v>
@@ -63007,7 +63097,7 @@
         <v>2110</v>
       </c>
       <c r="Q945" s="6">
-        <v>1108.2</v>
+        <v>1043.8</v>
       </c>
       <c r="R945" s="6" t="s">
         <v>23</v>
@@ -63184,7 +63274,7 @@
         <v>2119</v>
       </c>
       <c r="Q948" s="6">
-        <v>2183.9</v>
+        <v>4137.7</v>
       </c>
       <c r="R948" s="6" t="s">
         <v>23</v>
@@ -63243,7 +63333,7 @@
         <v>2122</v>
       </c>
       <c r="Q949" s="6">
-        <v>207.57</v>
+        <v>106.97</v>
       </c>
       <c r="R949" s="6" t="s">
         <v>23</v>
@@ -63302,7 +63392,7 @@
         <v>2125</v>
       </c>
       <c r="Q950" s="6">
-        <v>895.505</v>
+        <v>392.505</v>
       </c>
       <c r="R950" s="6" t="s">
         <v>23</v>
@@ -63361,7 +63451,7 @@
         <v>2128</v>
       </c>
       <c r="Q951" s="6">
-        <v>401.2</v>
+        <v>98.991299999999995</v>
       </c>
       <c r="R951" s="6" t="s">
         <v>23</v>
@@ -63420,7 +63510,7 @@
         <v>2131</v>
       </c>
       <c r="Q952" s="6">
-        <v>251.74</v>
+        <v>201.44</v>
       </c>
       <c r="R952" s="6" t="s">
         <v>23</v>
@@ -63538,7 +63628,7 @@
         <v>2137</v>
       </c>
       <c r="Q954" s="6">
-        <v>201.1</v>
+        <v>100.5</v>
       </c>
       <c r="R954" s="6" t="s">
         <v>23</v>
@@ -63597,7 +63687,7 @@
         <v>2140</v>
       </c>
       <c r="Q955" s="6">
-        <v>191.4</v>
+        <v>141.1</v>
       </c>
       <c r="R955" s="6" t="s">
         <v>23</v>
@@ -63735,7 +63825,7 @@
         <v>2149</v>
       </c>
       <c r="D958" s="5" t="s">
-        <v>2150</v>
+        <v>2272</v>
       </c>
       <c r="E958" s="6" t="s">
         <v>23</v>
@@ -63774,7 +63864,7 @@
         <v>2149</v>
       </c>
       <c r="Q958" s="6">
-        <v>5698.4903999999997</v>
+        <v>3748.5803999999998</v>
       </c>
       <c r="R958" s="6" t="s">
         <v>23</v>
@@ -63785,16 +63875,16 @@
     </row>
     <row r="959" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A959" s="5" t="s">
+        <v>2150</v>
+      </c>
+      <c r="B959" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C959" s="5" t="s">
         <v>2151</v>
       </c>
-      <c r="B959" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C959" s="5" t="s">
+      <c r="D959" s="5" t="s">
         <v>2152</v>
-      </c>
-      <c r="D959" s="5" t="s">
-        <v>2153</v>
       </c>
       <c r="E959" s="6" t="s">
         <v>23</v>
@@ -63830,10 +63920,10 @@
         <v>21</v>
       </c>
       <c r="P959" s="5" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="Q959" s="6">
-        <v>1473.2</v>
+        <v>3535.2</v>
       </c>
       <c r="R959" s="6" t="s">
         <v>23</v>
@@ -63844,16 +63934,16 @@
     </row>
     <row r="960" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A960" s="5" t="s">
+        <v>2153</v>
+      </c>
+      <c r="B960" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C960" s="5" t="s">
         <v>2154</v>
       </c>
-      <c r="B960" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C960" s="5" t="s">
+      <c r="D960" s="5" t="s">
         <v>2155</v>
-      </c>
-      <c r="D960" s="5" t="s">
-        <v>2156</v>
       </c>
       <c r="E960" s="6" t="s">
         <v>23</v>
@@ -63889,10 +63979,10 @@
         <v>21</v>
       </c>
       <c r="P960" s="5" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="Q960" s="6">
-        <v>458.3</v>
+        <v>703.9</v>
       </c>
       <c r="R960" s="6" t="s">
         <v>23</v>
@@ -63903,16 +63993,16 @@
     </row>
     <row r="961" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A961" s="5" t="s">
+        <v>2156</v>
+      </c>
+      <c r="B961" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C961" s="5" t="s">
         <v>2157</v>
       </c>
-      <c r="B961" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C961" s="5" t="s">
+      <c r="D961" s="5" t="s">
         <v>2158</v>
-      </c>
-      <c r="D961" s="5" t="s">
-        <v>2159</v>
       </c>
       <c r="E961" s="6" t="s">
         <v>23</v>
@@ -63948,10 +64038,10 @@
         <v>21</v>
       </c>
       <c r="P961" s="5" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="Q961" s="6">
-        <v>314.05</v>
+        <v>3710.45</v>
       </c>
       <c r="R961" s="6" t="s">
         <v>23</v>
@@ -63962,16 +64052,16 @@
     </row>
     <row r="962" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A962" s="5" t="s">
+        <v>2159</v>
+      </c>
+      <c r="B962" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C962" s="5" t="s">
         <v>2160</v>
       </c>
-      <c r="B962" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C962" s="5" t="s">
+      <c r="D962" s="5" t="s">
         <v>2161</v>
-      </c>
-      <c r="D962" s="5" t="s">
-        <v>2162</v>
       </c>
       <c r="E962" s="6" t="s">
         <v>23</v>
@@ -64007,7 +64097,7 @@
         <v>21</v>
       </c>
       <c r="P962" s="5" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="Q962" s="6">
         <v>0</v>
@@ -64021,16 +64111,16 @@
     </row>
     <row r="963" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A963" s="5" t="s">
+        <v>2162</v>
+      </c>
+      <c r="B963" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C963" s="5" t="s">
         <v>2163</v>
       </c>
-      <c r="B963" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C963" s="5" t="s">
+      <c r="D963" s="5" t="s">
         <v>2164</v>
-      </c>
-      <c r="D963" s="5" t="s">
-        <v>2165</v>
       </c>
       <c r="E963" s="6" t="s">
         <v>23</v>
@@ -64066,7 +64156,7 @@
         <v>21</v>
       </c>
       <c r="P963" s="5" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="Q963" s="6">
         <v>0</v>
@@ -64080,16 +64170,16 @@
     </row>
     <row r="964" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A964" s="5" t="s">
+        <v>2180</v>
+      </c>
+      <c r="B964" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C964" s="5" t="s">
         <v>2181</v>
       </c>
-      <c r="B964" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C964" s="5" t="s">
+      <c r="D964" s="5" t="s">
         <v>2182</v>
-      </c>
-      <c r="D964" s="5" t="s">
-        <v>2183</v>
       </c>
       <c r="E964" s="6" t="s">
         <v>23</v>
@@ -64125,7 +64215,7 @@
         <v>21</v>
       </c>
       <c r="P964" s="5" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="Q964" s="6">
         <v>0</v>
@@ -64139,16 +64229,16 @@
     </row>
     <row r="965" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A965" s="5" t="s">
+        <v>2183</v>
+      </c>
+      <c r="B965" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C965" s="5" t="s">
         <v>2184</v>
       </c>
-      <c r="B965" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C965" s="5" t="s">
+      <c r="D965" s="5" t="s">
         <v>2185</v>
-      </c>
-      <c r="D965" s="5" t="s">
-        <v>2186</v>
       </c>
       <c r="E965" s="6" t="s">
         <v>23</v>
@@ -64184,7 +64274,7 @@
         <v>21</v>
       </c>
       <c r="P965" s="5" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="Q965" s="6">
         <v>0</v>
@@ -64198,16 +64288,16 @@
     </row>
     <row r="966" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A966" s="5" t="s">
+        <v>2186</v>
+      </c>
+      <c r="B966" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C966" s="5" t="s">
         <v>2187</v>
       </c>
-      <c r="B966" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C966" s="5" t="s">
+      <c r="D966" s="5" t="s">
         <v>2188</v>
-      </c>
-      <c r="D966" s="5" t="s">
-        <v>2189</v>
       </c>
       <c r="E966" s="6" t="s">
         <v>23</v>
@@ -64243,7 +64333,7 @@
         <v>21</v>
       </c>
       <c r="P966" s="5" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="Q966" s="6">
         <v>0</v>
@@ -64257,16 +64347,16 @@
     </row>
     <row r="967" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A967" s="5" t="s">
+        <v>2195</v>
+      </c>
+      <c r="B967" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C967" s="5" t="s">
         <v>2196</v>
       </c>
-      <c r="B967" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C967" s="5" t="s">
-        <v>2197</v>
-      </c>
       <c r="D967" s="5" t="s">
-        <v>2228</v>
+        <v>2273</v>
       </c>
       <c r="E967" s="6" t="s">
         <v>23</v>
@@ -64302,7 +64392,7 @@
         <v>21</v>
       </c>
       <c r="P967" s="5" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="Q967" s="6">
         <v>0</v>
@@ -64316,16 +64406,16 @@
     </row>
     <row r="968" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A968" s="5" t="s">
+        <v>2197</v>
+      </c>
+      <c r="B968" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C968" s="5" t="s">
         <v>2198</v>
       </c>
-      <c r="B968" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C968" s="5" t="s">
+      <c r="D968" s="5" t="s">
         <v>2199</v>
-      </c>
-      <c r="D968" s="5" t="s">
-        <v>2200</v>
       </c>
       <c r="E968" s="6" t="s">
         <v>23</v>
@@ -64361,7 +64451,7 @@
         <v>21</v>
       </c>
       <c r="P968" s="5" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="Q968" s="6">
         <v>0</v>
@@ -64375,16 +64465,16 @@
     </row>
     <row r="969" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A969" s="5" t="s">
+        <v>2200</v>
+      </c>
+      <c r="B969" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C969" s="5" t="s">
         <v>2201</v>
       </c>
-      <c r="B969" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C969" s="5" t="s">
+      <c r="D969" s="5" t="s">
         <v>2202</v>
-      </c>
-      <c r="D969" s="5" t="s">
-        <v>2203</v>
       </c>
       <c r="E969" s="6" t="s">
         <v>23</v>
@@ -64420,7 +64510,7 @@
         <v>21</v>
       </c>
       <c r="P969" s="5" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="Q969" s="6">
         <v>0</v>
@@ -64434,16 +64524,16 @@
     </row>
     <row r="970" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A970" s="5" t="s">
+        <v>2203</v>
+      </c>
+      <c r="B970" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C970" s="5" t="s">
         <v>2204</v>
       </c>
-      <c r="B970" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C970" s="5" t="s">
+      <c r="D970" s="5" t="s">
         <v>2205</v>
-      </c>
-      <c r="D970" s="5" t="s">
-        <v>2206</v>
       </c>
       <c r="E970" s="6" t="s">
         <v>23</v>
@@ -64479,7 +64569,7 @@
         <v>21</v>
       </c>
       <c r="P970" s="5" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="Q970" s="6">
         <v>0</v>
@@ -64493,16 +64583,16 @@
     </row>
     <row r="971" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A971" s="5" t="s">
+        <v>2206</v>
+      </c>
+      <c r="B971" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C971" s="5" t="s">
         <v>2207</v>
       </c>
-      <c r="B971" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C971" s="5" t="s">
+      <c r="D971" s="5" t="s">
         <v>2208</v>
-      </c>
-      <c r="D971" s="5" t="s">
-        <v>2209</v>
       </c>
       <c r="E971" s="6" t="s">
         <v>23</v>
@@ -64538,7 +64628,7 @@
         <v>21</v>
       </c>
       <c r="P971" s="5" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="Q971" s="6">
         <v>0</v>
@@ -64552,16 +64642,16 @@
     </row>
     <row r="972" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A972" s="5" t="s">
+        <v>2209</v>
+      </c>
+      <c r="B972" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C972" s="5" t="s">
         <v>2210</v>
       </c>
-      <c r="B972" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C972" s="5" t="s">
+      <c r="D972" s="5" t="s">
         <v>2211</v>
-      </c>
-      <c r="D972" s="5" t="s">
-        <v>2212</v>
       </c>
       <c r="E972" s="6" t="s">
         <v>23</v>
@@ -64597,7 +64687,7 @@
         <v>21</v>
       </c>
       <c r="P972" s="5" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="Q972" s="6">
         <v>0</v>
@@ -64611,16 +64701,16 @@
     </row>
     <row r="973" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A973" s="5" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B973" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C973" s="5" t="s">
         <v>2213</v>
       </c>
-      <c r="B973" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C973" s="5" t="s">
+      <c r="D973" s="5" t="s">
         <v>2214</v>
-      </c>
-      <c r="D973" s="5" t="s">
-        <v>2215</v>
       </c>
       <c r="E973" s="6" t="s">
         <v>23</v>
@@ -64656,7 +64746,7 @@
         <v>21</v>
       </c>
       <c r="P973" s="5" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="Q973" s="6">
         <v>0</v>
@@ -64670,16 +64760,16 @@
     </row>
     <row r="974" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A974" s="5" t="s">
+        <v>2215</v>
+      </c>
+      <c r="B974" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C974" s="5" t="s">
         <v>2216</v>
       </c>
-      <c r="B974" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C974" s="5" t="s">
+      <c r="D974" s="5" t="s">
         <v>2217</v>
-      </c>
-      <c r="D974" s="5" t="s">
-        <v>2218</v>
       </c>
       <c r="E974" s="6" t="s">
         <v>23</v>
@@ -64715,7 +64805,7 @@
         <v>21</v>
       </c>
       <c r="P974" s="5" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="Q974" s="6">
         <v>0</v>
@@ -64729,16 +64819,16 @@
     </row>
     <row r="975" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A975" s="5" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B975" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C975" s="5" t="s">
         <v>2219</v>
       </c>
-      <c r="B975" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C975" s="5" t="s">
+      <c r="D975" s="5" t="s">
         <v>2220</v>
-      </c>
-      <c r="D975" s="5" t="s">
-        <v>2221</v>
       </c>
       <c r="E975" s="6" t="s">
         <v>23</v>
@@ -64774,7 +64864,7 @@
         <v>21</v>
       </c>
       <c r="P975" s="5" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="Q975" s="6">
         <v>0</v>
@@ -64788,16 +64878,16 @@
     </row>
     <row r="976" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A976" s="5" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B976" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C976" s="5" t="s">
         <v>2222</v>
       </c>
-      <c r="B976" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C976" s="5" t="s">
+      <c r="D976" s="5" t="s">
         <v>2223</v>
-      </c>
-      <c r="D976" s="5" t="s">
-        <v>2224</v>
       </c>
       <c r="E976" s="6" t="s">
         <v>23</v>
@@ -64833,7 +64923,7 @@
         <v>21</v>
       </c>
       <c r="P976" s="5" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="Q976" s="6">
         <v>0</v>
@@ -64847,16 +64937,16 @@
     </row>
     <row r="977" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A977" s="5" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B977" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C977" s="5" t="s">
         <v>2225</v>
       </c>
-      <c r="B977" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C977" s="5" t="s">
+      <c r="D977" s="5" t="s">
         <v>2226</v>
-      </c>
-      <c r="D977" s="5" t="s">
-        <v>2227</v>
       </c>
       <c r="E977" s="6" t="s">
         <v>23</v>
@@ -64892,7 +64982,7 @@
         <v>21</v>
       </c>
       <c r="P977" s="5" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="Q977" s="6">
         <v>0</v>
@@ -64906,16 +64996,16 @@
     </row>
     <row r="978" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A978" s="5" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
       <c r="B978" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C978" s="5" t="s">
-        <v>2230</v>
+        <v>2228</v>
       </c>
       <c r="D978" s="5" t="s">
-        <v>2231</v>
+        <v>2274</v>
       </c>
       <c r="E978" s="6" t="s">
         <v>23</v>
@@ -64951,10 +65041,10 @@
         <v>21</v>
       </c>
       <c r="P978" s="5" t="s">
-        <v>2230</v>
+        <v>2228</v>
       </c>
       <c r="Q978" s="6">
-        <v>541.6</v>
+        <v>583.1</v>
       </c>
       <c r="R978" s="6" t="s">
         <v>23</v>
@@ -64965,16 +65055,16 @@
     </row>
     <row r="979" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A979" s="5" t="s">
-        <v>2232</v>
+        <v>2229</v>
       </c>
       <c r="B979" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C979" s="5" t="s">
-        <v>2233</v>
+        <v>2230</v>
       </c>
       <c r="D979" s="5" t="s">
-        <v>2234</v>
+        <v>2231</v>
       </c>
       <c r="E979" s="6" t="s">
         <v>23</v>
@@ -65010,7 +65100,7 @@
         <v>21</v>
       </c>
       <c r="P979" s="5" t="s">
-        <v>2233</v>
+        <v>2230</v>
       </c>
       <c r="Q979" s="6">
         <v>2054.8000000000002</v>
@@ -65024,16 +65114,16 @@
     </row>
     <row r="980" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A980" s="5" t="s">
-        <v>2235</v>
+        <v>2232</v>
       </c>
       <c r="B980" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C980" s="5" t="s">
-        <v>2236</v>
+        <v>2233</v>
       </c>
       <c r="D980" s="5" t="s">
-        <v>2237</v>
+        <v>2234</v>
       </c>
       <c r="E980" s="6" t="s">
         <v>23</v>
@@ -65069,7 +65159,7 @@
         <v>21</v>
       </c>
       <c r="P980" s="5" t="s">
-        <v>2236</v>
+        <v>2233</v>
       </c>
       <c r="Q980" s="6">
         <v>0</v>
@@ -65083,16 +65173,16 @@
     </row>
     <row r="981" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A981" s="5" t="s">
-        <v>2238</v>
+        <v>2235</v>
       </c>
       <c r="B981" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C981" s="5" t="s">
-        <v>2239</v>
+        <v>2236</v>
       </c>
       <c r="D981" s="5" t="s">
-        <v>2240</v>
+        <v>2237</v>
       </c>
       <c r="E981" s="6" t="s">
         <v>23</v>
@@ -65128,7 +65218,7 @@
         <v>21</v>
       </c>
       <c r="P981" s="5" t="s">
-        <v>2239</v>
+        <v>2236</v>
       </c>
       <c r="Q981" s="6">
         <v>0</v>
@@ -65142,16 +65232,16 @@
     </row>
     <row r="982" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A982" s="5" t="s">
-        <v>2241</v>
+        <v>2238</v>
       </c>
       <c r="B982" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C982" s="5" t="s">
-        <v>2242</v>
+        <v>2239</v>
       </c>
       <c r="D982" s="5" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="E982" s="6" t="s">
         <v>23</v>
@@ -65187,7 +65277,7 @@
         <v>21</v>
       </c>
       <c r="P982" s="5" t="s">
-        <v>2242</v>
+        <v>2239</v>
       </c>
       <c r="Q982" s="6">
         <v>0</v>
@@ -65201,16 +65291,16 @@
     </row>
     <row r="983" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A983" s="5" t="s">
-        <v>2244</v>
+        <v>2241</v>
       </c>
       <c r="B983" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C983" s="5" t="s">
-        <v>2245</v>
+        <v>2242</v>
       </c>
       <c r="D983" s="5" t="s">
-        <v>2246</v>
+        <v>2243</v>
       </c>
       <c r="E983" s="6" t="s">
         <v>23</v>
@@ -65246,7 +65336,7 @@
         <v>21</v>
       </c>
       <c r="P983" s="5" t="s">
-        <v>2245</v>
+        <v>2242</v>
       </c>
       <c r="Q983" s="6">
         <v>0</v>
@@ -65260,16 +65350,16 @@
     </row>
     <row r="984" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A984" s="5" t="s">
-        <v>2247</v>
+        <v>2244</v>
       </c>
       <c r="B984" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C984" s="5" t="s">
-        <v>2248</v>
+        <v>2245</v>
       </c>
       <c r="D984" s="5" t="s">
-        <v>2249</v>
+        <v>2246</v>
       </c>
       <c r="E984" s="6" t="s">
         <v>23</v>
@@ -65305,7 +65395,7 @@
         <v>21</v>
       </c>
       <c r="P984" s="5" t="s">
-        <v>2248</v>
+        <v>2245</v>
       </c>
       <c r="Q984" s="6">
         <v>0</v>
@@ -65319,16 +65409,16 @@
     </row>
     <row r="985" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A985" s="5" t="s">
-        <v>2250</v>
+        <v>2247</v>
       </c>
       <c r="B985" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C985" s="5" t="s">
-        <v>2251</v>
+        <v>2248</v>
       </c>
       <c r="D985" s="5" t="s">
-        <v>2252</v>
+        <v>2249</v>
       </c>
       <c r="E985" s="6" t="s">
         <v>23</v>
@@ -65364,7 +65454,7 @@
         <v>21</v>
       </c>
       <c r="P985" s="5" t="s">
-        <v>2251</v>
+        <v>2248</v>
       </c>
       <c r="Q985" s="6">
         <v>0</v>
@@ -65378,16 +65468,16 @@
     </row>
     <row r="986" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A986" s="5" t="s">
-        <v>2253</v>
+        <v>2250</v>
       </c>
       <c r="B986" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C986" s="5" t="s">
-        <v>2254</v>
+        <v>2251</v>
       </c>
       <c r="D986" s="5" t="s">
-        <v>2255</v>
+        <v>2252</v>
       </c>
       <c r="E986" s="6" t="s">
         <v>23</v>
@@ -65408,7 +65498,7 @@
         <v>21</v>
       </c>
       <c r="K986" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L986" s="6">
         <v>0</v>
@@ -65423,10 +65513,10 @@
         <v>21</v>
       </c>
       <c r="P986" s="5" t="s">
-        <v>2254</v>
+        <v>2251</v>
       </c>
       <c r="Q986" s="6">
-        <v>0</v>
+        <v>505.8</v>
       </c>
       <c r="R986" s="6" t="s">
         <v>23</v>
@@ -65437,16 +65527,16 @@
     </row>
     <row r="987" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A987" s="5" t="s">
-        <v>2256</v>
+        <v>2253</v>
       </c>
       <c r="B987" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C987" s="5" t="s">
-        <v>2257</v>
+        <v>2254</v>
       </c>
       <c r="D987" s="5" t="s">
-        <v>2258</v>
+        <v>2255</v>
       </c>
       <c r="E987" s="6" t="s">
         <v>23</v>
@@ -65467,10 +65557,10 @@
         <v>21</v>
       </c>
       <c r="K987" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L987" s="6">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M987" s="6">
         <v>0</v>
@@ -65482,10 +65572,10 @@
         <v>21</v>
       </c>
       <c r="P987" s="5" t="s">
-        <v>2257</v>
+        <v>2254</v>
       </c>
       <c r="Q987" s="6">
-        <v>0</v>
+        <v>43.19</v>
       </c>
       <c r="R987" s="6" t="s">
         <v>23</v>
@@ -65496,16 +65586,16 @@
     </row>
     <row r="988" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A988" s="5" t="s">
-        <v>2259</v>
+        <v>2256</v>
       </c>
       <c r="B988" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C988" s="5" t="s">
-        <v>2260</v>
+        <v>2257</v>
       </c>
       <c r="D988" s="5" t="s">
-        <v>2261</v>
+        <v>2258</v>
       </c>
       <c r="E988" s="6" t="s">
         <v>23</v>
@@ -65541,7 +65631,7 @@
         <v>21</v>
       </c>
       <c r="P988" s="5" t="s">
-        <v>2260</v>
+        <v>2257</v>
       </c>
       <c r="Q988" s="6">
         <v>0</v>
@@ -65555,16 +65645,16 @@
     </row>
     <row r="989" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A989" s="5" t="s">
-        <v>2262</v>
+        <v>2259</v>
       </c>
       <c r="B989" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C989" s="5" t="s">
-        <v>2263</v>
+        <v>2260</v>
       </c>
       <c r="D989" s="5" t="s">
-        <v>2264</v>
+        <v>2261</v>
       </c>
       <c r="E989" s="6" t="s">
         <v>23</v>
@@ -65600,7 +65690,7 @@
         <v>21</v>
       </c>
       <c r="P989" s="5" t="s">
-        <v>2263</v>
+        <v>2260</v>
       </c>
       <c r="Q989" s="6">
         <v>0</v>
@@ -65614,16 +65704,16 @@
     </row>
     <row r="990" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A990" s="5" t="s">
-        <v>2266</v>
+        <v>2262</v>
       </c>
       <c r="B990" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C990" s="5" t="s">
-        <v>2267</v>
+        <v>2263</v>
       </c>
       <c r="D990" s="5" t="s">
-        <v>2268</v>
+        <v>2264</v>
       </c>
       <c r="E990" s="6" t="s">
         <v>23</v>
@@ -65659,7 +65749,7 @@
         <v>21</v>
       </c>
       <c r="P990" s="5" t="s">
-        <v>2267</v>
+        <v>2263</v>
       </c>
       <c r="Q990" s="6">
         <v>0</v>
@@ -65673,16 +65763,16 @@
     </row>
     <row r="991" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A991" s="5" t="s">
-        <v>2269</v>
+        <v>2265</v>
       </c>
       <c r="B991" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C991" s="5" t="s">
-        <v>2270</v>
+        <v>2266</v>
       </c>
       <c r="D991" s="5" t="s">
-        <v>2271</v>
+        <v>2267</v>
       </c>
       <c r="E991" s="6" t="s">
         <v>23</v>
@@ -65718,7 +65808,7 @@
         <v>21</v>
       </c>
       <c r="P991" s="5" t="s">
-        <v>2270</v>
+        <v>2266</v>
       </c>
       <c r="Q991" s="6">
         <v>0</v>
@@ -65732,16 +65822,16 @@
     </row>
     <row r="992" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A992" s="5" t="s">
-        <v>2272</v>
+        <v>2268</v>
       </c>
       <c r="B992" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C992" s="5" t="s">
-        <v>2273</v>
+        <v>2269</v>
       </c>
       <c r="D992" s="5" t="s">
-        <v>2274</v>
+        <v>2270</v>
       </c>
       <c r="E992" s="6" t="s">
         <v>23</v>
@@ -65762,7 +65852,7 @@
         <v>21</v>
       </c>
       <c r="K992" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L992" s="6">
         <v>0</v>
@@ -65777,10 +65867,10 @@
         <v>21</v>
       </c>
       <c r="P992" s="5" t="s">
-        <v>2273</v>
+        <v>2269</v>
       </c>
       <c r="Q992" s="6">
-        <v>0</v>
+        <v>133.80000000000001</v>
       </c>
       <c r="R992" s="6" t="s">
         <v>23</v>
@@ -65791,16 +65881,16 @@
     </row>
     <row r="993" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A993" s="5" t="s">
-        <v>2166</v>
+        <v>2275</v>
       </c>
       <c r="B993" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C993" s="5" t="s">
-        <v>2167</v>
+        <v>2276</v>
       </c>
       <c r="D993" s="5" t="s">
-        <v>2168</v>
+        <v>2277</v>
       </c>
       <c r="E993" s="6" t="s">
         <v>23</v>
@@ -65821,10 +65911,10 @@
         <v>21</v>
       </c>
       <c r="K993" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L993" s="6">
-        <v>1.98</v>
+        <v>0</v>
       </c>
       <c r="M993" s="6">
         <v>0</v>
@@ -65836,10 +65926,10 @@
         <v>21</v>
       </c>
       <c r="P993" s="5" t="s">
-        <v>2167</v>
+        <v>2276</v>
       </c>
       <c r="Q993" s="6">
-        <v>589.70000000000005</v>
+        <v>0</v>
       </c>
       <c r="R993" s="6" t="s">
         <v>23</v>
@@ -65850,16 +65940,16 @@
     </row>
     <row r="994" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A994" s="5" t="s">
-        <v>2169</v>
+        <v>2278</v>
       </c>
       <c r="B994" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C994" s="5" t="s">
-        <v>2170</v>
+        <v>2279</v>
       </c>
       <c r="D994" s="5" t="s">
-        <v>2171</v>
+        <v>2280</v>
       </c>
       <c r="E994" s="6" t="s">
         <v>23</v>
@@ -65880,10 +65970,10 @@
         <v>21</v>
       </c>
       <c r="K994" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L994" s="6">
-        <v>3.75</v>
+        <v>0</v>
       </c>
       <c r="M994" s="6">
         <v>0</v>
@@ -65895,10 +65985,10 @@
         <v>21</v>
       </c>
       <c r="P994" s="5" t="s">
-        <v>2170</v>
+        <v>2279</v>
       </c>
       <c r="Q994" s="6">
-        <v>200.73</v>
+        <v>0</v>
       </c>
       <c r="R994" s="6" t="s">
         <v>23</v>
@@ -65909,16 +65999,16 @@
     </row>
     <row r="995" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A995" s="5" t="s">
-        <v>2172</v>
+        <v>2281</v>
       </c>
       <c r="B995" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C995" s="5" t="s">
-        <v>2173</v>
+        <v>2282</v>
       </c>
       <c r="D995" s="5" t="s">
-        <v>2174</v>
+        <v>2283</v>
       </c>
       <c r="E995" s="6" t="s">
         <v>23</v>
@@ -65942,7 +66032,7 @@
         <v>23</v>
       </c>
       <c r="L995" s="6">
-        <v>2.65</v>
+        <v>1.61</v>
       </c>
       <c r="M995" s="6">
         <v>0</v>
@@ -65954,10 +66044,10 @@
         <v>21</v>
       </c>
       <c r="P995" s="5" t="s">
-        <v>2173</v>
+        <v>2282</v>
       </c>
       <c r="Q995" s="6">
-        <v>1479.87</v>
+        <v>2257</v>
       </c>
       <c r="R995" s="6" t="s">
         <v>23</v>
@@ -65968,16 +66058,16 @@
     </row>
     <row r="996" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A996" s="5" t="s">
-        <v>2190</v>
+        <v>2284</v>
       </c>
       <c r="B996" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C996" s="5" t="s">
-        <v>2191</v>
+        <v>2285</v>
       </c>
       <c r="D996" s="5" t="s">
-        <v>2192</v>
+        <v>2286</v>
       </c>
       <c r="E996" s="6" t="s">
         <v>23</v>
@@ -65998,10 +66088,10 @@
         <v>21</v>
       </c>
       <c r="K996" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L996" s="6">
-        <v>0</v>
+        <v>1.61</v>
       </c>
       <c r="M996" s="6">
         <v>0</v>
@@ -66013,10 +66103,10 @@
         <v>21</v>
       </c>
       <c r="P996" s="5" t="s">
-        <v>2191</v>
+        <v>2285</v>
       </c>
       <c r="Q996" s="6">
-        <v>0</v>
+        <v>2754</v>
       </c>
       <c r="R996" s="6" t="s">
         <v>23</v>
@@ -66027,60 +66117,650 @@
     </row>
     <row r="997" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A997" s="5" t="s">
+        <v>2287</v>
+      </c>
+      <c r="B997" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C997" s="5" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D997" s="5" t="s">
+        <v>2289</v>
+      </c>
+      <c r="E997" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F997" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G997" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H997" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I997" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J997" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K997" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L997" s="6">
+        <v>1.61</v>
+      </c>
+      <c r="M997" s="6">
+        <v>0</v>
+      </c>
+      <c r="N997" s="6">
+        <v>0</v>
+      </c>
+      <c r="O997" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P997" s="5" t="s">
+        <v>2288</v>
+      </c>
+      <c r="Q997" s="6">
+        <v>22355.75</v>
+      </c>
+      <c r="R997" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S997" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="998" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A998" s="5" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B998" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C998" s="5" t="s">
+        <v>2291</v>
+      </c>
+      <c r="D998" s="5" t="s">
+        <v>2292</v>
+      </c>
+      <c r="E998" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F998" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G998" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H998" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I998" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J998" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K998" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L998" s="6">
+        <v>0</v>
+      </c>
+      <c r="M998" s="6">
+        <v>0</v>
+      </c>
+      <c r="N998" s="6">
+        <v>0</v>
+      </c>
+      <c r="O998" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P998" s="5" t="s">
+        <v>2291</v>
+      </c>
+      <c r="Q998" s="6">
+        <v>0</v>
+      </c>
+      <c r="R998" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S998" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="999" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A999" s="5" t="s">
+        <v>2293</v>
+      </c>
+      <c r="B999" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C999" s="5" t="s">
+        <v>2294</v>
+      </c>
+      <c r="D999" s="5" t="s">
+        <v>2295</v>
+      </c>
+      <c r="E999" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F999" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G999" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H999" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I999" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J999" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K999" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L999" s="6">
+        <v>1.61</v>
+      </c>
+      <c r="M999" s="6">
+        <v>0</v>
+      </c>
+      <c r="N999" s="6">
+        <v>0</v>
+      </c>
+      <c r="O999" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P999" s="5" t="s">
+        <v>2294</v>
+      </c>
+      <c r="Q999" s="6">
+        <v>1632</v>
+      </c>
+      <c r="R999" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S999" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1000" s="5" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B1000" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1000" s="5" t="s">
+        <v>2297</v>
+      </c>
+      <c r="D1000" s="5" t="s">
+        <v>2298</v>
+      </c>
+      <c r="E1000" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1000" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1000" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1000" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1000" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1000" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1000" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1000" s="6">
+        <v>1.61</v>
+      </c>
+      <c r="M1000" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1000" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1000" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1000" s="5" t="s">
+        <v>2297</v>
+      </c>
+      <c r="Q1000" s="6">
+        <v>646.5</v>
+      </c>
+      <c r="R1000" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1000" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1001" s="5" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B1001" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1001" s="5" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D1001" s="5" t="s">
+        <v>2301</v>
+      </c>
+      <c r="E1001" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1001" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1001" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1001" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1001" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1001" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1001" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1001" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1001" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1001" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1001" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1001" s="5" t="s">
+        <v>2300</v>
+      </c>
+      <c r="Q1001" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1001" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1001" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1002" s="5" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B1002" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1002" s="5" t="s">
+        <v>2303</v>
+      </c>
+      <c r="D1002" s="5" t="s">
+        <v>2304</v>
+      </c>
+      <c r="E1002" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1002" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1002" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1002" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1002" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1002" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1002" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1002" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1002" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1002" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1002" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1002" s="5" t="s">
+        <v>2303</v>
+      </c>
+      <c r="Q1002" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1002" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1002" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1003" s="5" t="s">
+        <v>2165</v>
+      </c>
+      <c r="B1003" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1003" s="5" t="s">
+        <v>2166</v>
+      </c>
+      <c r="D1003" s="5" t="s">
+        <v>2167</v>
+      </c>
+      <c r="E1003" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1003" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1003" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1003" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1003" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1003" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1003" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1003" s="6">
+        <v>1.98</v>
+      </c>
+      <c r="M1003" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1003" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1003" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1003" s="5" t="s">
+        <v>2166</v>
+      </c>
+      <c r="Q1003" s="6">
+        <v>589.70000000000005</v>
+      </c>
+      <c r="R1003" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1003" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1004" s="5" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B1004" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1004" s="5" t="s">
+        <v>2169</v>
+      </c>
+      <c r="D1004" s="5" t="s">
+        <v>2170</v>
+      </c>
+      <c r="E1004" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1004" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1004" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1004" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1004" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1004" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1004" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1004" s="6">
+        <v>3.02</v>
+      </c>
+      <c r="M1004" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1004" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1004" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1004" s="5" t="s">
+        <v>2169</v>
+      </c>
+      <c r="Q1004" s="6">
+        <v>200.07</v>
+      </c>
+      <c r="R1004" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1004" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1005" s="5" t="s">
+        <v>2171</v>
+      </c>
+      <c r="B1005" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1005" s="5" t="s">
+        <v>2172</v>
+      </c>
+      <c r="D1005" s="5" t="s">
+        <v>2173</v>
+      </c>
+      <c r="E1005" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1005" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1005" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1005" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1005" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1005" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1005" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1005" s="6">
+        <v>2.65</v>
+      </c>
+      <c r="M1005" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1005" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1005" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1005" s="5" t="s">
+        <v>2172</v>
+      </c>
+      <c r="Q1005" s="6">
+        <v>1479.87</v>
+      </c>
+      <c r="R1005" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1005" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1006" s="5" t="s">
+        <v>2189</v>
+      </c>
+      <c r="B1006" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1006" s="5" t="s">
+        <v>2190</v>
+      </c>
+      <c r="D1006" s="5" t="s">
+        <v>2191</v>
+      </c>
+      <c r="E1006" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1006" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1006" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1006" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1006" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1006" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1006" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1006" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1006" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1006" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1006" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1006" s="5" t="s">
+        <v>2190</v>
+      </c>
+      <c r="Q1006" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1006" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1006" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1007" s="5" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B1007" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1007" s="5" t="s">
         <v>2193</v>
       </c>
-      <c r="B997" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C997" s="5" t="s">
+      <c r="D1007" s="5" t="s">
         <v>2194</v>
       </c>
-      <c r="D997" s="5" t="s">
-        <v>2195</v>
-      </c>
-      <c r="E997" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F997" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G997" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H997" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I997" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J997" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K997" s="6" t="s">
+      <c r="E1007" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1007" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1007" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1007" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1007" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1007" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1007" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="L997" s="6">
-        <v>0</v>
-      </c>
-      <c r="M997" s="6">
-        <v>0</v>
-      </c>
-      <c r="N997" s="6">
-        <v>0</v>
-      </c>
-      <c r="O997" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P997" s="5" t="s">
-        <v>2194</v>
-      </c>
-      <c r="Q997" s="6">
-        <v>0</v>
-      </c>
-      <c r="R997" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="S997" s="5" t="s">
+      <c r="L1007" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1007" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1007" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1007" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1007" s="5" t="s">
+        <v>2193</v>
+      </c>
+      <c r="Q1007" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1007" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1007" s="5" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
act db excel 05032020
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/TC_02.xlsx
+++ b/EXCEL LIBS/TC_02.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15111" uniqueCount="2311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15231" uniqueCount="2335">
   <si>
     <t>sqlnav01.aquinos.org : Aquinos, S.A.</t>
   </si>
@@ -6937,9 +6937,6 @@
     <t>LUX 06 - DARK GREY</t>
   </si>
   <si>
-    <t>Lista Produto : 26-02-2020 09:06:11</t>
-  </si>
-  <si>
     <t>TC15183</t>
   </si>
   <si>
@@ -6956,6 +6953,81 @@
   </si>
   <si>
     <t>QUEENS BORDEAUX</t>
+  </si>
+  <si>
+    <t>TC15185</t>
+  </si>
+  <si>
+    <t>G4001</t>
+  </si>
+  <si>
+    <t>KANSAS 8801 (PRETO)</t>
+  </si>
+  <si>
+    <t>TC15186</t>
+  </si>
+  <si>
+    <t>G4040</t>
+  </si>
+  <si>
+    <t>KANSAS 8012 (CASTANHO)</t>
+  </si>
+  <si>
+    <t>TC15187</t>
+  </si>
+  <si>
+    <t>G4140</t>
+  </si>
+  <si>
+    <t>ATLANTA 06 (CASTANHO)</t>
+  </si>
+  <si>
+    <t>TC15188</t>
+  </si>
+  <si>
+    <t>G3330</t>
+  </si>
+  <si>
+    <t>DEXTER - 59 VERDE</t>
+  </si>
+  <si>
+    <t>TC16006</t>
+  </si>
+  <si>
+    <t>V0330</t>
+  </si>
+  <si>
+    <t>BLUVEL 78 (VERDE)</t>
+  </si>
+  <si>
+    <t>TC16007</t>
+  </si>
+  <si>
+    <t>V0230</t>
+  </si>
+  <si>
+    <t>QUARTZ - 501 (VERDE)</t>
+  </si>
+  <si>
+    <t>Lista Produto : 05-03-2020 13:50:45</t>
+  </si>
+  <si>
+    <t>TC15189</t>
+  </si>
+  <si>
+    <t>G1914</t>
+  </si>
+  <si>
+    <t>MELVA 4380</t>
+  </si>
+  <si>
+    <t>TC15190</t>
+  </si>
+  <si>
+    <t>G4240</t>
+  </si>
+  <si>
+    <t>MONET 22 (BEGE)</t>
   </si>
 </sst>
 </file>
@@ -7122,8 +7194,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NavDataRegion" displayName="NavDataRegion" ref="A3:S1009" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A3:S1009"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NavDataRegion" displayName="NavDataRegion" ref="A3:S1017" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A3:S1017"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Nº" dataDxfId="16"/>
     <tableColumn id="2" name="Cód. Barras Efacec" dataDxfId="15"/>
@@ -7412,10 +7484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1009"/>
+  <dimension ref="A1:S1017"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F977" sqref="F977"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7466,7 +7538,7 @@
     </row>
     <row r="2" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2304</v>
+        <v>2328</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -17862,7 +17934,7 @@
         <v>376</v>
       </c>
       <c r="Q178" s="6">
-        <v>627.7636</v>
+        <v>594.2636</v>
       </c>
       <c r="R178" s="6" t="s">
         <v>23</v>
@@ -17921,7 +17993,7 @@
         <v>378</v>
       </c>
       <c r="Q179" s="6">
-        <v>559.69000000000005</v>
+        <v>501.69</v>
       </c>
       <c r="R179" s="6" t="s">
         <v>23</v>
@@ -18393,7 +18465,7 @@
         <v>394</v>
       </c>
       <c r="Q187" s="6">
-        <v>3098.88</v>
+        <v>6634.14</v>
       </c>
       <c r="R187" s="6" t="s">
         <v>23</v>
@@ -18747,7 +18819,7 @@
         <v>406</v>
       </c>
       <c r="Q193" s="6">
-        <v>1470.35</v>
+        <v>1133.1500000000001</v>
       </c>
       <c r="R193" s="6" t="s">
         <v>23</v>
@@ -19042,7 +19114,7 @@
         <v>416</v>
       </c>
       <c r="Q198" s="6">
-        <v>680.4</v>
+        <v>435.4</v>
       </c>
       <c r="R198" s="6" t="s">
         <v>23</v>
@@ -19514,7 +19586,7 @@
         <v>432</v>
       </c>
       <c r="Q206" s="6">
-        <v>2645.54</v>
+        <v>2348.09</v>
       </c>
       <c r="R206" s="6" t="s">
         <v>23</v>
@@ -19573,7 +19645,7 @@
         <v>434</v>
       </c>
       <c r="Q207" s="6">
-        <v>3665.61</v>
+        <v>3632.9692</v>
       </c>
       <c r="R207" s="6" t="s">
         <v>23</v>
@@ -19691,7 +19763,7 @@
         <v>438</v>
       </c>
       <c r="Q209" s="6">
-        <v>2459.04</v>
+        <v>2449.04</v>
       </c>
       <c r="R209" s="6" t="s">
         <v>23</v>
@@ -20458,7 +20530,7 @@
         <v>464</v>
       </c>
       <c r="Q222" s="6">
-        <v>2728.5012000000002</v>
+        <v>1786.1612</v>
       </c>
       <c r="R222" s="6" t="s">
         <v>23</v>
@@ -20517,7 +20589,7 @@
         <v>466</v>
       </c>
       <c r="Q223" s="6">
-        <v>1894.99</v>
+        <v>1884</v>
       </c>
       <c r="R223" s="6" t="s">
         <v>23</v>
@@ -21520,7 +21592,7 @@
         <v>500</v>
       </c>
       <c r="Q240" s="6">
-        <v>3151.8389999999999</v>
+        <v>4503.7190000000001</v>
       </c>
       <c r="R240" s="6" t="s">
         <v>23</v>
@@ -21697,7 +21769,7 @@
         <v>506</v>
       </c>
       <c r="Q243" s="6">
-        <v>608.91999999999996</v>
+        <v>607.63</v>
       </c>
       <c r="R243" s="6" t="s">
         <v>23</v>
@@ -21992,7 +22064,7 @@
         <v>516</v>
       </c>
       <c r="Q248" s="6">
-        <v>877.86</v>
+        <v>830</v>
       </c>
       <c r="R248" s="6" t="s">
         <v>23</v>
@@ -22110,7 +22182,7 @@
         <v>520</v>
       </c>
       <c r="Q250" s="6">
-        <v>-2450.36</v>
+        <v>-205.46</v>
       </c>
       <c r="R250" s="6" t="s">
         <v>23</v>
@@ -22169,7 +22241,7 @@
         <v>522</v>
       </c>
       <c r="Q251" s="6">
-        <v>587.05999999999995</v>
+        <v>1882.5</v>
       </c>
       <c r="R251" s="6" t="s">
         <v>23</v>
@@ -22995,7 +23067,7 @@
         <v>550</v>
       </c>
       <c r="Q265" s="6">
-        <v>1330.63</v>
+        <v>886.48</v>
       </c>
       <c r="R265" s="6" t="s">
         <v>23</v>
@@ -23054,7 +23126,7 @@
         <v>552</v>
       </c>
       <c r="Q266" s="6">
-        <v>2473.9299999999998</v>
+        <v>1458.93</v>
       </c>
       <c r="R266" s="6" t="s">
         <v>23</v>
@@ -23821,7 +23893,7 @@
         <v>579</v>
       </c>
       <c r="Q279" s="6">
-        <v>107.4618</v>
+        <v>106.2118</v>
       </c>
       <c r="R279" s="6" t="s">
         <v>23</v>
@@ -23880,7 +23952,7 @@
         <v>581</v>
       </c>
       <c r="Q280" s="6">
-        <v>554.98</v>
+        <v>611.6</v>
       </c>
       <c r="R280" s="6" t="s">
         <v>23</v>
@@ -24175,7 +24247,7 @@
         <v>591</v>
       </c>
       <c r="Q285" s="6">
-        <v>843.9</v>
+        <v>843.13</v>
       </c>
       <c r="R285" s="6" t="s">
         <v>23</v>
@@ -24234,7 +24306,7 @@
         <v>593</v>
       </c>
       <c r="Q286" s="6">
-        <v>1028.98</v>
+        <v>1020.88</v>
       </c>
       <c r="R286" s="6" t="s">
         <v>23</v>
@@ -24293,7 +24365,7 @@
         <v>595</v>
       </c>
       <c r="Q287" s="6">
-        <v>2381.7049999999999</v>
+        <v>1972.635</v>
       </c>
       <c r="R287" s="6" t="s">
         <v>23</v>
@@ -24352,7 +24424,7 @@
         <v>597</v>
       </c>
       <c r="Q288" s="6">
-        <v>1814.77</v>
+        <v>1656.81</v>
       </c>
       <c r="R288" s="6" t="s">
         <v>23</v>
@@ -24411,7 +24483,7 @@
         <v>599</v>
       </c>
       <c r="Q289" s="6">
-        <v>1252.1400000000001</v>
+        <v>1239.43</v>
       </c>
       <c r="R289" s="6" t="s">
         <v>23</v>
@@ -24470,7 +24542,7 @@
         <v>601</v>
       </c>
       <c r="Q290" s="6">
-        <v>3566.68</v>
+        <v>3463.87</v>
       </c>
       <c r="R290" s="6" t="s">
         <v>23</v>
@@ -24529,7 +24601,7 @@
         <v>603</v>
       </c>
       <c r="Q291" s="6">
-        <v>2595.569</v>
+        <v>2728.34</v>
       </c>
       <c r="R291" s="6" t="s">
         <v>23</v>
@@ -24824,7 +24896,7 @@
         <v>613</v>
       </c>
       <c r="Q296" s="6">
-        <v>1244.93</v>
+        <v>1244.6500000000001</v>
       </c>
       <c r="R296" s="6" t="s">
         <v>23</v>
@@ -24883,7 +24955,7 @@
         <v>615</v>
       </c>
       <c r="Q297" s="6">
-        <v>3419.41</v>
+        <v>3404.55</v>
       </c>
       <c r="R297" s="6" t="s">
         <v>23</v>
@@ -25001,7 +25073,7 @@
         <v>619</v>
       </c>
       <c r="Q299" s="6">
-        <v>908.45</v>
+        <v>183.19</v>
       </c>
       <c r="R299" s="6" t="s">
         <v>23</v>
@@ -25060,7 +25132,7 @@
         <v>621</v>
       </c>
       <c r="Q300" s="6">
-        <v>1752.895</v>
+        <v>2381.0549999999998</v>
       </c>
       <c r="R300" s="6" t="s">
         <v>23</v>
@@ -25119,7 +25191,7 @@
         <v>623</v>
       </c>
       <c r="Q301" s="6">
-        <v>1171.18</v>
+        <v>1779.36</v>
       </c>
       <c r="R301" s="6" t="s">
         <v>23</v>
@@ -25178,7 +25250,7 @@
         <v>625</v>
       </c>
       <c r="Q302" s="6">
-        <v>1418.87</v>
+        <v>985.87</v>
       </c>
       <c r="R302" s="6" t="s">
         <v>23</v>
@@ -25237,7 +25309,7 @@
         <v>627</v>
       </c>
       <c r="Q303" s="6">
-        <v>42264.657399999996</v>
+        <v>24381.207399999999</v>
       </c>
       <c r="R303" s="6" t="s">
         <v>23</v>
@@ -25296,7 +25368,7 @@
         <v>629</v>
       </c>
       <c r="Q304" s="6">
-        <v>35271.891000000003</v>
+        <v>36568.580999999998</v>
       </c>
       <c r="R304" s="6" t="s">
         <v>23</v>
@@ -25399,7 +25471,7 @@
         <v>23</v>
       </c>
       <c r="L306" s="6">
-        <v>2.29</v>
+        <v>2.75</v>
       </c>
       <c r="M306" s="6">
         <v>0</v>
@@ -25414,7 +25486,7 @@
         <v>633</v>
       </c>
       <c r="Q306" s="6">
-        <v>24.585000000000001</v>
+        <v>506.65499999999997</v>
       </c>
       <c r="R306" s="6" t="s">
         <v>23</v>
@@ -25650,7 +25722,7 @@
         <v>641</v>
       </c>
       <c r="Q310" s="6">
-        <v>3672.36</v>
+        <v>3610.22</v>
       </c>
       <c r="R310" s="6" t="s">
         <v>23</v>
@@ -25768,7 +25840,7 @@
         <v>646</v>
       </c>
       <c r="Q312" s="6">
-        <v>2241.98</v>
+        <v>1654.65</v>
       </c>
       <c r="R312" s="6" t="s">
         <v>23</v>
@@ -25827,7 +25899,7 @@
         <v>649</v>
       </c>
       <c r="Q313" s="6">
-        <v>178.88</v>
+        <v>98.38</v>
       </c>
       <c r="R313" s="6" t="s">
         <v>23</v>
@@ -25886,7 +25958,7 @@
         <v>652</v>
       </c>
       <c r="Q314" s="6">
-        <v>2268.33</v>
+        <v>2226.64</v>
       </c>
       <c r="R314" s="6" t="s">
         <v>23</v>
@@ -26004,7 +26076,7 @@
         <v>658</v>
       </c>
       <c r="Q316" s="6">
-        <v>254.19</v>
+        <v>247.24</v>
       </c>
       <c r="R316" s="6" t="s">
         <v>23</v>
@@ -26063,7 +26135,7 @@
         <v>660</v>
       </c>
       <c r="Q317" s="6">
-        <v>8737.5650000000005</v>
+        <v>8724.0550000000003</v>
       </c>
       <c r="R317" s="6" t="s">
         <v>23</v>
@@ -26122,7 +26194,7 @@
         <v>662</v>
       </c>
       <c r="Q318" s="6">
-        <v>3547.14</v>
+        <v>3340.16</v>
       </c>
       <c r="R318" s="6" t="s">
         <v>23</v>
@@ -26181,7 +26253,7 @@
         <v>664</v>
       </c>
       <c r="Q319" s="6">
-        <v>7132.64</v>
+        <v>8484.6</v>
       </c>
       <c r="R319" s="6" t="s">
         <v>23</v>
@@ -26240,7 +26312,7 @@
         <v>666</v>
       </c>
       <c r="Q320" s="6">
-        <v>2879.79</v>
+        <v>2613.27</v>
       </c>
       <c r="R320" s="6" t="s">
         <v>23</v>
@@ -26299,7 +26371,7 @@
         <v>668</v>
       </c>
       <c r="Q321" s="6">
-        <v>6430.21</v>
+        <v>5088.82</v>
       </c>
       <c r="R321" s="6" t="s">
         <v>23</v>
@@ -26358,7 +26430,7 @@
         <v>670</v>
       </c>
       <c r="Q322" s="6">
-        <v>2011.1004</v>
+        <v>1972.9304</v>
       </c>
       <c r="R322" s="6" t="s">
         <v>23</v>
@@ -26417,7 +26489,7 @@
         <v>672</v>
       </c>
       <c r="Q323" s="6">
-        <v>1404.345</v>
+        <v>1876.5150000000001</v>
       </c>
       <c r="R323" s="6" t="s">
         <v>23</v>
@@ -26476,7 +26548,7 @@
         <v>674</v>
       </c>
       <c r="Q324" s="6">
-        <v>2708.52</v>
+        <v>2638.05</v>
       </c>
       <c r="R324" s="6" t="s">
         <v>23</v>
@@ -26535,7 +26607,7 @@
         <v>676</v>
       </c>
       <c r="Q325" s="6">
-        <v>3878.4025999999999</v>
+        <v>3849.2125999999998</v>
       </c>
       <c r="R325" s="6" t="s">
         <v>23</v>
@@ -26594,7 +26666,7 @@
         <v>678</v>
       </c>
       <c r="Q326" s="6">
-        <v>1880.9</v>
+        <v>1772.309</v>
       </c>
       <c r="R326" s="6" t="s">
         <v>23</v>
@@ -26712,7 +26784,7 @@
         <v>683</v>
       </c>
       <c r="Q328" s="6">
-        <v>3359.681</v>
+        <v>3242.0810000000001</v>
       </c>
       <c r="R328" s="6" t="s">
         <v>23</v>
@@ -26771,7 +26843,7 @@
         <v>686</v>
       </c>
       <c r="Q329" s="6">
-        <v>2052.11</v>
+        <v>2038.53</v>
       </c>
       <c r="R329" s="6" t="s">
         <v>23</v>
@@ -26830,7 +26902,7 @@
         <v>689</v>
       </c>
       <c r="Q330" s="6">
-        <v>716.53</v>
+        <v>715.82</v>
       </c>
       <c r="R330" s="6" t="s">
         <v>23</v>
@@ -26889,7 +26961,7 @@
         <v>692</v>
       </c>
       <c r="Q331" s="6">
-        <v>1125.4749999999999</v>
+        <v>2540.0450000000001</v>
       </c>
       <c r="R331" s="6" t="s">
         <v>23</v>
@@ -26948,7 +27020,7 @@
         <v>694</v>
       </c>
       <c r="Q332" s="6">
-        <v>2995</v>
+        <v>2990.77</v>
       </c>
       <c r="R332" s="6" t="s">
         <v>23</v>
@@ -27007,7 +27079,7 @@
         <v>697</v>
       </c>
       <c r="Q333" s="6">
-        <v>1910.09</v>
+        <v>1903.2</v>
       </c>
       <c r="R333" s="6" t="s">
         <v>23</v>
@@ -27125,7 +27197,7 @@
         <v>703</v>
       </c>
       <c r="Q335" s="6">
-        <v>1315.7950000000001</v>
+        <v>1313.1949999999999</v>
       </c>
       <c r="R335" s="6" t="s">
         <v>23</v>
@@ -27184,7 +27256,7 @@
         <v>706</v>
       </c>
       <c r="Q336" s="6">
-        <v>2289.87</v>
+        <v>2236.31</v>
       </c>
       <c r="R336" s="6" t="s">
         <v>23</v>
@@ -27420,7 +27492,7 @@
         <v>714</v>
       </c>
       <c r="Q340" s="6">
-        <v>158.35499999999999</v>
+        <v>155.84</v>
       </c>
       <c r="R340" s="6" t="s">
         <v>23</v>
@@ -27538,7 +27610,7 @@
         <v>718</v>
       </c>
       <c r="Q342" s="6">
-        <v>2669.8</v>
+        <v>2664.93</v>
       </c>
       <c r="R342" s="6" t="s">
         <v>23</v>
@@ -27715,7 +27787,7 @@
         <v>724</v>
       </c>
       <c r="Q345" s="6">
-        <v>1951.7</v>
+        <v>867.82</v>
       </c>
       <c r="R345" s="6" t="s">
         <v>23</v>
@@ -27774,7 +27846,7 @@
         <v>726</v>
       </c>
       <c r="Q346" s="6">
-        <v>197.22</v>
+        <v>153.5</v>
       </c>
       <c r="R346" s="6" t="s">
         <v>23</v>
@@ -27833,7 +27905,7 @@
         <v>728</v>
       </c>
       <c r="Q347" s="6">
-        <v>177.6</v>
+        <v>164.96</v>
       </c>
       <c r="R347" s="6" t="s">
         <v>23</v>
@@ -27892,7 +27964,7 @@
         <v>731</v>
       </c>
       <c r="Q348" s="6">
-        <v>401.49</v>
+        <v>334.44</v>
       </c>
       <c r="R348" s="6" t="s">
         <v>23</v>
@@ -27936,7 +28008,7 @@
         <v>23</v>
       </c>
       <c r="L349" s="6">
-        <v>3.75</v>
+        <v>3.02</v>
       </c>
       <c r="M349" s="6">
         <v>0</v>
@@ -27951,7 +28023,7 @@
         <v>734</v>
       </c>
       <c r="Q349" s="6">
-        <v>1162.08</v>
+        <v>643.53</v>
       </c>
       <c r="R349" s="6" t="s">
         <v>23</v>
@@ -28010,7 +28082,7 @@
         <v>736</v>
       </c>
       <c r="Q350" s="6">
-        <v>4857.5550000000003</v>
+        <v>4799.0050000000001</v>
       </c>
       <c r="R350" s="6" t="s">
         <v>23</v>
@@ -28069,7 +28141,7 @@
         <v>738</v>
       </c>
       <c r="Q351" s="6">
-        <v>28336.23</v>
+        <v>24788.5</v>
       </c>
       <c r="R351" s="6" t="s">
         <v>23</v>
@@ -28128,7 +28200,7 @@
         <v>741</v>
       </c>
       <c r="Q352" s="6">
-        <v>3544.45</v>
+        <v>3537.05</v>
       </c>
       <c r="R352" s="6" t="s">
         <v>23</v>
@@ -28246,7 +28318,7 @@
         <v>747</v>
       </c>
       <c r="Q354" s="6">
-        <v>166.43</v>
+        <v>165.13</v>
       </c>
       <c r="R354" s="6" t="s">
         <v>23</v>
@@ -28305,7 +28377,7 @@
         <v>749</v>
       </c>
       <c r="Q355" s="6">
-        <v>1458.98</v>
+        <v>1423.43</v>
       </c>
       <c r="R355" s="6" t="s">
         <v>23</v>
@@ -28541,7 +28613,7 @@
         <v>757</v>
       </c>
       <c r="Q359" s="6">
-        <v>921.47</v>
+        <v>909.97</v>
       </c>
       <c r="R359" s="6" t="s">
         <v>23</v>
@@ -28600,7 +28672,7 @@
         <v>759</v>
       </c>
       <c r="Q360" s="6">
-        <v>1531.57</v>
+        <v>1517.35</v>
       </c>
       <c r="R360" s="6" t="s">
         <v>23</v>
@@ -29190,7 +29262,7 @@
         <v>791</v>
       </c>
       <c r="Q370" s="6">
-        <v>155.9</v>
+        <v>154.4</v>
       </c>
       <c r="R370" s="6" t="s">
         <v>23</v>
@@ -35385,7 +35457,7 @@
         <v>1004</v>
       </c>
       <c r="Q475" s="6">
-        <v>207.785</v>
+        <v>181.79499999999999</v>
       </c>
       <c r="R475" s="6" t="s">
         <v>23</v>
@@ -35444,7 +35516,7 @@
         <v>1006</v>
       </c>
       <c r="Q476" s="6">
-        <v>130.47</v>
+        <v>-68.290000000000006</v>
       </c>
       <c r="R476" s="6" t="s">
         <v>23</v>
@@ -35503,7 +35575,7 @@
         <v>1008</v>
       </c>
       <c r="Q477" s="6">
-        <v>288.84500000000003</v>
+        <v>275.42750000000001</v>
       </c>
       <c r="R477" s="6" t="s">
         <v>23</v>
@@ -35562,7 +35634,7 @@
         <v>1010</v>
       </c>
       <c r="Q478" s="6">
-        <v>1193.33</v>
+        <v>401.93</v>
       </c>
       <c r="R478" s="6" t="s">
         <v>23</v>
@@ -35606,7 +35678,7 @@
         <v>23</v>
       </c>
       <c r="L479" s="6">
-        <v>4.22</v>
+        <v>3.99</v>
       </c>
       <c r="M479" s="6">
         <v>0</v>
@@ -35621,7 +35693,7 @@
         <v>1012</v>
       </c>
       <c r="Q479" s="6">
-        <v>149.13999999999999</v>
+        <v>709.84</v>
       </c>
       <c r="R479" s="6" t="s">
         <v>23</v>
@@ -51197,7 +51269,7 @@
         <v>1546</v>
       </c>
       <c r="Q743" s="6">
-        <v>445.72</v>
+        <v>422.92</v>
       </c>
       <c r="R743" s="6" t="s">
         <v>23</v>
@@ -51492,7 +51564,7 @@
         <v>1563</v>
       </c>
       <c r="Q748" s="6">
-        <v>444.22</v>
+        <v>391.61</v>
       </c>
       <c r="R748" s="6" t="s">
         <v>23</v>
@@ -53970,7 +54042,7 @@
         <v>1655</v>
       </c>
       <c r="Q790" s="6">
-        <v>7418.4906799999999</v>
+        <v>12082.10204</v>
       </c>
       <c r="R790" s="6" t="s">
         <v>23</v>
@@ -54088,7 +54160,7 @@
         <v>1659</v>
       </c>
       <c r="Q792" s="6">
-        <v>933.49</v>
+        <v>2217.83</v>
       </c>
       <c r="R792" s="6" t="s">
         <v>23</v>
@@ -54206,7 +54278,7 @@
         <v>1663</v>
       </c>
       <c r="Q794" s="6">
-        <v>2521.585</v>
+        <v>1817.7550000000001</v>
       </c>
       <c r="R794" s="6" t="s">
         <v>23</v>
@@ -54265,7 +54337,7 @@
         <v>1665</v>
       </c>
       <c r="Q795" s="6">
-        <v>18926.71</v>
+        <v>21715.87</v>
       </c>
       <c r="R795" s="6" t="s">
         <v>23</v>
@@ -54560,7 +54632,7 @@
         <v>1675</v>
       </c>
       <c r="Q800" s="6">
-        <v>6565.2</v>
+        <v>8729.5732800000005</v>
       </c>
       <c r="R800" s="6" t="s">
         <v>23</v>
@@ -54678,7 +54750,7 @@
         <v>1679</v>
       </c>
       <c r="Q802" s="6">
-        <v>636.15</v>
+        <v>523.49159999999995</v>
       </c>
       <c r="R802" s="6" t="s">
         <v>23</v>
@@ -54737,7 +54809,7 @@
         <v>1681</v>
       </c>
       <c r="Q803" s="6">
-        <v>12195.367</v>
+        <v>7169.2556000000004</v>
       </c>
       <c r="R803" s="6" t="s">
         <v>23</v>
@@ -54796,7 +54868,7 @@
         <v>1684</v>
       </c>
       <c r="Q804" s="6">
-        <v>19350.52</v>
+        <v>17726.02</v>
       </c>
       <c r="R804" s="6" t="s">
         <v>23</v>
@@ -54855,7 +54927,7 @@
         <v>1687</v>
       </c>
       <c r="Q805" s="6">
-        <v>33533.708299999998</v>
+        <v>30800.445</v>
       </c>
       <c r="R805" s="6" t="s">
         <v>23</v>
@@ -54914,7 +54986,7 @@
         <v>1690</v>
       </c>
       <c r="Q806" s="6">
-        <v>1289.9000000000001</v>
+        <v>442.11919999999998</v>
       </c>
       <c r="R806" s="6" t="s">
         <v>23</v>
@@ -54973,7 +55045,7 @@
         <v>1693</v>
       </c>
       <c r="Q807" s="6">
-        <v>5187.8100000000004</v>
+        <v>6185.01</v>
       </c>
       <c r="R807" s="6" t="s">
         <v>23</v>
@@ -55917,7 +55989,7 @@
         <v>1735</v>
       </c>
       <c r="Q823" s="6">
-        <v>3073.08</v>
+        <v>4427.08</v>
       </c>
       <c r="R823" s="6" t="s">
         <v>23</v>
@@ -56389,7 +56461,7 @@
         <v>1758</v>
       </c>
       <c r="Q831" s="6">
-        <v>13903.52</v>
+        <v>8321.66</v>
       </c>
       <c r="R831" s="6" t="s">
         <v>23</v>
@@ -56448,7 +56520,7 @@
         <v>1762</v>
       </c>
       <c r="Q832" s="6">
-        <v>9023.4699999999993</v>
+        <v>4921.47</v>
       </c>
       <c r="R832" s="6" t="s">
         <v>23</v>
@@ -56625,7 +56697,7 @@
         <v>1771</v>
       </c>
       <c r="Q835" s="6">
-        <v>2180.38</v>
+        <v>223.92</v>
       </c>
       <c r="R835" s="6" t="s">
         <v>23</v>
@@ -56979,7 +57051,7 @@
         <v>747</v>
       </c>
       <c r="Q841" s="6">
-        <v>663.49</v>
+        <v>627.48</v>
       </c>
       <c r="R841" s="6" t="s">
         <v>23</v>
@@ -57097,7 +57169,7 @@
         <v>1800</v>
       </c>
       <c r="Q843" s="6">
-        <v>278.67</v>
+        <v>194.01</v>
       </c>
       <c r="R843" s="6" t="s">
         <v>23</v>
@@ -57274,7 +57346,7 @@
         <v>1809</v>
       </c>
       <c r="Q846" s="6">
-        <v>189.3</v>
+        <v>179.58</v>
       </c>
       <c r="R846" s="6" t="s">
         <v>23</v>
@@ -57495,7 +57567,7 @@
         <v>23</v>
       </c>
       <c r="L850" s="6">
-        <v>2.4</v>
+        <v>1.72</v>
       </c>
       <c r="M850" s="6">
         <v>0</v>
@@ -57510,7 +57582,7 @@
         <v>1822</v>
       </c>
       <c r="Q850" s="6">
-        <v>0</v>
+        <v>22809.1</v>
       </c>
       <c r="R850" s="6" t="s">
         <v>23</v>
@@ -58513,7 +58585,7 @@
         <v>1874</v>
       </c>
       <c r="Q867" s="6">
-        <v>11598.33</v>
+        <v>11689.17</v>
       </c>
       <c r="R867" s="6" t="s">
         <v>23</v>
@@ -58631,7 +58703,7 @@
         <v>1880</v>
       </c>
       <c r="Q869" s="6">
-        <v>175.9</v>
+        <v>166.08</v>
       </c>
       <c r="R869" s="6" t="s">
         <v>23</v>
@@ -58808,7 +58880,7 @@
         <v>1889</v>
       </c>
       <c r="Q872" s="6">
-        <v>185.69</v>
+        <v>161.38999999999999</v>
       </c>
       <c r="R872" s="6" t="s">
         <v>23</v>
@@ -58867,7 +58939,7 @@
         <v>1892</v>
       </c>
       <c r="Q873" s="6">
-        <v>276.83</v>
+        <v>228.23</v>
       </c>
       <c r="R873" s="6" t="s">
         <v>23</v>
@@ -58926,7 +58998,7 @@
         <v>1895</v>
       </c>
       <c r="Q874" s="6">
-        <v>664.17</v>
+        <v>627.09</v>
       </c>
       <c r="R874" s="6" t="s">
         <v>23</v>
@@ -58985,7 +59057,7 @@
         <v>1898</v>
       </c>
       <c r="Q875" s="6">
-        <v>101.19</v>
+        <v>79.33</v>
       </c>
       <c r="R875" s="6" t="s">
         <v>23</v>
@@ -59870,7 +59942,7 @@
         <v>1944</v>
       </c>
       <c r="Q890" s="6">
-        <v>246.05500000000001</v>
+        <v>75.084999999999994</v>
       </c>
       <c r="R890" s="6" t="s">
         <v>23</v>
@@ -61684,7 +61756,7 @@
         <v>23</v>
       </c>
       <c r="L921" s="6">
-        <v>1.1599999999999999</v>
+        <v>1.51</v>
       </c>
       <c r="M921" s="6">
         <v>0</v>
@@ -61699,7 +61771,7 @@
         <v>2038</v>
       </c>
       <c r="Q921" s="6">
-        <v>2256.6799999999998</v>
+        <v>2650.92</v>
       </c>
       <c r="R921" s="6" t="s">
         <v>23</v>
@@ -61758,7 +61830,7 @@
         <v>2041</v>
       </c>
       <c r="Q922" s="6">
-        <v>14639.15</v>
+        <v>12258.17</v>
       </c>
       <c r="R922" s="6" t="s">
         <v>23</v>
@@ -61876,7 +61948,7 @@
         <v>2047</v>
       </c>
       <c r="Q924" s="6">
-        <v>6058.6030000000001</v>
+        <v>5990.2730000000001</v>
       </c>
       <c r="R924" s="6" t="s">
         <v>23</v>
@@ -61920,7 +61992,7 @@
         <v>23</v>
       </c>
       <c r="L925" s="6">
-        <v>2.48</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M925" s="6">
         <v>0</v>
@@ -61935,7 +62007,7 @@
         <v>2050</v>
       </c>
       <c r="Q925" s="6">
-        <v>489</v>
+        <v>742</v>
       </c>
       <c r="R925" s="6" t="s">
         <v>23</v>
@@ -61994,7 +62066,7 @@
         <v>2053</v>
       </c>
       <c r="Q926" s="6">
-        <v>1492.02</v>
+        <v>2782.52</v>
       </c>
       <c r="R926" s="6" t="s">
         <v>23</v>
@@ -62053,7 +62125,7 @@
         <v>2056</v>
       </c>
       <c r="Q927" s="6">
-        <v>2316</v>
+        <v>3099.21</v>
       </c>
       <c r="R927" s="6" t="s">
         <v>23</v>
@@ -62112,7 +62184,7 @@
         <v>2059</v>
       </c>
       <c r="Q928" s="6">
-        <v>318.2</v>
+        <v>308.63</v>
       </c>
       <c r="R928" s="6" t="s">
         <v>23</v>
@@ -62171,7 +62243,7 @@
         <v>2062</v>
       </c>
       <c r="Q929" s="6">
-        <v>444.17</v>
+        <v>540.03</v>
       </c>
       <c r="R929" s="6" t="s">
         <v>23</v>
@@ -62230,7 +62302,7 @@
         <v>2065</v>
       </c>
       <c r="Q930" s="6">
-        <v>2208.09</v>
+        <v>1798.69</v>
       </c>
       <c r="R930" s="6" t="s">
         <v>23</v>
@@ -62289,7 +62361,7 @@
         <v>2068</v>
       </c>
       <c r="Q931" s="6">
-        <v>490</v>
+        <v>758.14</v>
       </c>
       <c r="R931" s="6" t="s">
         <v>23</v>
@@ -62584,7 +62656,7 @@
         <v>2083</v>
       </c>
       <c r="Q936" s="6">
-        <v>3917.6</v>
+        <v>3536.36</v>
       </c>
       <c r="R936" s="6" t="s">
         <v>23</v>
@@ -62761,7 +62833,7 @@
         <v>2092</v>
       </c>
       <c r="Q939" s="6">
-        <v>3749.72</v>
+        <v>3554.11</v>
       </c>
       <c r="R939" s="6" t="s">
         <v>23</v>
@@ -62820,7 +62892,7 @@
         <v>2095</v>
       </c>
       <c r="Q940" s="6">
-        <v>1734.42</v>
+        <v>1613.42</v>
       </c>
       <c r="R940" s="6" t="s">
         <v>23</v>
@@ -62879,7 +62951,7 @@
         <v>2098</v>
       </c>
       <c r="Q941" s="6">
-        <v>220.05</v>
+        <v>135.36000000000001</v>
       </c>
       <c r="R941" s="6" t="s">
         <v>23</v>
@@ -62938,7 +63010,7 @@
         <v>2101</v>
       </c>
       <c r="Q942" s="6">
-        <v>670.755</v>
+        <v>474.00236000000001</v>
       </c>
       <c r="R942" s="6" t="s">
         <v>23</v>
@@ -63056,7 +63128,7 @@
         <v>2107</v>
       </c>
       <c r="Q944" s="6">
-        <v>2491.12</v>
+        <v>2185.92</v>
       </c>
       <c r="R944" s="6" t="s">
         <v>23</v>
@@ -63292,7 +63364,7 @@
         <v>2119</v>
       </c>
       <c r="Q948" s="6">
-        <v>4137.7</v>
+        <v>2675.9090000000001</v>
       </c>
       <c r="R948" s="6" t="s">
         <v>23</v>
@@ -63351,7 +63423,7 @@
         <v>2122</v>
       </c>
       <c r="Q949" s="6">
-        <v>106.97</v>
+        <v>500.27</v>
       </c>
       <c r="R949" s="6" t="s">
         <v>23</v>
@@ -63410,7 +63482,7 @@
         <v>2125</v>
       </c>
       <c r="Q950" s="6">
-        <v>392.505</v>
+        <v>88.825000000000003</v>
       </c>
       <c r="R950" s="6" t="s">
         <v>23</v>
@@ -63469,7 +63541,7 @@
         <v>2128</v>
       </c>
       <c r="Q951" s="6">
-        <v>98.991299999999995</v>
+        <v>614.59130000000005</v>
       </c>
       <c r="R951" s="6" t="s">
         <v>23</v>
@@ -63528,7 +63600,7 @@
         <v>2131</v>
       </c>
       <c r="Q952" s="6">
-        <v>201.44</v>
+        <v>353.64</v>
       </c>
       <c r="R952" s="6" t="s">
         <v>23</v>
@@ -63587,7 +63659,7 @@
         <v>2134</v>
       </c>
       <c r="Q953" s="6">
-        <v>292.05</v>
+        <v>191.45</v>
       </c>
       <c r="R953" s="6" t="s">
         <v>23</v>
@@ -63646,7 +63718,7 @@
         <v>2137</v>
       </c>
       <c r="Q954" s="6">
-        <v>100.5</v>
+        <v>506.7</v>
       </c>
       <c r="R954" s="6" t="s">
         <v>23</v>
@@ -63705,7 +63777,7 @@
         <v>2140</v>
       </c>
       <c r="Q955" s="6">
-        <v>141.1</v>
+        <v>462.3</v>
       </c>
       <c r="R955" s="6" t="s">
         <v>23</v>
@@ -63882,7 +63954,7 @@
         <v>2149</v>
       </c>
       <c r="Q958" s="6">
-        <v>3748.5803999999998</v>
+        <v>5775.0803999999998</v>
       </c>
       <c r="R958" s="6" t="s">
         <v>23</v>
@@ -63941,7 +64013,7 @@
         <v>2151</v>
       </c>
       <c r="Q959" s="6">
-        <v>3535.2</v>
+        <v>2456.44</v>
       </c>
       <c r="R959" s="6" t="s">
         <v>23</v>
@@ -64000,7 +64072,7 @@
         <v>2154</v>
       </c>
       <c r="Q960" s="6">
-        <v>703.9</v>
+        <v>909.28</v>
       </c>
       <c r="R960" s="6" t="s">
         <v>23</v>
@@ -64059,7 +64131,7 @@
         <v>2157</v>
       </c>
       <c r="Q961" s="6">
-        <v>3710.45</v>
+        <v>3446.65</v>
       </c>
       <c r="R961" s="6" t="s">
         <v>23</v>
@@ -64395,10 +64467,10 @@
         <v>21</v>
       </c>
       <c r="K967" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L967" s="6">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="M967" s="6">
         <v>0</v>
@@ -64413,7 +64485,7 @@
         <v>2196</v>
       </c>
       <c r="Q967" s="6">
-        <v>0</v>
+        <v>960.1</v>
       </c>
       <c r="R967" s="6" t="s">
         <v>23</v>
@@ -65062,7 +65134,7 @@
         <v>2228</v>
       </c>
       <c r="Q978" s="6">
-        <v>583.1</v>
+        <v>3388.22</v>
       </c>
       <c r="R978" s="6" t="s">
         <v>23</v>
@@ -65162,10 +65234,10 @@
         <v>21</v>
       </c>
       <c r="K980" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L980" s="6">
-        <v>0</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="M980" s="6">
         <v>0</v>
@@ -65180,7 +65252,7 @@
         <v>2233</v>
       </c>
       <c r="Q980" s="6">
-        <v>0</v>
+        <v>7950.7</v>
       </c>
       <c r="R980" s="6" t="s">
         <v>23</v>
@@ -65221,10 +65293,10 @@
         <v>21</v>
       </c>
       <c r="K981" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L981" s="6">
-        <v>0</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="M981" s="6">
         <v>0</v>
@@ -65239,7 +65311,7 @@
         <v>2236</v>
       </c>
       <c r="Q981" s="6">
-        <v>0</v>
+        <v>6942.5</v>
       </c>
       <c r="R981" s="6" t="s">
         <v>23</v>
@@ -65280,10 +65352,10 @@
         <v>21</v>
       </c>
       <c r="K982" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L982" s="6">
-        <v>0</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="M982" s="6">
         <v>0</v>
@@ -65298,7 +65370,7 @@
         <v>2239</v>
       </c>
       <c r="Q982" s="6">
-        <v>0</v>
+        <v>717.2</v>
       </c>
       <c r="R982" s="6" t="s">
         <v>23</v>
@@ -65339,10 +65411,10 @@
         <v>21</v>
       </c>
       <c r="K983" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L983" s="6">
-        <v>0</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="M983" s="6">
         <v>0</v>
@@ -65357,7 +65429,7 @@
         <v>2242</v>
       </c>
       <c r="Q983" s="6">
-        <v>0</v>
+        <v>1691.2</v>
       </c>
       <c r="R983" s="6" t="s">
         <v>23</v>
@@ -65398,10 +65470,10 @@
         <v>21</v>
       </c>
       <c r="K984" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L984" s="6">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="M984" s="6">
         <v>0</v>
@@ -65416,7 +65488,7 @@
         <v>2245</v>
       </c>
       <c r="Q984" s="6">
-        <v>0</v>
+        <v>254.2</v>
       </c>
       <c r="R984" s="6" t="s">
         <v>23</v>
@@ -65457,10 +65529,10 @@
         <v>21</v>
       </c>
       <c r="K985" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L985" s="6">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="M985" s="6">
         <v>0</v>
@@ -65475,7 +65547,7 @@
         <v>2248</v>
       </c>
       <c r="Q985" s="6">
-        <v>0</v>
+        <v>466.1</v>
       </c>
       <c r="R985" s="6" t="s">
         <v>23</v>
@@ -65519,7 +65591,7 @@
         <v>23</v>
       </c>
       <c r="L986" s="6">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="M986" s="6">
         <v>0</v>
@@ -65593,7 +65665,7 @@
         <v>2254</v>
       </c>
       <c r="Q987" s="6">
-        <v>43.19</v>
+        <v>343.19</v>
       </c>
       <c r="R987" s="6" t="s">
         <v>23</v>
@@ -65752,10 +65824,10 @@
         <v>21</v>
       </c>
       <c r="K990" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L990" s="6">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="M990" s="6">
         <v>0</v>
@@ -65770,7 +65842,7 @@
         <v>2263</v>
       </c>
       <c r="Q990" s="6">
-        <v>0</v>
+        <v>156.19999999999999</v>
       </c>
       <c r="R990" s="6" t="s">
         <v>23</v>
@@ -65811,10 +65883,10 @@
         <v>21</v>
       </c>
       <c r="K991" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L991" s="6">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="M991" s="6">
         <v>0</v>
@@ -65829,7 +65901,7 @@
         <v>2266</v>
       </c>
       <c r="Q991" s="6">
-        <v>0</v>
+        <v>151.4</v>
       </c>
       <c r="R991" s="6" t="s">
         <v>23</v>
@@ -65873,7 +65945,7 @@
         <v>23</v>
       </c>
       <c r="L992" s="6">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="M992" s="6">
         <v>0</v>
@@ -65888,7 +65960,7 @@
         <v>2269</v>
       </c>
       <c r="Q992" s="6">
-        <v>133.80000000000001</v>
+        <v>138.04</v>
       </c>
       <c r="R992" s="6" t="s">
         <v>23</v>
@@ -65988,10 +66060,10 @@
         <v>21</v>
       </c>
       <c r="K994" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L994" s="6">
-        <v>0</v>
+        <v>1.58</v>
       </c>
       <c r="M994" s="6">
         <v>0</v>
@@ -66006,7 +66078,7 @@
         <v>2278</v>
       </c>
       <c r="Q994" s="6">
-        <v>0</v>
+        <v>1622</v>
       </c>
       <c r="R994" s="6" t="s">
         <v>23</v>
@@ -66065,7 +66137,7 @@
         <v>2281</v>
       </c>
       <c r="Q995" s="6">
-        <v>2257</v>
+        <v>2238.5</v>
       </c>
       <c r="R995" s="6" t="s">
         <v>23</v>
@@ -66124,7 +66196,7 @@
         <v>2284</v>
       </c>
       <c r="Q996" s="6">
-        <v>2754</v>
+        <v>15849.15</v>
       </c>
       <c r="R996" s="6" t="s">
         <v>23</v>
@@ -66183,7 +66255,7 @@
         <v>2287</v>
       </c>
       <c r="Q997" s="6">
-        <v>19297.64</v>
+        <v>36056.769999999997</v>
       </c>
       <c r="R997" s="6" t="s">
         <v>23</v>
@@ -66224,7 +66296,7 @@
         <v>21</v>
       </c>
       <c r="K998" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L998" s="6">
         <v>0</v>
@@ -66242,7 +66314,7 @@
         <v>2290</v>
       </c>
       <c r="Q998" s="6">
-        <v>0</v>
+        <v>-191.8</v>
       </c>
       <c r="R998" s="6" t="s">
         <v>23</v>
@@ -66301,7 +66373,7 @@
         <v>2293</v>
       </c>
       <c r="Q999" s="6">
-        <v>1056.5999999999999</v>
+        <v>548.13</v>
       </c>
       <c r="R999" s="6" t="s">
         <v>23</v>
@@ -66360,7 +66432,7 @@
         <v>2296</v>
       </c>
       <c r="Q1000" s="6">
-        <v>646.5</v>
+        <v>528.5</v>
       </c>
       <c r="R1000" s="6" t="s">
         <v>23</v>
@@ -66460,7 +66532,7 @@
         <v>21</v>
       </c>
       <c r="K1002" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1002" s="6">
         <v>0</v>
@@ -66478,7 +66550,7 @@
         <v>2302</v>
       </c>
       <c r="Q1002" s="6">
-        <v>0</v>
+        <v>315.5</v>
       </c>
       <c r="R1002" s="6" t="s">
         <v>23</v>
@@ -66489,16 +66561,16 @@
     </row>
     <row r="1003" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1003" s="5" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B1003" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1003" s="5" t="s">
         <v>2305</v>
       </c>
-      <c r="B1003" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1003" s="5" t="s">
+      <c r="D1003" s="5" t="s">
         <v>2306</v>
-      </c>
-      <c r="D1003" s="5" t="s">
-        <v>2307</v>
       </c>
       <c r="E1003" s="6" t="s">
         <v>23</v>
@@ -66534,7 +66606,7 @@
         <v>21</v>
       </c>
       <c r="P1003" s="5" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="Q1003" s="6">
         <v>0</v>
@@ -66548,16 +66620,16 @@
     </row>
     <row r="1004" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1004" s="5" t="s">
+        <v>2307</v>
+      </c>
+      <c r="B1004" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1004" s="5" t="s">
         <v>2308</v>
       </c>
-      <c r="B1004" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1004" s="5" t="s">
+      <c r="D1004" s="5" t="s">
         <v>2309</v>
-      </c>
-      <c r="D1004" s="5" t="s">
-        <v>2310</v>
       </c>
       <c r="E1004" s="6" t="s">
         <v>23</v>
@@ -66593,7 +66665,7 @@
         <v>21</v>
       </c>
       <c r="P1004" s="5" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="Q1004" s="6">
         <v>0</v>
@@ -66607,16 +66679,16 @@
     </row>
     <row r="1005" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1005" s="5" t="s">
-        <v>2165</v>
+        <v>2310</v>
       </c>
       <c r="B1005" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1005" s="5" t="s">
-        <v>2166</v>
+        <v>2311</v>
       </c>
       <c r="D1005" s="5" t="s">
-        <v>2167</v>
+        <v>2312</v>
       </c>
       <c r="E1005" s="6" t="s">
         <v>23</v>
@@ -66637,10 +66709,10 @@
         <v>21</v>
       </c>
       <c r="K1005" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L1005" s="6">
-        <v>1.98</v>
+        <v>0</v>
       </c>
       <c r="M1005" s="6">
         <v>0</v>
@@ -66652,10 +66724,10 @@
         <v>21</v>
       </c>
       <c r="P1005" s="5" t="s">
-        <v>2166</v>
+        <v>2311</v>
       </c>
       <c r="Q1005" s="6">
-        <v>589.70000000000005</v>
+        <v>0</v>
       </c>
       <c r="R1005" s="6" t="s">
         <v>23</v>
@@ -66666,16 +66738,16 @@
     </row>
     <row r="1006" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1006" s="5" t="s">
-        <v>2168</v>
+        <v>2313</v>
       </c>
       <c r="B1006" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1006" s="5" t="s">
-        <v>2169</v>
+        <v>2314</v>
       </c>
       <c r="D1006" s="5" t="s">
-        <v>2170</v>
+        <v>2315</v>
       </c>
       <c r="E1006" s="6" t="s">
         <v>23</v>
@@ -66696,10 +66768,10 @@
         <v>21</v>
       </c>
       <c r="K1006" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L1006" s="6">
-        <v>3.02</v>
+        <v>0</v>
       </c>
       <c r="M1006" s="6">
         <v>0</v>
@@ -66711,10 +66783,10 @@
         <v>21</v>
       </c>
       <c r="P1006" s="5" t="s">
-        <v>2169</v>
+        <v>2314</v>
       </c>
       <c r="Q1006" s="6">
-        <v>200.07</v>
+        <v>0</v>
       </c>
       <c r="R1006" s="6" t="s">
         <v>23</v>
@@ -66725,16 +66797,16 @@
     </row>
     <row r="1007" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1007" s="5" t="s">
-        <v>2171</v>
+        <v>2316</v>
       </c>
       <c r="B1007" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1007" s="5" t="s">
-        <v>2172</v>
+        <v>2317</v>
       </c>
       <c r="D1007" s="5" t="s">
-        <v>2173</v>
+        <v>2318</v>
       </c>
       <c r="E1007" s="6" t="s">
         <v>23</v>
@@ -66755,10 +66827,10 @@
         <v>21</v>
       </c>
       <c r="K1007" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L1007" s="6">
-        <v>2.65</v>
+        <v>0</v>
       </c>
       <c r="M1007" s="6">
         <v>0</v>
@@ -66770,10 +66842,10 @@
         <v>21</v>
       </c>
       <c r="P1007" s="5" t="s">
-        <v>2172</v>
+        <v>2317</v>
       </c>
       <c r="Q1007" s="6">
-        <v>1479.87</v>
+        <v>0</v>
       </c>
       <c r="R1007" s="6" t="s">
         <v>23</v>
@@ -66784,16 +66856,16 @@
     </row>
     <row r="1008" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1008" s="5" t="s">
-        <v>2189</v>
+        <v>2319</v>
       </c>
       <c r="B1008" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1008" s="5" t="s">
-        <v>2190</v>
+        <v>2320</v>
       </c>
       <c r="D1008" s="5" t="s">
-        <v>2191</v>
+        <v>2321</v>
       </c>
       <c r="E1008" s="6" t="s">
         <v>23</v>
@@ -66829,7 +66901,7 @@
         <v>21</v>
       </c>
       <c r="P1008" s="5" t="s">
-        <v>2190</v>
+        <v>2320</v>
       </c>
       <c r="Q1008" s="6">
         <v>0</v>
@@ -66843,16 +66915,16 @@
     </row>
     <row r="1009" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1009" s="5" t="s">
-        <v>2192</v>
+        <v>2329</v>
       </c>
       <c r="B1009" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1009" s="5" t="s">
-        <v>2193</v>
+        <v>2330</v>
       </c>
       <c r="D1009" s="5" t="s">
-        <v>2194</v>
+        <v>2331</v>
       </c>
       <c r="E1009" s="6" t="s">
         <v>23</v>
@@ -66888,15 +66960,487 @@
         <v>21</v>
       </c>
       <c r="P1009" s="5" t="s">
+        <v>2330</v>
+      </c>
+      <c r="Q1009" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1009" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1009" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1010" s="5" t="s">
+        <v>2332</v>
+      </c>
+      <c r="B1010" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1010" s="5" t="s">
+        <v>2333</v>
+      </c>
+      <c r="D1010" s="5" t="s">
+        <v>2334</v>
+      </c>
+      <c r="E1010" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1010" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1010" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1010" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1010" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1010" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1010" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1010" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1010" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1010" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1010" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1010" s="5" t="s">
+        <v>2333</v>
+      </c>
+      <c r="Q1010" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1010" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1010" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1011" s="5" t="s">
+        <v>2165</v>
+      </c>
+      <c r="B1011" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1011" s="5" t="s">
+        <v>2166</v>
+      </c>
+      <c r="D1011" s="5" t="s">
+        <v>2167</v>
+      </c>
+      <c r="E1011" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1011" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1011" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1011" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1011" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1011" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1011" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1011" s="6">
+        <v>1.98</v>
+      </c>
+      <c r="M1011" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1011" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1011" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1011" s="5" t="s">
+        <v>2166</v>
+      </c>
+      <c r="Q1011" s="6">
+        <v>589.70000000000005</v>
+      </c>
+      <c r="R1011" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1011" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1012" s="5" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B1012" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1012" s="5" t="s">
+        <v>2169</v>
+      </c>
+      <c r="D1012" s="5" t="s">
+        <v>2170</v>
+      </c>
+      <c r="E1012" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1012" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1012" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1012" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1012" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1012" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1012" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1012" s="6">
+        <v>3.02</v>
+      </c>
+      <c r="M1012" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1012" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1012" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1012" s="5" t="s">
+        <v>2169</v>
+      </c>
+      <c r="Q1012" s="6">
+        <v>200.07</v>
+      </c>
+      <c r="R1012" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1012" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1013" s="5" t="s">
+        <v>2171</v>
+      </c>
+      <c r="B1013" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1013" s="5" t="s">
+        <v>2172</v>
+      </c>
+      <c r="D1013" s="5" t="s">
+        <v>2173</v>
+      </c>
+      <c r="E1013" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1013" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1013" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1013" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1013" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1013" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1013" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1013" s="6">
+        <v>2.65</v>
+      </c>
+      <c r="M1013" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1013" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1013" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1013" s="5" t="s">
+        <v>2172</v>
+      </c>
+      <c r="Q1013" s="6">
+        <v>1106.52</v>
+      </c>
+      <c r="R1013" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1013" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1014" s="5" t="s">
+        <v>2189</v>
+      </c>
+      <c r="B1014" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1014" s="5" t="s">
+        <v>2190</v>
+      </c>
+      <c r="D1014" s="5" t="s">
+        <v>2191</v>
+      </c>
+      <c r="E1014" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1014" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1014" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1014" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1014" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1014" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1014" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1014" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1014" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1014" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1014" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1014" s="5" t="s">
+        <v>2190</v>
+      </c>
+      <c r="Q1014" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1014" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1014" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1015" s="5" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B1015" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1015" s="5" t="s">
         <v>2193</v>
       </c>
-      <c r="Q1009" s="6">
-        <v>0</v>
-      </c>
-      <c r="R1009" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1009" s="5" t="s">
+      <c r="D1015" s="5" t="s">
+        <v>2194</v>
+      </c>
+      <c r="E1015" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1015" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1015" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1015" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1015" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1015" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1015" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1015" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1015" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1015" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1015" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1015" s="5" t="s">
+        <v>2193</v>
+      </c>
+      <c r="Q1015" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1015" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1015" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1016" s="5" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B1016" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1016" s="5" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D1016" s="5" t="s">
+        <v>2324</v>
+      </c>
+      <c r="E1016" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1016" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1016" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1016" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1016" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1016" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1016" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1016" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1016" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1016" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1016" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1016" s="5" t="s">
+        <v>2323</v>
+      </c>
+      <c r="Q1016" s="6">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="R1016" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1016" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1017" s="5" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B1017" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1017" s="5" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D1017" s="5" t="s">
+        <v>2327</v>
+      </c>
+      <c r="E1017" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1017" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1017" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1017" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1017" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1017" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1017" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1017" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1017" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1017" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1017" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1017" s="5" t="s">
+        <v>2326</v>
+      </c>
+      <c r="Q1017" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1017" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1017" s="5" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix color mode in !size command (adobe rgb to sRGB)
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/TC_02.xlsx
+++ b/EXCEL LIBS/TC_02.xlsx
@@ -7090,9 +7090,6 @@
     <t>MONET 31 (VERDE)</t>
   </si>
   <si>
-    <t>Lista Produto : 17-06-2020 09:18:00</t>
-  </si>
-  <si>
     <t>TC16008</t>
   </si>
   <si>
@@ -7100,6 +7097,9 @@
   </si>
   <si>
     <t>MACAU - SAND (BEJE)</t>
+  </si>
+  <si>
+    <t>Lista Produto : 18-06-2020 10:15:32</t>
   </si>
 </sst>
 </file>
@@ -7610,7 +7610,7 @@
     </row>
     <row r="2" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2355</v>
+        <v>2358</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -28213,7 +28213,7 @@
         <v>738</v>
       </c>
       <c r="Q351" s="6">
-        <v>27990.73</v>
+        <v>26532.03</v>
       </c>
       <c r="R351" s="6" t="s">
         <v>23</v>
@@ -54114,7 +54114,7 @@
         <v>1655</v>
       </c>
       <c r="Q790" s="6">
-        <v>6527.88</v>
+        <v>9169.68</v>
       </c>
       <c r="R790" s="6" t="s">
         <v>23</v>
@@ -54409,7 +54409,7 @@
         <v>1665</v>
       </c>
       <c r="Q795" s="6">
-        <v>15922.8</v>
+        <v>15232.6</v>
       </c>
       <c r="R795" s="6" t="s">
         <v>23</v>
@@ -54704,7 +54704,7 @@
         <v>1675</v>
       </c>
       <c r="Q800" s="6">
-        <v>4614.66</v>
+        <v>7308.76</v>
       </c>
       <c r="R800" s="6" t="s">
         <v>23</v>
@@ -54881,7 +54881,7 @@
         <v>1681</v>
       </c>
       <c r="Q803" s="6">
-        <v>6290.9</v>
+        <v>6280.5</v>
       </c>
       <c r="R803" s="6" t="s">
         <v>23</v>
@@ -56238,7 +56238,7 @@
         <v>1744</v>
       </c>
       <c r="Q826" s="6">
-        <v>655.6</v>
+        <v>643.4</v>
       </c>
       <c r="R826" s="6" t="s">
         <v>23</v>
@@ -56592,7 +56592,7 @@
         <v>1762</v>
       </c>
       <c r="Q832" s="6">
-        <v>12544.54</v>
+        <v>12534.95</v>
       </c>
       <c r="R832" s="6" t="s">
         <v>23</v>
@@ -58421,7 +58421,7 @@
         <v>1861</v>
       </c>
       <c r="Q863" s="6">
-        <v>1458.2</v>
+        <v>1390.99</v>
       </c>
       <c r="R863" s="6" t="s">
         <v>23</v>
@@ -58539,7 +58539,7 @@
         <v>1868</v>
       </c>
       <c r="Q865" s="6">
-        <v>752.44</v>
+        <v>501.93</v>
       </c>
       <c r="R865" s="6" t="s">
         <v>23</v>
@@ -63141,7 +63141,7 @@
         <v>2104</v>
       </c>
       <c r="Q943" s="6">
-        <v>2131.35</v>
+        <v>3163.55</v>
       </c>
       <c r="R943" s="6" t="s">
         <v>23</v>
@@ -65796,7 +65796,7 @@
         <v>2257</v>
       </c>
       <c r="Q988" s="6">
-        <v>7032.3</v>
+        <v>10074.6</v>
       </c>
       <c r="R988" s="6" t="s">
         <v>23</v>
@@ -66327,7 +66327,7 @@
         <v>2287</v>
       </c>
       <c r="Q997" s="6">
-        <v>74521.094200000007</v>
+        <v>71772.704199999993</v>
       </c>
       <c r="R997" s="6" t="s">
         <v>23</v>
@@ -66504,7 +66504,7 @@
         <v>2296</v>
       </c>
       <c r="Q1000" s="6">
-        <v>500.02</v>
+        <v>447.82</v>
       </c>
       <c r="R1000" s="6" t="s">
         <v>23</v>
@@ -67625,7 +67625,7 @@
         <v>2169</v>
       </c>
       <c r="Q1019" s="6">
-        <v>148.1</v>
+        <v>399.3</v>
       </c>
       <c r="R1019" s="6" t="s">
         <v>23</v>
@@ -67931,16 +67931,16 @@
     </row>
     <row r="1025" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1025" s="5" t="s">
+        <v>2355</v>
+      </c>
+      <c r="B1025" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1025" s="5" t="s">
         <v>2356</v>
       </c>
-      <c r="B1025" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1025" s="5" t="s">
+      <c r="D1025" s="5" t="s">
         <v>2357</v>
-      </c>
-      <c r="D1025" s="5" t="s">
-        <v>2358</v>
       </c>
       <c r="E1025" s="6" t="s">
         <v>23</v>
@@ -67976,7 +67976,7 @@
         <v>21</v>
       </c>
       <c r="P1025" s="5" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="Q1025" s="6">
         <v>36.200000000000003</v>

</xml_diff>

<commit_message>
act excell and controlers
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/TC_02.xlsx
+++ b/EXCEL LIBS/TC_02.xlsx
@@ -7156,7 +7156,7 @@
     <t>GOMERA 16 (BLACK)</t>
   </si>
   <si>
-    <t>Lista Produto : 30-07-2020 09:21:11</t>
+    <t>Lista Produto : 03-08-2020 09:32:46</t>
   </si>
 </sst>
 </file>
@@ -17827,7 +17827,7 @@
         <v>368</v>
       </c>
       <c r="Q174" s="6">
-        <v>2289</v>
+        <v>1545</v>
       </c>
       <c r="R174" s="6" t="s">
         <v>23</v>
@@ -19774,7 +19774,7 @@
         <v>434</v>
       </c>
       <c r="Q207" s="6">
-        <v>3589.72</v>
+        <v>3568.4</v>
       </c>
       <c r="R207" s="6" t="s">
         <v>23</v>
@@ -20659,7 +20659,7 @@
         <v>464</v>
       </c>
       <c r="Q222" s="6">
-        <v>1320.69</v>
+        <v>2608.4699999999998</v>
       </c>
       <c r="R222" s="6" t="s">
         <v>23</v>
@@ -21780,7 +21780,7 @@
         <v>502</v>
       </c>
       <c r="Q241" s="6">
-        <v>3135.77</v>
+        <v>3127.22</v>
       </c>
       <c r="R241" s="6" t="s">
         <v>23</v>
@@ -21898,7 +21898,7 @@
         <v>506</v>
       </c>
       <c r="Q243" s="6">
-        <v>613.83000000000004</v>
+        <v>597.27</v>
       </c>
       <c r="R243" s="6" t="s">
         <v>23</v>
@@ -24494,7 +24494,7 @@
         <v>595</v>
       </c>
       <c r="Q287" s="6">
-        <v>1927.68</v>
+        <v>1884.21</v>
       </c>
       <c r="R287" s="6" t="s">
         <v>23</v>
@@ -25261,7 +25261,7 @@
         <v>621</v>
       </c>
       <c r="Q300" s="6">
-        <v>1070.33</v>
+        <v>657.75</v>
       </c>
       <c r="R300" s="6" t="s">
         <v>23</v>
@@ -26323,7 +26323,7 @@
         <v>662</v>
       </c>
       <c r="Q318" s="6">
-        <v>2042.9</v>
+        <v>2023.76</v>
       </c>
       <c r="R318" s="6" t="s">
         <v>23</v>
@@ -26382,7 +26382,7 @@
         <v>664</v>
       </c>
       <c r="Q319" s="6">
-        <v>8025.22</v>
+        <v>8009.2</v>
       </c>
       <c r="R319" s="6" t="s">
         <v>23</v>
@@ -26441,7 +26441,7 @@
         <v>666</v>
       </c>
       <c r="Q320" s="6">
-        <v>3638.7</v>
+        <v>3629.13</v>
       </c>
       <c r="R320" s="6" t="s">
         <v>23</v>
@@ -26500,7 +26500,7 @@
         <v>668</v>
       </c>
       <c r="Q321" s="6">
-        <v>5639.86</v>
+        <v>5614.27</v>
       </c>
       <c r="R321" s="6" t="s">
         <v>23</v>
@@ -27090,7 +27090,7 @@
         <v>692</v>
       </c>
       <c r="Q331" s="6">
-        <v>2773.97</v>
+        <v>2746.52</v>
       </c>
       <c r="R331" s="6" t="s">
         <v>23</v>
@@ -27385,7 +27385,7 @@
         <v>706</v>
       </c>
       <c r="Q336" s="6">
-        <v>1850.94</v>
+        <v>1833.74</v>
       </c>
       <c r="R336" s="6" t="s">
         <v>23</v>
@@ -28152,7 +28152,7 @@
         <v>734</v>
       </c>
       <c r="Q349" s="6">
-        <v>258.64999999999998</v>
+        <v>722.35</v>
       </c>
       <c r="R349" s="6" t="s">
         <v>23</v>
@@ -28270,7 +28270,7 @@
         <v>738</v>
       </c>
       <c r="Q351" s="6">
-        <v>22759.97</v>
+        <v>21004.720000000001</v>
       </c>
       <c r="R351" s="6" t="s">
         <v>23</v>
@@ -29332,7 +29332,7 @@
         <v>787</v>
       </c>
       <c r="Q369" s="6">
-        <v>68</v>
+        <v>128.30000000000001</v>
       </c>
       <c r="R369" s="6" t="s">
         <v>23</v>
@@ -29627,7 +29627,7 @@
         <v>2360</v>
       </c>
       <c r="Q374" s="6">
-        <v>4995.8500000000004</v>
+        <v>4478.3900000000003</v>
       </c>
       <c r="R374" s="6" t="s">
         <v>23</v>
@@ -54525,7 +54525,7 @@
         <v>1665</v>
       </c>
       <c r="Q796" s="6">
-        <v>10891.77</v>
+        <v>10763.77</v>
       </c>
       <c r="R796" s="6" t="s">
         <v>23</v>
@@ -54820,7 +54820,7 @@
         <v>1675</v>
       </c>
       <c r="Q801" s="6">
-        <v>2574.9</v>
+        <v>1940.1</v>
       </c>
       <c r="R801" s="6" t="s">
         <v>23</v>
@@ -54997,7 +54997,7 @@
         <v>1681</v>
       </c>
       <c r="Q804" s="6">
-        <v>1782.79</v>
+        <v>507.2</v>
       </c>
       <c r="R804" s="6" t="s">
         <v>23</v>
@@ -55115,7 +55115,7 @@
         <v>1687</v>
       </c>
       <c r="Q806" s="6">
-        <v>2273.61</v>
+        <v>2261.02</v>
       </c>
       <c r="R806" s="6" t="s">
         <v>23</v>
@@ -56413,7 +56413,7 @@
         <v>1747</v>
       </c>
       <c r="Q828" s="6">
-        <v>649.79999999999995</v>
+        <v>529.6</v>
       </c>
       <c r="R828" s="6" t="s">
         <v>23</v>
@@ -56472,7 +56472,7 @@
         <v>1750</v>
       </c>
       <c r="Q829" s="6">
-        <v>3196.5</v>
+        <v>3136.4</v>
       </c>
       <c r="R829" s="6" t="s">
         <v>23</v>
@@ -56708,7 +56708,7 @@
         <v>1762</v>
       </c>
       <c r="Q833" s="6">
-        <v>10483</v>
+        <v>10470.83</v>
       </c>
       <c r="R833" s="6" t="s">
         <v>23</v>
@@ -56767,7 +56767,7 @@
         <v>1765</v>
       </c>
       <c r="Q834" s="6">
-        <v>4592.6000000000004</v>
+        <v>4472.3999999999996</v>
       </c>
       <c r="R834" s="6" t="s">
         <v>23</v>
@@ -56826,7 +56826,7 @@
         <v>1768</v>
       </c>
       <c r="Q835" s="6">
-        <v>5053.3</v>
+        <v>4993.2</v>
       </c>
       <c r="R835" s="6" t="s">
         <v>23</v>
@@ -57003,7 +57003,7 @@
         <v>1777</v>
       </c>
       <c r="Q838" s="6">
-        <v>504.5</v>
+        <v>466.46</v>
       </c>
       <c r="R838" s="6" t="s">
         <v>23</v>
@@ -59068,7 +59068,7 @@
         <v>1889</v>
       </c>
       <c r="Q873" s="6">
-        <v>382.92</v>
+        <v>326.51</v>
       </c>
       <c r="R873" s="6" t="s">
         <v>23</v>
@@ -59127,7 +59127,7 @@
         <v>1892</v>
       </c>
       <c r="Q874" s="6">
-        <v>452.87</v>
+        <v>331.21</v>
       </c>
       <c r="R874" s="6" t="s">
         <v>23</v>
@@ -59186,7 +59186,7 @@
         <v>1895</v>
       </c>
       <c r="Q875" s="6">
-        <v>415.58</v>
+        <v>403.43</v>
       </c>
       <c r="R875" s="6" t="s">
         <v>23</v>
@@ -61959,7 +61959,7 @@
         <v>2038</v>
       </c>
       <c r="Q922" s="6">
-        <v>638.22</v>
+        <v>249.15</v>
       </c>
       <c r="R922" s="6" t="s">
         <v>23</v>
@@ -62018,7 +62018,7 @@
         <v>2041</v>
       </c>
       <c r="Q923" s="6">
-        <v>554.58000000000004</v>
+        <v>524.87</v>
       </c>
       <c r="R923" s="6" t="s">
         <v>23</v>
@@ -63375,7 +63375,7 @@
         <v>2110</v>
       </c>
       <c r="Q946" s="6">
-        <v>2107.17</v>
+        <v>212.67</v>
       </c>
       <c r="R946" s="6" t="s">
         <v>23</v>
@@ -66207,7 +66207,7 @@
         <v>2275</v>
       </c>
       <c r="Q994" s="6">
-        <v>2580.25</v>
+        <v>2231.16</v>
       </c>
       <c r="R994" s="6" t="s">
         <v>23</v>
@@ -66384,7 +66384,7 @@
         <v>2284</v>
       </c>
       <c r="Q997" s="6">
-        <v>31669.25</v>
+        <v>30582.06</v>
       </c>
       <c r="R997" s="6" t="s">
         <v>23</v>
@@ -66443,7 +66443,7 @@
         <v>2287</v>
       </c>
       <c r="Q998" s="6">
-        <v>43992.325969999998</v>
+        <v>41981.15597</v>
       </c>
       <c r="R998" s="6" t="s">
         <v>23</v>
@@ -66679,7 +66679,7 @@
         <v>2299</v>
       </c>
       <c r="Q1002" s="6">
-        <v>3049.5</v>
+        <v>3032.72</v>
       </c>
       <c r="R1002" s="6" t="s">
         <v>23</v>
@@ -66738,7 +66738,7 @@
         <v>2302</v>
       </c>
       <c r="Q1003" s="6">
-        <v>14226.04</v>
+        <v>10974.02</v>
       </c>
       <c r="R1003" s="6" t="s">
         <v>23</v>
@@ -67546,7 +67546,7 @@
         <v>21</v>
       </c>
       <c r="K1017" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1017" s="6">
         <v>0</v>
@@ -67564,7 +67564,7 @@
         <v>2350</v>
       </c>
       <c r="Q1017" s="6">
-        <v>0</v>
+        <v>310.60000000000002</v>
       </c>
       <c r="R1017" s="6" t="s">
         <v>23</v>
@@ -67605,7 +67605,7 @@
         <v>21</v>
       </c>
       <c r="K1018" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1018" s="6">
         <v>0</v>
@@ -67623,7 +67623,7 @@
         <v>2352</v>
       </c>
       <c r="Q1018" s="6">
-        <v>0</v>
+        <v>404.4</v>
       </c>
       <c r="R1018" s="6" t="s">
         <v>23</v>
@@ -67664,7 +67664,7 @@
         <v>21</v>
       </c>
       <c r="K1019" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1019" s="6">
         <v>0</v>
@@ -67682,7 +67682,7 @@
         <v>2363</v>
       </c>
       <c r="Q1019" s="6">
-        <v>0</v>
+        <v>42.38</v>
       </c>
       <c r="R1019" s="6" t="s">
         <v>23</v>
@@ -67723,7 +67723,7 @@
         <v>21</v>
       </c>
       <c r="K1020" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1020" s="6">
         <v>0</v>
@@ -67741,7 +67741,7 @@
         <v>2366</v>
       </c>
       <c r="Q1020" s="6">
-        <v>0</v>
+        <v>11.54</v>
       </c>
       <c r="R1020" s="6" t="s">
         <v>23</v>
@@ -67782,7 +67782,7 @@
         <v>21</v>
       </c>
       <c r="K1021" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1021" s="6">
         <v>0</v>
@@ -67800,7 +67800,7 @@
         <v>2369</v>
       </c>
       <c r="Q1021" s="6">
-        <v>0</v>
+        <v>44.1</v>
       </c>
       <c r="R1021" s="6" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
act logs and excel files
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/TC_02.xlsx
+++ b/EXCEL LIBS/TC_02.xlsx
@@ -7156,7 +7156,7 @@
     <t>GOMERA 16 (BLACK)</t>
   </si>
   <si>
-    <t>Lista Produto : 03-08-2020 09:32:46</t>
+    <t>Lista Produto : 10-08-2020 17:04:14</t>
   </si>
 </sst>
 </file>
@@ -18063,7 +18063,7 @@
         <v>376</v>
       </c>
       <c r="Q178" s="6">
-        <v>142.49</v>
+        <v>1024.49</v>
       </c>
       <c r="R178" s="6" t="s">
         <v>23</v>
@@ -18107,7 +18107,7 @@
         <v>23</v>
       </c>
       <c r="L179" s="6">
-        <v>2.67</v>
+        <v>2.69</v>
       </c>
       <c r="M179" s="6">
         <v>0</v>
@@ -18122,7 +18122,7 @@
         <v>378</v>
       </c>
       <c r="Q179" s="6">
-        <v>84.21</v>
+        <v>1000.86</v>
       </c>
       <c r="R179" s="6" t="s">
         <v>23</v>
@@ -18594,7 +18594,7 @@
         <v>394</v>
       </c>
       <c r="Q187" s="6">
-        <v>4685.07</v>
+        <v>3084.57</v>
       </c>
       <c r="R187" s="6" t="s">
         <v>23</v>
@@ -18948,7 +18948,7 @@
         <v>406</v>
       </c>
       <c r="Q193" s="6">
-        <v>701</v>
+        <v>449</v>
       </c>
       <c r="R193" s="6" t="s">
         <v>23</v>
@@ -19715,7 +19715,7 @@
         <v>432</v>
       </c>
       <c r="Q206" s="6">
-        <v>1719.2</v>
+        <v>1601.3</v>
       </c>
       <c r="R206" s="6" t="s">
         <v>23</v>
@@ -20659,7 +20659,7 @@
         <v>464</v>
       </c>
       <c r="Q222" s="6">
-        <v>2608.4699999999998</v>
+        <v>2319.13</v>
       </c>
       <c r="R222" s="6" t="s">
         <v>23</v>
@@ -20718,7 +20718,7 @@
         <v>466</v>
       </c>
       <c r="Q223" s="6">
-        <v>137.99</v>
+        <v>310.47000000000003</v>
       </c>
       <c r="R223" s="6" t="s">
         <v>23</v>
@@ -20998,7 +20998,7 @@
         <v>23</v>
       </c>
       <c r="L228" s="6">
-        <v>2.75</v>
+        <v>3.3</v>
       </c>
       <c r="M228" s="6">
         <v>0</v>
@@ -21013,7 +21013,7 @@
         <v>476</v>
       </c>
       <c r="Q228" s="6">
-        <v>90.85</v>
+        <v>279</v>
       </c>
       <c r="R228" s="6" t="s">
         <v>23</v>
@@ -21780,7 +21780,7 @@
         <v>502</v>
       </c>
       <c r="Q241" s="6">
-        <v>3127.22</v>
+        <v>3097.36</v>
       </c>
       <c r="R241" s="6" t="s">
         <v>23</v>
@@ -24376,7 +24376,7 @@
         <v>591</v>
       </c>
       <c r="Q285" s="6">
-        <v>841.24</v>
+        <v>703.57</v>
       </c>
       <c r="R285" s="6" t="s">
         <v>23</v>
@@ -24553,7 +24553,7 @@
         <v>597</v>
       </c>
       <c r="Q288" s="6">
-        <v>582.52</v>
+        <v>559.24</v>
       </c>
       <c r="R288" s="6" t="s">
         <v>23</v>
@@ -24671,7 +24671,7 @@
         <v>601</v>
       </c>
       <c r="Q290" s="6">
-        <v>610.70000000000005</v>
+        <v>518.27</v>
       </c>
       <c r="R290" s="6" t="s">
         <v>23</v>
@@ -24730,7 +24730,7 @@
         <v>603</v>
       </c>
       <c r="Q291" s="6">
-        <v>1675.09</v>
+        <v>1664.95</v>
       </c>
       <c r="R291" s="6" t="s">
         <v>23</v>
@@ -25025,7 +25025,7 @@
         <v>613</v>
       </c>
       <c r="Q296" s="6">
-        <v>1214.79</v>
+        <v>1208.22</v>
       </c>
       <c r="R296" s="6" t="s">
         <v>23</v>
@@ -25143,7 +25143,7 @@
         <v>617</v>
       </c>
       <c r="Q298" s="6">
-        <v>149.03</v>
+        <v>147.63</v>
       </c>
       <c r="R298" s="6" t="s">
         <v>23</v>
@@ -25261,7 +25261,7 @@
         <v>621</v>
       </c>
       <c r="Q300" s="6">
-        <v>657.75</v>
+        <v>1049.83</v>
       </c>
       <c r="R300" s="6" t="s">
         <v>23</v>
@@ -25438,7 +25438,7 @@
         <v>627</v>
       </c>
       <c r="Q303" s="6">
-        <v>3074.43</v>
+        <v>3052.73</v>
       </c>
       <c r="R303" s="6" t="s">
         <v>23</v>
@@ -25497,7 +25497,7 @@
         <v>629</v>
       </c>
       <c r="Q304" s="6">
-        <v>1122.1300000000001</v>
+        <v>1091.33</v>
       </c>
       <c r="R304" s="6" t="s">
         <v>23</v>
@@ -25851,7 +25851,7 @@
         <v>641</v>
       </c>
       <c r="Q310" s="6">
-        <v>2060.1</v>
+        <v>1612.8</v>
       </c>
       <c r="R310" s="6" t="s">
         <v>23</v>
@@ -26028,7 +26028,7 @@
         <v>649</v>
       </c>
       <c r="Q313" s="6">
-        <v>211.4</v>
+        <v>197.5</v>
       </c>
       <c r="R313" s="6" t="s">
         <v>23</v>
@@ -26264,7 +26264,7 @@
         <v>660</v>
       </c>
       <c r="Q317" s="6">
-        <v>8680.48</v>
+        <v>8664.98</v>
       </c>
       <c r="R317" s="6" t="s">
         <v>23</v>
@@ -26382,7 +26382,7 @@
         <v>664</v>
       </c>
       <c r="Q319" s="6">
-        <v>8009.2</v>
+        <v>8005.9</v>
       </c>
       <c r="R319" s="6" t="s">
         <v>23</v>
@@ -26441,7 +26441,7 @@
         <v>666</v>
       </c>
       <c r="Q320" s="6">
-        <v>3629.13</v>
+        <v>3586.21</v>
       </c>
       <c r="R320" s="6" t="s">
         <v>23</v>
@@ -26500,7 +26500,7 @@
         <v>668</v>
       </c>
       <c r="Q321" s="6">
-        <v>5614.27</v>
+        <v>5952.56</v>
       </c>
       <c r="R321" s="6" t="s">
         <v>23</v>
@@ -26559,7 +26559,7 @@
         <v>670</v>
       </c>
       <c r="Q322" s="6">
-        <v>1373.65</v>
+        <v>1076.95</v>
       </c>
       <c r="R322" s="6" t="s">
         <v>23</v>
@@ -26677,7 +26677,7 @@
         <v>674</v>
       </c>
       <c r="Q324" s="6">
-        <v>2107.9499999999998</v>
+        <v>2076.85</v>
       </c>
       <c r="R324" s="6" t="s">
         <v>23</v>
@@ -26854,7 +26854,7 @@
         <v>680</v>
       </c>
       <c r="Q327" s="6">
-        <v>200.28</v>
+        <v>93.48</v>
       </c>
       <c r="R327" s="6" t="s">
         <v>23</v>
@@ -26913,7 +26913,7 @@
         <v>683</v>
       </c>
       <c r="Q328" s="6">
-        <v>1858.4</v>
+        <v>1847.12</v>
       </c>
       <c r="R328" s="6" t="s">
         <v>23</v>
@@ -27149,7 +27149,7 @@
         <v>694</v>
       </c>
       <c r="Q332" s="6">
-        <v>1656.3</v>
+        <v>1652.4</v>
       </c>
       <c r="R332" s="6" t="s">
         <v>23</v>
@@ -27385,7 +27385,7 @@
         <v>706</v>
       </c>
       <c r="Q336" s="6">
-        <v>1833.74</v>
+        <v>1830.37</v>
       </c>
       <c r="R336" s="6" t="s">
         <v>23</v>
@@ -27798,7 +27798,7 @@
         <v>720</v>
       </c>
       <c r="Q343" s="6">
-        <v>394.19</v>
+        <v>287.39</v>
       </c>
       <c r="R343" s="6" t="s">
         <v>23</v>
@@ -27916,7 +27916,7 @@
         <v>724</v>
       </c>
       <c r="Q345" s="6">
-        <v>1847.3</v>
+        <v>577.46</v>
       </c>
       <c r="R345" s="6" t="s">
         <v>23</v>
@@ -27975,7 +27975,7 @@
         <v>726</v>
       </c>
       <c r="Q346" s="6">
-        <v>37.880000000000003</v>
+        <v>342.28</v>
       </c>
       <c r="R346" s="6" t="s">
         <v>23</v>
@@ -28093,7 +28093,7 @@
         <v>731</v>
       </c>
       <c r="Q348" s="6">
-        <v>1046.73</v>
+        <v>1036.48</v>
       </c>
       <c r="R348" s="6" t="s">
         <v>23</v>
@@ -28270,7 +28270,7 @@
         <v>738</v>
       </c>
       <c r="Q351" s="6">
-        <v>21004.720000000001</v>
+        <v>16762.03</v>
       </c>
       <c r="R351" s="6" t="s">
         <v>23</v>
@@ -28447,7 +28447,7 @@
         <v>747</v>
       </c>
       <c r="Q354" s="6">
-        <v>92.37</v>
+        <v>90.07</v>
       </c>
       <c r="R354" s="6" t="s">
         <v>23</v>
@@ -28801,7 +28801,7 @@
         <v>759</v>
       </c>
       <c r="Q360" s="6">
-        <v>1505</v>
+        <v>1499.33</v>
       </c>
       <c r="R360" s="6" t="s">
         <v>23</v>
@@ -29627,7 +29627,7 @@
         <v>2360</v>
       </c>
       <c r="Q374" s="6">
-        <v>4478.3900000000003</v>
+        <v>2776.7</v>
       </c>
       <c r="R374" s="6" t="s">
         <v>23</v>
@@ -51457,7 +51457,7 @@
         <v>1546</v>
       </c>
       <c r="Q744" s="6">
-        <v>342.2</v>
+        <v>330.32</v>
       </c>
       <c r="R744" s="6" t="s">
         <v>23</v>
@@ -54230,7 +54230,7 @@
         <v>1655</v>
       </c>
       <c r="Q791" s="6">
-        <v>10891.73</v>
+        <v>8857.73</v>
       </c>
       <c r="R791" s="6" t="s">
         <v>23</v>
@@ -54525,7 +54525,7 @@
         <v>1665</v>
       </c>
       <c r="Q796" s="6">
-        <v>10763.77</v>
+        <v>8575.27</v>
       </c>
       <c r="R796" s="6" t="s">
         <v>23</v>
@@ -54820,7 +54820,7 @@
         <v>1675</v>
       </c>
       <c r="Q801" s="6">
-        <v>1940.1</v>
+        <v>1337.3</v>
       </c>
       <c r="R801" s="6" t="s">
         <v>23</v>
@@ -54997,7 +54997,7 @@
         <v>1681</v>
       </c>
       <c r="Q804" s="6">
-        <v>507.2</v>
+        <v>5570.63</v>
       </c>
       <c r="R804" s="6" t="s">
         <v>23</v>
@@ -55100,7 +55100,7 @@
         <v>23</v>
       </c>
       <c r="L806" s="6">
-        <v>3.67</v>
+        <v>3.83</v>
       </c>
       <c r="M806" s="6">
         <v>0</v>
@@ -55115,7 +55115,7 @@
         <v>1687</v>
       </c>
       <c r="Q806" s="6">
-        <v>2261.02</v>
+        <v>353.89</v>
       </c>
       <c r="R806" s="6" t="s">
         <v>23</v>
@@ -55159,7 +55159,7 @@
         <v>23</v>
       </c>
       <c r="L807" s="6">
-        <v>3.43</v>
+        <v>3.45</v>
       </c>
       <c r="M807" s="6">
         <v>0</v>
@@ -55174,7 +55174,7 @@
         <v>1690</v>
       </c>
       <c r="Q807" s="6">
-        <v>171.6</v>
+        <v>1171.5999999999999</v>
       </c>
       <c r="R807" s="6" t="s">
         <v>23</v>
@@ -55233,7 +55233,7 @@
         <v>1693</v>
       </c>
       <c r="Q808" s="6">
-        <v>1716.92</v>
+        <v>1310.1199999999999</v>
       </c>
       <c r="R808" s="6" t="s">
         <v>23</v>
@@ -56177,7 +56177,7 @@
         <v>1735</v>
       </c>
       <c r="Q824" s="6">
-        <v>1714.73</v>
+        <v>4516.43</v>
       </c>
       <c r="R824" s="6" t="s">
         <v>23</v>
@@ -56649,7 +56649,7 @@
         <v>1758</v>
       </c>
       <c r="Q832" s="6">
-        <v>2669.85</v>
+        <v>1623.75</v>
       </c>
       <c r="R832" s="6" t="s">
         <v>23</v>
@@ -56708,7 +56708,7 @@
         <v>1762</v>
       </c>
       <c r="Q833" s="6">
-        <v>10470.83</v>
+        <v>8568.83</v>
       </c>
       <c r="R833" s="6" t="s">
         <v>23</v>
@@ -57357,7 +57357,7 @@
         <v>1800</v>
       </c>
       <c r="Q844" s="6">
-        <v>49.13</v>
+        <v>2071.5300000000002</v>
       </c>
       <c r="R844" s="6" t="s">
         <v>23</v>
@@ -58360,7 +58360,7 @@
         <v>1852</v>
       </c>
       <c r="Q861" s="6">
-        <v>356.33</v>
+        <v>336.89</v>
       </c>
       <c r="R861" s="6" t="s">
         <v>23</v>
@@ -58537,7 +58537,7 @@
         <v>1861</v>
       </c>
       <c r="Q864" s="6">
-        <v>1160.77</v>
+        <v>811.93</v>
       </c>
       <c r="R864" s="6" t="s">
         <v>23</v>
@@ -58655,7 +58655,7 @@
         <v>1868</v>
       </c>
       <c r="Q866" s="6">
-        <v>40.03</v>
+        <v>24.64</v>
       </c>
       <c r="R866" s="6" t="s">
         <v>23</v>
@@ -59068,7 +59068,7 @@
         <v>1889</v>
       </c>
       <c r="Q873" s="6">
-        <v>326.51</v>
+        <v>317.67</v>
       </c>
       <c r="R873" s="6" t="s">
         <v>23</v>
@@ -59112,7 +59112,7 @@
         <v>23</v>
       </c>
       <c r="L874" s="6">
-        <v>2.4500000000000002</v>
+        <v>2.58</v>
       </c>
       <c r="M874" s="6">
         <v>0</v>
@@ -59127,7 +59127,7 @@
         <v>1892</v>
       </c>
       <c r="Q874" s="6">
-        <v>331.21</v>
+        <v>318.66000000000003</v>
       </c>
       <c r="R874" s="6" t="s">
         <v>23</v>
@@ -59540,7 +59540,7 @@
         <v>1913</v>
       </c>
       <c r="Q881" s="6">
-        <v>1445</v>
+        <v>1880.3</v>
       </c>
       <c r="R881" s="6" t="s">
         <v>23</v>
@@ -59776,7 +59776,7 @@
         <v>1925</v>
       </c>
       <c r="Q885" s="6">
-        <v>3442.89</v>
+        <v>3037.72</v>
       </c>
       <c r="R885" s="6" t="s">
         <v>23</v>
@@ -60012,7 +60012,7 @@
         <v>1938</v>
       </c>
       <c r="Q889" s="6">
-        <v>52.81</v>
+        <v>42.13</v>
       </c>
       <c r="R889" s="6" t="s">
         <v>23</v>
@@ -60189,7 +60189,7 @@
         <v>1947</v>
       </c>
       <c r="Q892" s="6">
-        <v>244.19</v>
+        <v>231.17</v>
       </c>
       <c r="R892" s="6" t="s">
         <v>23</v>
@@ -61959,7 +61959,7 @@
         <v>2038</v>
       </c>
       <c r="Q922" s="6">
-        <v>249.15</v>
+        <v>245.22</v>
       </c>
       <c r="R922" s="6" t="s">
         <v>23</v>
@@ -62018,7 +62018,7 @@
         <v>2041</v>
       </c>
       <c r="Q923" s="6">
-        <v>524.87</v>
+        <v>401.04</v>
       </c>
       <c r="R923" s="6" t="s">
         <v>23</v>
@@ -62313,7 +62313,7 @@
         <v>2056</v>
       </c>
       <c r="Q928" s="6">
-        <v>1309.74</v>
+        <v>1373.74</v>
       </c>
       <c r="R928" s="6" t="s">
         <v>23</v>
@@ -62372,7 +62372,7 @@
         <v>2059</v>
       </c>
       <c r="Q929" s="6">
-        <v>171.4</v>
+        <v>161.83000000000001</v>
       </c>
       <c r="R929" s="6" t="s">
         <v>23</v>
@@ -62608,7 +62608,7 @@
         <v>2071</v>
       </c>
       <c r="Q933" s="6">
-        <v>530.5</v>
+        <v>221.65</v>
       </c>
       <c r="R933" s="6" t="s">
         <v>23</v>
@@ -62844,7 +62844,7 @@
         <v>2083</v>
       </c>
       <c r="Q937" s="6">
-        <v>1609.06</v>
+        <v>1295.26</v>
       </c>
       <c r="R937" s="6" t="s">
         <v>23</v>
@@ -63080,7 +63080,7 @@
         <v>2095</v>
       </c>
       <c r="Q941" s="6">
-        <v>1177.79</v>
+        <v>1124.3900000000001</v>
       </c>
       <c r="R941" s="6" t="s">
         <v>23</v>
@@ -63301,7 +63301,7 @@
         <v>23</v>
       </c>
       <c r="L945" s="6">
-        <v>3.47</v>
+        <v>3.48</v>
       </c>
       <c r="M945" s="6">
         <v>0</v>
@@ -63552,7 +63552,7 @@
         <v>2119</v>
       </c>
       <c r="Q949" s="6">
-        <v>1502.92</v>
+        <v>622.02</v>
       </c>
       <c r="R949" s="6" t="s">
         <v>23</v>
@@ -63729,7 +63729,7 @@
         <v>2128</v>
       </c>
       <c r="Q952" s="6">
-        <v>391.48</v>
+        <v>381.45</v>
       </c>
       <c r="R952" s="6" t="s">
         <v>23</v>
@@ -63788,7 +63788,7 @@
         <v>2131</v>
       </c>
       <c r="Q953" s="6">
-        <v>344</v>
+        <v>293.85000000000002</v>
       </c>
       <c r="R953" s="6" t="s">
         <v>23</v>
@@ -63965,7 +63965,7 @@
         <v>2140</v>
       </c>
       <c r="Q956" s="6">
-        <v>415.7</v>
+        <v>365.55</v>
       </c>
       <c r="R956" s="6" t="s">
         <v>23</v>
@@ -64083,7 +64083,7 @@
         <v>2146</v>
       </c>
       <c r="Q958" s="6">
-        <v>632.70000000000005</v>
+        <v>500.1</v>
       </c>
       <c r="R958" s="6" t="s">
         <v>23</v>
@@ -64201,7 +64201,7 @@
         <v>2151</v>
       </c>
       <c r="Q960" s="6">
-        <v>1870.05</v>
+        <v>1273.05</v>
       </c>
       <c r="R960" s="6" t="s">
         <v>23</v>
@@ -64319,7 +64319,7 @@
         <v>2157</v>
       </c>
       <c r="Q962" s="6">
-        <v>3611.4</v>
+        <v>3014.35</v>
       </c>
       <c r="R962" s="6" t="s">
         <v>23</v>
@@ -64714,7 +64714,7 @@
         <v>21</v>
       </c>
       <c r="K969" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L969" s="6">
         <v>0</v>
@@ -64732,7 +64732,7 @@
         <v>2198</v>
       </c>
       <c r="Q969" s="6">
-        <v>0</v>
+        <v>-31</v>
       </c>
       <c r="R969" s="6" t="s">
         <v>23</v>
@@ -65440,7 +65440,7 @@
         <v>2233</v>
       </c>
       <c r="Q981" s="6">
-        <v>11084.88</v>
+        <v>9799.23</v>
       </c>
       <c r="R981" s="6" t="s">
         <v>23</v>
@@ -65499,7 +65499,7 @@
         <v>2236</v>
       </c>
       <c r="Q982" s="6">
-        <v>8071.1</v>
+        <v>7219.25</v>
       </c>
       <c r="R982" s="6" t="s">
         <v>23</v>
@@ -65558,7 +65558,7 @@
         <v>2239</v>
       </c>
       <c r="Q983" s="6">
-        <v>1483.9</v>
+        <v>2128.3000000000002</v>
       </c>
       <c r="R983" s="6" t="s">
         <v>23</v>
@@ -65617,7 +65617,7 @@
         <v>2242</v>
       </c>
       <c r="Q984" s="6">
-        <v>1724</v>
+        <v>1292.9000000000001</v>
       </c>
       <c r="R984" s="6" t="s">
         <v>23</v>
@@ -65912,7 +65912,7 @@
         <v>2257</v>
       </c>
       <c r="Q989" s="6">
-        <v>7605.35</v>
+        <v>5716.84</v>
       </c>
       <c r="R989" s="6" t="s">
         <v>23</v>
@@ -66207,7 +66207,7 @@
         <v>2275</v>
       </c>
       <c r="Q994" s="6">
-        <v>2231.16</v>
+        <v>1487.34</v>
       </c>
       <c r="R994" s="6" t="s">
         <v>23</v>
@@ -66325,7 +66325,7 @@
         <v>2281</v>
       </c>
       <c r="Q996" s="6">
-        <v>995.61</v>
+        <v>786.91</v>
       </c>
       <c r="R996" s="6" t="s">
         <v>23</v>
@@ -66384,7 +66384,7 @@
         <v>2284</v>
       </c>
       <c r="Q997" s="6">
-        <v>30582.06</v>
+        <v>28038.21</v>
       </c>
       <c r="R997" s="6" t="s">
         <v>23</v>
@@ -66443,7 +66443,7 @@
         <v>2287</v>
       </c>
       <c r="Q998" s="6">
-        <v>41981.15597</v>
+        <v>48546.22597</v>
       </c>
       <c r="R998" s="6" t="s">
         <v>23</v>
@@ -66502,7 +66502,7 @@
         <v>2290</v>
       </c>
       <c r="Q999" s="6">
-        <v>346.5</v>
+        <v>251.4</v>
       </c>
       <c r="R999" s="6" t="s">
         <v>23</v>
@@ -66561,7 +66561,7 @@
         <v>2293</v>
       </c>
       <c r="Q1000" s="6">
-        <v>9885.93</v>
+        <v>9229.74</v>
       </c>
       <c r="R1000" s="6" t="s">
         <v>23</v>
@@ -66679,7 +66679,7 @@
         <v>2299</v>
       </c>
       <c r="Q1002" s="6">
-        <v>3032.72</v>
+        <v>2576.52</v>
       </c>
       <c r="R1002" s="6" t="s">
         <v>23</v>
@@ -66738,7 +66738,7 @@
         <v>2302</v>
       </c>
       <c r="Q1003" s="6">
-        <v>10974.02</v>
+        <v>8968.83</v>
       </c>
       <c r="R1003" s="6" t="s">
         <v>23</v>
@@ -66797,7 +66797,7 @@
         <v>2305</v>
       </c>
       <c r="Q1004" s="6">
-        <v>-20.97</v>
+        <v>15.97</v>
       </c>
       <c r="R1004" s="6" t="s">
         <v>23</v>
@@ -67487,7 +67487,7 @@
         <v>21</v>
       </c>
       <c r="K1016" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1016" s="6">
         <v>0</v>
@@ -67505,7 +67505,7 @@
         <v>2347</v>
       </c>
       <c r="Q1016" s="6">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="R1016" s="6" t="s">
         <v>23</v>
@@ -67549,7 +67549,7 @@
         <v>23</v>
       </c>
       <c r="L1017" s="6">
-        <v>0</v>
+        <v>3.46</v>
       </c>
       <c r="M1017" s="6">
         <v>0</v>
@@ -67608,7 +67608,7 @@
         <v>23</v>
       </c>
       <c r="L1018" s="6">
-        <v>0</v>
+        <v>3.46</v>
       </c>
       <c r="M1018" s="6">
         <v>0</v>
@@ -67623,7 +67623,7 @@
         <v>2352</v>
       </c>
       <c r="Q1018" s="6">
-        <v>404.4</v>
+        <v>393.72</v>
       </c>
       <c r="R1018" s="6" t="s">
         <v>23</v>
@@ -67667,7 +67667,7 @@
         <v>23</v>
       </c>
       <c r="L1019" s="6">
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="M1019" s="6">
         <v>0</v>
@@ -67726,7 +67726,7 @@
         <v>23</v>
       </c>
       <c r="L1020" s="6">
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="M1020" s="6">
         <v>0</v>
@@ -67785,7 +67785,7 @@
         <v>23</v>
       </c>
       <c r="L1021" s="6">
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="M1021" s="6">
         <v>0</v>
@@ -67844,7 +67844,7 @@
         <v>23</v>
       </c>
       <c r="L1022" s="6">
-        <v>0</v>
+        <v>3.58</v>
       </c>
       <c r="M1022" s="6">
         <v>0</v>
@@ -67859,7 +67859,7 @@
         <v>2372</v>
       </c>
       <c r="Q1022" s="6">
-        <v>0</v>
+        <v>139.94</v>
       </c>
       <c r="R1022" s="6" t="s">
         <v>23</v>
@@ -67900,10 +67900,10 @@
         <v>21</v>
       </c>
       <c r="K1023" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1023" s="6">
-        <v>0</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="M1023" s="6">
         <v>0</v>
@@ -67918,7 +67918,7 @@
         <v>2375</v>
       </c>
       <c r="Q1023" s="6">
-        <v>0</v>
+        <v>300.32</v>
       </c>
       <c r="R1023" s="6" t="s">
         <v>23</v>
@@ -68272,7 +68272,7 @@
         <v>2323</v>
       </c>
       <c r="Q1029" s="6">
-        <v>343.28</v>
+        <v>338.96</v>
       </c>
       <c r="R1029" s="6" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
act excell and logs
</commit_message>
<xml_diff>
--- a/EXCEL LIBS/TC_02.xlsx
+++ b/EXCEL LIBS/TC_02.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15441" uniqueCount="2378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15486" uniqueCount="2387">
   <si>
     <t>sqlnav01.aquinos.org : Aquinos, S.A.</t>
   </si>
@@ -7156,7 +7156,34 @@
     <t>GOMERA 16 (BLACK)</t>
   </si>
   <si>
-    <t>Lista Produto : 14-08-2020 09:37:29</t>
+    <t>TC15203</t>
+  </si>
+  <si>
+    <t>G4710</t>
+  </si>
+  <si>
+    <t>ZENITH 802 (CINZA ESCURO)</t>
+  </si>
+  <si>
+    <t>TC15204</t>
+  </si>
+  <si>
+    <t>G4760</t>
+  </si>
+  <si>
+    <t>ZENITH 807 (BEGE CLARO)</t>
+  </si>
+  <si>
+    <t>TC15205</t>
+  </si>
+  <si>
+    <t>G2940</t>
+  </si>
+  <si>
+    <t>SORRENTO 801 (CASTANHO)</t>
+  </si>
+  <si>
+    <t>Lista Produto : 31-08-2020 09:11:52</t>
   </si>
 </sst>
 </file>
@@ -7323,8 +7350,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NavDataRegion" displayName="NavDataRegion" ref="A3:S1031" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A3:S1031"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NavDataRegion" displayName="NavDataRegion" ref="A3:S1034" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A3:S1034"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Nº" dataDxfId="16"/>
     <tableColumn id="2" name="Cód. Barras Efacec" dataDxfId="15"/>
@@ -7613,7 +7640,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1031"/>
+  <dimension ref="A1:S1034"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
@@ -7667,7 +7694,7 @@
     </row>
     <row r="2" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2377</v>
+        <v>2386</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -10983,7 +11010,7 @@
         <v>134</v>
       </c>
       <c r="Q58" s="6">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="R58" s="6" t="s">
         <v>23</v>
@@ -12281,7 +12308,7 @@
         <v>178</v>
       </c>
       <c r="Q80" s="6">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R80" s="6" t="s">
         <v>23</v>
@@ -15880,7 +15907,7 @@
         <v>300</v>
       </c>
       <c r="Q141" s="6">
-        <v>510</v>
+        <v>0</v>
       </c>
       <c r="R141" s="6" t="s">
         <v>23</v>
@@ -16352,7 +16379,7 @@
         <v>317</v>
       </c>
       <c r="Q149" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R149" s="6" t="s">
         <v>23</v>
@@ -16411,7 +16438,7 @@
         <v>319</v>
       </c>
       <c r="Q150" s="6">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="R150" s="6" t="s">
         <v>23</v>
@@ -16529,7 +16556,7 @@
         <v>323</v>
       </c>
       <c r="Q152" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R152" s="6" t="s">
         <v>23</v>
@@ -16588,7 +16615,7 @@
         <v>325</v>
       </c>
       <c r="Q153" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R153" s="6" t="s">
         <v>23</v>
@@ -17414,7 +17441,7 @@
         <v>353</v>
       </c>
       <c r="Q167" s="6">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="R167" s="6" t="s">
         <v>23</v>
@@ -17532,7 +17559,7 @@
         <v>358</v>
       </c>
       <c r="Q169" s="6">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="R169" s="6" t="s">
         <v>23</v>
@@ -17591,7 +17618,7 @@
         <v>360</v>
       </c>
       <c r="Q170" s="6">
-        <v>642</v>
+        <v>665</v>
       </c>
       <c r="R170" s="6" t="s">
         <v>23</v>
@@ -17650,7 +17677,7 @@
         <v>362</v>
       </c>
       <c r="Q171" s="6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="R171" s="6" t="s">
         <v>23</v>
@@ -17827,7 +17854,7 @@
         <v>368</v>
       </c>
       <c r="Q174" s="6">
-        <v>1329.24</v>
+        <v>2231.8000000000002</v>
       </c>
       <c r="R174" s="6" t="s">
         <v>23</v>
@@ -17886,7 +17913,7 @@
         <v>370</v>
       </c>
       <c r="Q175" s="6">
-        <v>1237</v>
+        <v>1317</v>
       </c>
       <c r="R175" s="6" t="s">
         <v>23</v>
@@ -18063,7 +18090,7 @@
         <v>376</v>
       </c>
       <c r="Q178" s="6">
-        <v>1005.89</v>
+        <v>990</v>
       </c>
       <c r="R178" s="6" t="s">
         <v>23</v>
@@ -18122,7 +18149,7 @@
         <v>378</v>
       </c>
       <c r="Q179" s="6">
-        <v>1000.86</v>
+        <v>978</v>
       </c>
       <c r="R179" s="6" t="s">
         <v>23</v>
@@ -18358,7 +18385,7 @@
         <v>386</v>
       </c>
       <c r="Q183" s="6">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="R183" s="6" t="s">
         <v>23</v>
@@ -18594,7 +18621,7 @@
         <v>394</v>
       </c>
       <c r="Q187" s="6">
-        <v>3052.67</v>
+        <v>1906</v>
       </c>
       <c r="R187" s="6" t="s">
         <v>23</v>
@@ -18948,7 +18975,7 @@
         <v>406</v>
       </c>
       <c r="Q193" s="6">
-        <v>449</v>
+        <v>237</v>
       </c>
       <c r="R193" s="6" t="s">
         <v>23</v>
@@ -19243,7 +19270,7 @@
         <v>416</v>
       </c>
       <c r="Q198" s="6">
-        <v>1394.5</v>
+        <v>1546.2</v>
       </c>
       <c r="R198" s="6" t="s">
         <v>23</v>
@@ -19302,7 +19329,7 @@
         <v>418</v>
       </c>
       <c r="Q199" s="6">
-        <v>283.39999999999998</v>
+        <v>293.39999999999998</v>
       </c>
       <c r="R199" s="6" t="s">
         <v>23</v>
@@ -19361,7 +19388,7 @@
         <v>420</v>
       </c>
       <c r="Q200" s="6">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="R200" s="6" t="s">
         <v>23</v>
@@ -19479,7 +19506,7 @@
         <v>424</v>
       </c>
       <c r="Q202" s="6">
-        <v>280</v>
+        <v>290.5</v>
       </c>
       <c r="R202" s="6" t="s">
         <v>23</v>
@@ -19538,7 +19565,7 @@
         <v>426</v>
       </c>
       <c r="Q203" s="6">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="R203" s="6" t="s">
         <v>23</v>
@@ -19656,7 +19683,7 @@
         <v>430</v>
       </c>
       <c r="Q205" s="6">
-        <v>14.4</v>
+        <v>15</v>
       </c>
       <c r="R205" s="6" t="s">
         <v>23</v>
@@ -19715,7 +19742,7 @@
         <v>432</v>
       </c>
       <c r="Q206" s="6">
-        <v>1601.3</v>
+        <v>1457.5</v>
       </c>
       <c r="R206" s="6" t="s">
         <v>23</v>
@@ -19774,7 +19801,7 @@
         <v>434</v>
       </c>
       <c r="Q207" s="6">
-        <v>3568.4</v>
+        <v>3550.9</v>
       </c>
       <c r="R207" s="6" t="s">
         <v>23</v>
@@ -19833,7 +19860,7 @@
         <v>436</v>
       </c>
       <c r="Q208" s="6">
-        <v>944.5</v>
+        <v>1021.5</v>
       </c>
       <c r="R208" s="6" t="s">
         <v>23</v>
@@ -19892,7 +19919,7 @@
         <v>438</v>
       </c>
       <c r="Q209" s="6">
-        <v>2283.92</v>
+        <v>2476.36</v>
       </c>
       <c r="R209" s="6" t="s">
         <v>23</v>
@@ -20128,7 +20155,7 @@
         <v>446</v>
       </c>
       <c r="Q213" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R213" s="6" t="s">
         <v>23</v>
@@ -20246,7 +20273,7 @@
         <v>450</v>
       </c>
       <c r="Q215" s="6">
-        <v>383.5</v>
+        <v>288.5</v>
       </c>
       <c r="R215" s="6" t="s">
         <v>23</v>
@@ -20600,7 +20627,7 @@
         <v>462</v>
       </c>
       <c r="Q221" s="6">
-        <v>0</v>
+        <v>358.2</v>
       </c>
       <c r="R221" s="6" t="s">
         <v>23</v>
@@ -20659,7 +20686,7 @@
         <v>464</v>
       </c>
       <c r="Q222" s="6">
-        <v>2808.63</v>
+        <v>3178.3</v>
       </c>
       <c r="R222" s="6" t="s">
         <v>23</v>
@@ -20718,7 +20745,7 @@
         <v>466</v>
       </c>
       <c r="Q223" s="6">
-        <v>282.38</v>
+        <v>177.5</v>
       </c>
       <c r="R223" s="6" t="s">
         <v>23</v>
@@ -21013,7 +21040,7 @@
         <v>476</v>
       </c>
       <c r="Q228" s="6">
-        <v>279</v>
+        <v>148</v>
       </c>
       <c r="R228" s="6" t="s">
         <v>23</v>
@@ -21131,7 +21158,7 @@
         <v>480</v>
       </c>
       <c r="Q230" s="6">
-        <v>3559.2</v>
+        <v>3559.5</v>
       </c>
       <c r="R230" s="6" t="s">
         <v>23</v>
@@ -21190,7 +21217,7 @@
         <v>482</v>
       </c>
       <c r="Q231" s="6">
-        <v>261.5</v>
+        <v>260.5</v>
       </c>
       <c r="R231" s="6" t="s">
         <v>23</v>
@@ -21721,7 +21748,7 @@
         <v>500</v>
       </c>
       <c r="Q240" s="6">
-        <v>2665.02</v>
+        <v>2486</v>
       </c>
       <c r="R240" s="6" t="s">
         <v>23</v>
@@ -21780,7 +21807,7 @@
         <v>502</v>
       </c>
       <c r="Q241" s="6">
-        <v>3097.36</v>
+        <v>2944.8</v>
       </c>
       <c r="R241" s="6" t="s">
         <v>23</v>
@@ -21898,7 +21925,7 @@
         <v>506</v>
       </c>
       <c r="Q243" s="6">
-        <v>597.27</v>
+        <v>591.70000000000005</v>
       </c>
       <c r="R243" s="6" t="s">
         <v>23</v>
@@ -21957,7 +21984,7 @@
         <v>508</v>
       </c>
       <c r="Q244" s="6">
-        <v>1119.03</v>
+        <v>1101.5999999999999</v>
       </c>
       <c r="R244" s="6" t="s">
         <v>23</v>
@@ -22016,7 +22043,7 @@
         <v>510</v>
       </c>
       <c r="Q245" s="6">
-        <v>784</v>
+        <v>276.5</v>
       </c>
       <c r="R245" s="6" t="s">
         <v>23</v>
@@ -22075,7 +22102,7 @@
         <v>512</v>
       </c>
       <c r="Q246" s="6">
-        <v>1217.4000000000001</v>
+        <v>1216.4000000000001</v>
       </c>
       <c r="R246" s="6" t="s">
         <v>23</v>
@@ -22134,7 +22161,7 @@
         <v>514</v>
       </c>
       <c r="Q247" s="6">
-        <v>290</v>
+        <v>335.7</v>
       </c>
       <c r="R247" s="6" t="s">
         <v>23</v>
@@ -22193,7 +22220,7 @@
         <v>516</v>
       </c>
       <c r="Q248" s="6">
-        <v>525.20000000000005</v>
+        <v>325.5</v>
       </c>
       <c r="R248" s="6" t="s">
         <v>23</v>
@@ -22252,7 +22279,7 @@
         <v>518</v>
       </c>
       <c r="Q249" s="6">
-        <v>6104.7</v>
+        <v>6119.7</v>
       </c>
       <c r="R249" s="6" t="s">
         <v>23</v>
@@ -22311,7 +22338,7 @@
         <v>520</v>
       </c>
       <c r="Q250" s="6">
-        <v>574</v>
+        <v>656.9</v>
       </c>
       <c r="R250" s="6" t="s">
         <v>23</v>
@@ -22370,7 +22397,7 @@
         <v>522</v>
       </c>
       <c r="Q251" s="6">
-        <v>1001.9</v>
+        <v>795.3</v>
       </c>
       <c r="R251" s="6" t="s">
         <v>23</v>
@@ -22429,7 +22456,7 @@
         <v>524</v>
       </c>
       <c r="Q252" s="6">
-        <v>2917.9</v>
+        <v>3030.7</v>
       </c>
       <c r="R252" s="6" t="s">
         <v>23</v>
@@ -22488,7 +22515,7 @@
         <v>526</v>
       </c>
       <c r="Q253" s="6">
-        <v>2134.3000000000002</v>
+        <v>2034.6</v>
       </c>
       <c r="R253" s="6" t="s">
         <v>23</v>
@@ -22606,7 +22633,7 @@
         <v>530</v>
       </c>
       <c r="Q255" s="6">
-        <v>13128.8</v>
+        <v>13096</v>
       </c>
       <c r="R255" s="6" t="s">
         <v>23</v>
@@ -22724,7 +22751,7 @@
         <v>534</v>
       </c>
       <c r="Q257" s="6">
-        <v>5604.8</v>
+        <v>5579.3</v>
       </c>
       <c r="R257" s="6" t="s">
         <v>23</v>
@@ -22783,7 +22810,7 @@
         <v>536</v>
       </c>
       <c r="Q258" s="6">
-        <v>4434.5</v>
+        <v>4385</v>
       </c>
       <c r="R258" s="6" t="s">
         <v>23</v>
@@ -22842,7 +22869,7 @@
         <v>538</v>
       </c>
       <c r="Q259" s="6">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R259" s="6" t="s">
         <v>23</v>
@@ -22901,7 +22928,7 @@
         <v>540</v>
       </c>
       <c r="Q260" s="6">
-        <v>3212.65</v>
+        <v>3204.5</v>
       </c>
       <c r="R260" s="6" t="s">
         <v>23</v>
@@ -23019,7 +23046,7 @@
         <v>544</v>
       </c>
       <c r="Q262" s="6">
-        <v>1856.5</v>
+        <v>1856.7</v>
       </c>
       <c r="R262" s="6" t="s">
         <v>23</v>
@@ -23137,7 +23164,7 @@
         <v>548</v>
       </c>
       <c r="Q264" s="6">
-        <v>2470</v>
+        <v>2411</v>
       </c>
       <c r="R264" s="6" t="s">
         <v>23</v>
@@ -23196,7 +23223,7 @@
         <v>550</v>
       </c>
       <c r="Q265" s="6">
-        <v>325.2</v>
+        <v>280.2</v>
       </c>
       <c r="R265" s="6" t="s">
         <v>23</v>
@@ -23255,7 +23282,7 @@
         <v>552</v>
       </c>
       <c r="Q266" s="6">
-        <v>260.5</v>
+        <v>72.8</v>
       </c>
       <c r="R266" s="6" t="s">
         <v>23</v>
@@ -23314,7 +23341,7 @@
         <v>554</v>
       </c>
       <c r="Q267" s="6">
-        <v>805.6</v>
+        <v>805.4</v>
       </c>
       <c r="R267" s="6" t="s">
         <v>23</v>
@@ -23491,7 +23518,7 @@
         <v>561</v>
       </c>
       <c r="Q270" s="6">
-        <v>277.04000000000002</v>
+        <v>266.2</v>
       </c>
       <c r="R270" s="6" t="s">
         <v>23</v>
@@ -23609,7 +23636,7 @@
         <v>565</v>
       </c>
       <c r="Q272" s="6">
-        <v>2197.46</v>
+        <v>2132.9</v>
       </c>
       <c r="R272" s="6" t="s">
         <v>23</v>
@@ -23727,7 +23754,7 @@
         <v>569</v>
       </c>
       <c r="Q274" s="6">
-        <v>3969</v>
+        <v>3969.3</v>
       </c>
       <c r="R274" s="6" t="s">
         <v>23</v>
@@ -23904,7 +23931,7 @@
         <v>575</v>
       </c>
       <c r="Q277" s="6">
-        <v>1698.98</v>
+        <v>1673.9</v>
       </c>
       <c r="R277" s="6" t="s">
         <v>23</v>
@@ -24022,7 +24049,7 @@
         <v>579</v>
       </c>
       <c r="Q279" s="6">
-        <v>0</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="R279" s="6" t="s">
         <v>23</v>
@@ -24140,7 +24167,7 @@
         <v>583</v>
       </c>
       <c r="Q281" s="6">
-        <v>347.2</v>
+        <v>332.9</v>
       </c>
       <c r="R281" s="6" t="s">
         <v>23</v>
@@ -24258,7 +24285,7 @@
         <v>587</v>
       </c>
       <c r="Q283" s="6">
-        <v>427.5</v>
+        <v>434.9</v>
       </c>
       <c r="R283" s="6" t="s">
         <v>23</v>
@@ -24317,7 +24344,7 @@
         <v>589</v>
       </c>
       <c r="Q284" s="6">
-        <v>445</v>
+        <v>462.9</v>
       </c>
       <c r="R284" s="6" t="s">
         <v>23</v>
@@ -24376,7 +24403,7 @@
         <v>591</v>
       </c>
       <c r="Q285" s="6">
-        <v>687.81</v>
+        <v>424.1</v>
       </c>
       <c r="R285" s="6" t="s">
         <v>23</v>
@@ -24494,7 +24521,7 @@
         <v>595</v>
       </c>
       <c r="Q287" s="6">
-        <v>1847.31</v>
+        <v>1647.6</v>
       </c>
       <c r="R287" s="6" t="s">
         <v>23</v>
@@ -24553,7 +24580,7 @@
         <v>597</v>
       </c>
       <c r="Q288" s="6">
-        <v>551.48</v>
+        <v>609.70000000000005</v>
       </c>
       <c r="R288" s="6" t="s">
         <v>23</v>
@@ -24612,7 +24639,7 @@
         <v>599</v>
       </c>
       <c r="Q289" s="6">
-        <v>644.16</v>
+        <v>895.9</v>
       </c>
       <c r="R289" s="6" t="s">
         <v>23</v>
@@ -24671,7 +24698,7 @@
         <v>601</v>
       </c>
       <c r="Q290" s="6">
-        <v>326.29000000000002</v>
+        <v>209.2</v>
       </c>
       <c r="R290" s="6" t="s">
         <v>23</v>
@@ -24730,7 +24757,7 @@
         <v>603</v>
       </c>
       <c r="Q291" s="6">
-        <v>1569.18</v>
+        <v>1689.1</v>
       </c>
       <c r="R291" s="6" t="s">
         <v>23</v>
@@ -24789,7 +24816,7 @@
         <v>605</v>
       </c>
       <c r="Q292" s="6">
-        <v>1078.9000000000001</v>
+        <v>1083.9000000000001</v>
       </c>
       <c r="R292" s="6" t="s">
         <v>23</v>
@@ -24966,7 +24993,7 @@
         <v>611</v>
       </c>
       <c r="Q295" s="6">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="R295" s="6" t="s">
         <v>23</v>
@@ -25025,7 +25052,7 @@
         <v>613</v>
       </c>
       <c r="Q296" s="6">
-        <v>1208.22</v>
+        <v>1191.2</v>
       </c>
       <c r="R296" s="6" t="s">
         <v>23</v>
@@ -25084,7 +25111,7 @@
         <v>615</v>
       </c>
       <c r="Q297" s="6">
-        <v>3039.43</v>
+        <v>2976.3</v>
       </c>
       <c r="R297" s="6" t="s">
         <v>23</v>
@@ -25143,7 +25170,7 @@
         <v>617</v>
       </c>
       <c r="Q298" s="6">
-        <v>147.63</v>
+        <v>152</v>
       </c>
       <c r="R298" s="6" t="s">
         <v>23</v>
@@ -25202,7 +25229,7 @@
         <v>619</v>
       </c>
       <c r="Q299" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R299" s="6" t="s">
         <v>23</v>
@@ -25261,7 +25288,7 @@
         <v>621</v>
       </c>
       <c r="Q300" s="6">
-        <v>1040.58</v>
+        <v>1138.7</v>
       </c>
       <c r="R300" s="6" t="s">
         <v>23</v>
@@ -25320,7 +25347,7 @@
         <v>623</v>
       </c>
       <c r="Q301" s="6">
-        <v>462.5</v>
+        <v>417.8</v>
       </c>
       <c r="R301" s="6" t="s">
         <v>23</v>
@@ -25379,7 +25406,7 @@
         <v>625</v>
       </c>
       <c r="Q302" s="6">
-        <v>708.82</v>
+        <v>758.9</v>
       </c>
       <c r="R302" s="6" t="s">
         <v>23</v>
@@ -25438,7 +25465,7 @@
         <v>627</v>
       </c>
       <c r="Q303" s="6">
-        <v>3052.73</v>
+        <v>2594.5</v>
       </c>
       <c r="R303" s="6" t="s">
         <v>23</v>
@@ -25497,7 +25524,7 @@
         <v>629</v>
       </c>
       <c r="Q304" s="6">
-        <v>1525.83</v>
+        <v>1632.6</v>
       </c>
       <c r="R304" s="6" t="s">
         <v>23</v>
@@ -25556,7 +25583,7 @@
         <v>631</v>
       </c>
       <c r="Q305" s="6">
-        <v>50.6</v>
+        <v>215.2</v>
       </c>
       <c r="R305" s="6" t="s">
         <v>23</v>
@@ -25615,7 +25642,7 @@
         <v>633</v>
       </c>
       <c r="Q306" s="6">
-        <v>1314.4</v>
+        <v>1437.5</v>
       </c>
       <c r="R306" s="6" t="s">
         <v>23</v>
@@ -25674,7 +25701,7 @@
         <v>635</v>
       </c>
       <c r="Q307" s="6">
-        <v>969.2</v>
+        <v>971.2</v>
       </c>
       <c r="R307" s="6" t="s">
         <v>23</v>
@@ -25733,7 +25760,7 @@
         <v>637</v>
       </c>
       <c r="Q308" s="6">
-        <v>287.5</v>
+        <v>184.5</v>
       </c>
       <c r="R308" s="6" t="s">
         <v>23</v>
@@ -25792,7 +25819,7 @@
         <v>639</v>
       </c>
       <c r="Q309" s="6">
-        <v>1930.03</v>
+        <v>1882.3</v>
       </c>
       <c r="R309" s="6" t="s">
         <v>23</v>
@@ -25851,7 +25878,7 @@
         <v>641</v>
       </c>
       <c r="Q310" s="6">
-        <v>1557.3</v>
+        <v>991.8</v>
       </c>
       <c r="R310" s="6" t="s">
         <v>23</v>
@@ -25910,7 +25937,7 @@
         <v>643</v>
       </c>
       <c r="Q311" s="6">
-        <v>118.6</v>
+        <v>123.6</v>
       </c>
       <c r="R311" s="6" t="s">
         <v>23</v>
@@ -25969,7 +25996,7 @@
         <v>646</v>
       </c>
       <c r="Q312" s="6">
-        <v>3520.23</v>
+        <v>5827.5</v>
       </c>
       <c r="R312" s="6" t="s">
         <v>23</v>
@@ -26028,7 +26055,7 @@
         <v>649</v>
       </c>
       <c r="Q313" s="6">
-        <v>159.9</v>
+        <v>1190.7</v>
       </c>
       <c r="R313" s="6" t="s">
         <v>23</v>
@@ -26087,7 +26114,7 @@
         <v>652</v>
       </c>
       <c r="Q314" s="6">
-        <v>2137.9299999999998</v>
+        <v>2080</v>
       </c>
       <c r="R314" s="6" t="s">
         <v>23</v>
@@ -26205,7 +26232,7 @@
         <v>658</v>
       </c>
       <c r="Q316" s="6">
-        <v>196.99</v>
+        <v>171</v>
       </c>
       <c r="R316" s="6" t="s">
         <v>23</v>
@@ -26264,7 +26291,7 @@
         <v>660</v>
       </c>
       <c r="Q317" s="6">
-        <v>8664.98</v>
+        <v>8550.2999999999993</v>
       </c>
       <c r="R317" s="6" t="s">
         <v>23</v>
@@ -26323,7 +26350,7 @@
         <v>662</v>
       </c>
       <c r="Q318" s="6">
-        <v>2015.42</v>
+        <v>1565.7</v>
       </c>
       <c r="R318" s="6" t="s">
         <v>23</v>
@@ -26382,7 +26409,7 @@
         <v>664</v>
       </c>
       <c r="Q319" s="6">
-        <v>8005.9</v>
+        <v>8062.9</v>
       </c>
       <c r="R319" s="6" t="s">
         <v>23</v>
@@ -26438,10 +26465,10 @@
         <v>21</v>
       </c>
       <c r="P320" s="5" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="Q320" s="6">
-        <v>3586.21</v>
+        <v>3132.7</v>
       </c>
       <c r="R320" s="6" t="s">
         <v>23</v>
@@ -26500,7 +26527,7 @@
         <v>668</v>
       </c>
       <c r="Q321" s="6">
-        <v>5952.56</v>
+        <v>5358.1</v>
       </c>
       <c r="R321" s="6" t="s">
         <v>23</v>
@@ -26559,7 +26586,7 @@
         <v>670</v>
       </c>
       <c r="Q322" s="6">
-        <v>1940.29</v>
+        <v>1532.4</v>
       </c>
       <c r="R322" s="6" t="s">
         <v>23</v>
@@ -26618,7 +26645,7 @@
         <v>672</v>
       </c>
       <c r="Q323" s="6">
-        <v>2757.82</v>
+        <v>2524.5</v>
       </c>
       <c r="R323" s="6" t="s">
         <v>23</v>
@@ -26677,7 +26704,7 @@
         <v>674</v>
       </c>
       <c r="Q324" s="6">
-        <v>2058.92</v>
+        <v>1970.9</v>
       </c>
       <c r="R324" s="6" t="s">
         <v>23</v>
@@ -26736,7 +26763,7 @@
         <v>676</v>
       </c>
       <c r="Q325" s="6">
-        <v>3364.91</v>
+        <v>3314.1</v>
       </c>
       <c r="R325" s="6" t="s">
         <v>23</v>
@@ -26795,7 +26822,7 @@
         <v>678</v>
       </c>
       <c r="Q326" s="6">
-        <v>2247.0300000000002</v>
+        <v>2110</v>
       </c>
       <c r="R326" s="6" t="s">
         <v>23</v>
@@ -26854,7 +26881,7 @@
         <v>680</v>
       </c>
       <c r="Q327" s="6">
-        <v>93.48</v>
+        <v>7</v>
       </c>
       <c r="R327" s="6" t="s">
         <v>23</v>
@@ -26913,7 +26940,7 @@
         <v>683</v>
       </c>
       <c r="Q328" s="6">
-        <v>1771.92</v>
+        <v>1721.4</v>
       </c>
       <c r="R328" s="6" t="s">
         <v>23</v>
@@ -26972,7 +26999,7 @@
         <v>686</v>
       </c>
       <c r="Q329" s="6">
-        <v>1893.29</v>
+        <v>1871.5</v>
       </c>
       <c r="R329" s="6" t="s">
         <v>23</v>
@@ -27031,7 +27058,7 @@
         <v>689</v>
       </c>
       <c r="Q330" s="6">
-        <v>711.59</v>
+        <v>649.70000000000005</v>
       </c>
       <c r="R330" s="6" t="s">
         <v>23</v>
@@ -27090,7 +27117,7 @@
         <v>692</v>
       </c>
       <c r="Q331" s="6">
-        <v>2742.2</v>
+        <v>3261.7</v>
       </c>
       <c r="R331" s="6" t="s">
         <v>23</v>
@@ -27149,7 +27176,7 @@
         <v>694</v>
       </c>
       <c r="Q332" s="6">
-        <v>1652.4</v>
+        <v>1720.8</v>
       </c>
       <c r="R332" s="6" t="s">
         <v>23</v>
@@ -27208,7 +27235,7 @@
         <v>697</v>
       </c>
       <c r="Q333" s="6">
-        <v>1418.49</v>
+        <v>1354.8</v>
       </c>
       <c r="R333" s="6" t="s">
         <v>23</v>
@@ -27267,7 +27294,7 @@
         <v>700</v>
       </c>
       <c r="Q334" s="6">
-        <v>59.7</v>
+        <v>32</v>
       </c>
       <c r="R334" s="6" t="s">
         <v>23</v>
@@ -27326,7 +27353,7 @@
         <v>703</v>
       </c>
       <c r="Q335" s="6">
-        <v>1356.85</v>
+        <v>1280</v>
       </c>
       <c r="R335" s="6" t="s">
         <v>23</v>
@@ -27385,7 +27412,7 @@
         <v>706</v>
       </c>
       <c r="Q336" s="6">
-        <v>1813.74</v>
+        <v>1640.5</v>
       </c>
       <c r="R336" s="6" t="s">
         <v>23</v>
@@ -27444,7 +27471,7 @@
         <v>708</v>
       </c>
       <c r="Q337" s="6">
-        <v>215.2</v>
+        <v>200.8</v>
       </c>
       <c r="R337" s="6" t="s">
         <v>23</v>
@@ -27562,7 +27589,7 @@
         <v>712</v>
       </c>
       <c r="Q339" s="6">
-        <v>732.4</v>
+        <v>732.8</v>
       </c>
       <c r="R339" s="6" t="s">
         <v>23</v>
@@ -27739,7 +27766,7 @@
         <v>718</v>
       </c>
       <c r="Q342" s="6">
-        <v>2661.3</v>
+        <v>2661.8</v>
       </c>
       <c r="R342" s="6" t="s">
         <v>23</v>
@@ -27798,7 +27825,7 @@
         <v>720</v>
       </c>
       <c r="Q343" s="6">
-        <v>228.72</v>
+        <v>216.3</v>
       </c>
       <c r="R343" s="6" t="s">
         <v>23</v>
@@ -27916,7 +27943,7 @@
         <v>724</v>
       </c>
       <c r="Q345" s="6">
-        <v>567.84</v>
+        <v>366.9</v>
       </c>
       <c r="R345" s="6" t="s">
         <v>23</v>
@@ -27975,7 +28002,7 @@
         <v>726</v>
       </c>
       <c r="Q346" s="6">
-        <v>323.77999999999997</v>
+        <v>372.3</v>
       </c>
       <c r="R346" s="6" t="s">
         <v>23</v>
@@ -28034,7 +28061,7 @@
         <v>728</v>
       </c>
       <c r="Q347" s="6">
-        <v>42.28</v>
+        <v>160.6</v>
       </c>
       <c r="R347" s="6" t="s">
         <v>23</v>
@@ -28093,7 +28120,7 @@
         <v>731</v>
       </c>
       <c r="Q348" s="6">
-        <v>1036.48</v>
+        <v>1049.9000000000001</v>
       </c>
       <c r="R348" s="6" t="s">
         <v>23</v>
@@ -28152,7 +28179,7 @@
         <v>734</v>
       </c>
       <c r="Q349" s="6">
-        <v>722.35</v>
+        <v>1799.1</v>
       </c>
       <c r="R349" s="6" t="s">
         <v>23</v>
@@ -28211,7 +28238,7 @@
         <v>736</v>
       </c>
       <c r="Q350" s="6">
-        <v>4453.05</v>
+        <v>3485.3</v>
       </c>
       <c r="R350" s="6" t="s">
         <v>23</v>
@@ -28270,7 +28297,7 @@
         <v>738</v>
       </c>
       <c r="Q351" s="6">
-        <v>12630.58</v>
+        <v>3344.6</v>
       </c>
       <c r="R351" s="6" t="s">
         <v>23</v>
@@ -28329,7 +28356,7 @@
         <v>741</v>
       </c>
       <c r="Q352" s="6">
-        <v>3514.76</v>
+        <v>3502.5</v>
       </c>
       <c r="R352" s="6" t="s">
         <v>23</v>
@@ -28388,7 +28415,7 @@
         <v>744</v>
       </c>
       <c r="Q353" s="6">
-        <v>227.46</v>
+        <v>194.9</v>
       </c>
       <c r="R353" s="6" t="s">
         <v>23</v>
@@ -28447,7 +28474,7 @@
         <v>747</v>
       </c>
       <c r="Q354" s="6">
-        <v>90.07</v>
+        <v>29</v>
       </c>
       <c r="R354" s="6" t="s">
         <v>23</v>
@@ -28506,7 +28533,7 @@
         <v>749</v>
       </c>
       <c r="Q355" s="6">
-        <v>1367.7</v>
+        <v>1388.7</v>
       </c>
       <c r="R355" s="6" t="s">
         <v>23</v>
@@ -28742,7 +28769,7 @@
         <v>757</v>
       </c>
       <c r="Q359" s="6">
-        <v>840.05</v>
+        <v>770.5</v>
       </c>
       <c r="R359" s="6" t="s">
         <v>23</v>
@@ -28801,7 +28828,7 @@
         <v>759</v>
       </c>
       <c r="Q360" s="6">
-        <v>1499.33</v>
+        <v>1491</v>
       </c>
       <c r="R360" s="6" t="s">
         <v>23</v>
@@ -28919,7 +28946,7 @@
         <v>765</v>
       </c>
       <c r="Q362" s="6">
-        <v>1017.6</v>
+        <v>965.4</v>
       </c>
       <c r="R362" s="6" t="s">
         <v>23</v>
@@ -29155,7 +29182,7 @@
         <v>777</v>
       </c>
       <c r="Q366" s="6">
-        <v>390.1</v>
+        <v>401</v>
       </c>
       <c r="R366" s="6" t="s">
         <v>23</v>
@@ -29214,7 +29241,7 @@
         <v>779</v>
       </c>
       <c r="Q367" s="6">
-        <v>629.70000000000005</v>
+        <v>614.70000000000005</v>
       </c>
       <c r="R367" s="6" t="s">
         <v>23</v>
@@ -29332,7 +29359,7 @@
         <v>787</v>
       </c>
       <c r="Q369" s="6">
-        <v>128.30000000000001</v>
+        <v>85.3</v>
       </c>
       <c r="R369" s="6" t="s">
         <v>23</v>
@@ -29391,7 +29418,7 @@
         <v>791</v>
       </c>
       <c r="Q370" s="6">
-        <v>151.4</v>
+        <v>133.6</v>
       </c>
       <c r="R370" s="6" t="s">
         <v>23</v>
@@ -29450,7 +29477,7 @@
         <v>794</v>
       </c>
       <c r="Q371" s="6">
-        <v>3307.58</v>
+        <v>3666.9</v>
       </c>
       <c r="R371" s="6" t="s">
         <v>23</v>
@@ -29568,7 +29595,7 @@
         <v>800</v>
       </c>
       <c r="Q373" s="6">
-        <v>514.9</v>
+        <v>512.9</v>
       </c>
       <c r="R373" s="6" t="s">
         <v>23</v>
@@ -29627,7 +29654,7 @@
         <v>2360</v>
       </c>
       <c r="Q374" s="6">
-        <v>1864.45</v>
+        <v>964.6</v>
       </c>
       <c r="R374" s="6" t="s">
         <v>23</v>
@@ -35409,7 +35436,7 @@
         <v>996</v>
       </c>
       <c r="Q472" s="6">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="R472" s="6" t="s">
         <v>23</v>
@@ -35527,7 +35554,7 @@
         <v>1000</v>
       </c>
       <c r="Q474" s="6">
-        <v>240</v>
+        <v>222.1</v>
       </c>
       <c r="R474" s="6" t="s">
         <v>23</v>
@@ -35586,7 +35613,7 @@
         <v>1002</v>
       </c>
       <c r="Q475" s="6">
-        <v>79.2</v>
+        <v>93.2</v>
       </c>
       <c r="R475" s="6" t="s">
         <v>23</v>
@@ -35645,7 +35672,7 @@
         <v>1004</v>
       </c>
       <c r="Q476" s="6">
-        <v>136.80000000000001</v>
+        <v>126.8</v>
       </c>
       <c r="R476" s="6" t="s">
         <v>23</v>
@@ -35704,7 +35731,7 @@
         <v>1006</v>
       </c>
       <c r="Q477" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R477" s="6" t="s">
         <v>23</v>
@@ -35763,7 +35790,7 @@
         <v>1008</v>
       </c>
       <c r="Q478" s="6">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="R478" s="6" t="s">
         <v>23</v>
@@ -35881,7 +35908,7 @@
         <v>1012</v>
       </c>
       <c r="Q480" s="6">
-        <v>175.1</v>
+        <v>3</v>
       </c>
       <c r="R480" s="6" t="s">
         <v>23</v>
@@ -51457,7 +51484,7 @@
         <v>1546</v>
       </c>
       <c r="Q744" s="6">
-        <v>330.32</v>
+        <v>306</v>
       </c>
       <c r="R744" s="6" t="s">
         <v>23</v>
@@ -51752,7 +51779,7 @@
         <v>1563</v>
       </c>
       <c r="Q749" s="6">
-        <v>247.3</v>
+        <v>250.5</v>
       </c>
       <c r="R749" s="6" t="s">
         <v>23</v>
@@ -54053,7 +54080,7 @@
         <v>1649</v>
       </c>
       <c r="Q788" s="6">
-        <v>1569.04</v>
+        <v>1131</v>
       </c>
       <c r="R788" s="6" t="s">
         <v>23</v>
@@ -54230,7 +54257,7 @@
         <v>1655</v>
       </c>
       <c r="Q791" s="6">
-        <v>7094.93</v>
+        <v>11483.2</v>
       </c>
       <c r="R791" s="6" t="s">
         <v>23</v>
@@ -54348,7 +54375,7 @@
         <v>1659</v>
       </c>
       <c r="Q793" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R793" s="6" t="s">
         <v>23</v>
@@ -54466,7 +54493,7 @@
         <v>1663</v>
       </c>
       <c r="Q795" s="6">
-        <v>37</v>
+        <v>141.05404999999999</v>
       </c>
       <c r="R795" s="6" t="s">
         <v>23</v>
@@ -54525,7 +54552,7 @@
         <v>1665</v>
       </c>
       <c r="Q796" s="6">
-        <v>6946.27</v>
+        <v>2369.9</v>
       </c>
       <c r="R796" s="6" t="s">
         <v>23</v>
@@ -54820,7 +54847,7 @@
         <v>1675</v>
       </c>
       <c r="Q801" s="6">
-        <v>830.5</v>
+        <v>310</v>
       </c>
       <c r="R801" s="6" t="s">
         <v>23</v>
@@ -54938,7 +54965,7 @@
         <v>1679</v>
       </c>
       <c r="Q803" s="6">
-        <v>91.53</v>
+        <v>95</v>
       </c>
       <c r="R803" s="6" t="s">
         <v>23</v>
@@ -54982,7 +55009,7 @@
         <v>23</v>
       </c>
       <c r="L804" s="6">
-        <v>4.74</v>
+        <v>4.58</v>
       </c>
       <c r="M804" s="6">
         <v>0</v>
@@ -54997,7 +55024,7 @@
         <v>1681</v>
       </c>
       <c r="Q804" s="6">
-        <v>7327.16</v>
+        <v>88963</v>
       </c>
       <c r="R804" s="6" t="s">
         <v>23</v>
@@ -55041,7 +55068,7 @@
         <v>23</v>
       </c>
       <c r="L805" s="6">
-        <v>3.43</v>
+        <v>3.23</v>
       </c>
       <c r="M805" s="6">
         <v>0</v>
@@ -55056,7 +55083,7 @@
         <v>1684</v>
       </c>
       <c r="Q805" s="6">
-        <v>317.31</v>
+        <v>25005</v>
       </c>
       <c r="R805" s="6" t="s">
         <v>23</v>
@@ -55115,7 +55142,7 @@
         <v>1687</v>
       </c>
       <c r="Q806" s="6">
-        <v>353.89</v>
+        <v>54241.5</v>
       </c>
       <c r="R806" s="6" t="s">
         <v>23</v>
@@ -55159,7 +55186,7 @@
         <v>23</v>
       </c>
       <c r="L807" s="6">
-        <v>3.45</v>
+        <v>2.98</v>
       </c>
       <c r="M807" s="6">
         <v>0</v>
@@ -55174,7 +55201,7 @@
         <v>1690</v>
       </c>
       <c r="Q807" s="6">
-        <v>1171.5999999999999</v>
+        <v>11007</v>
       </c>
       <c r="R807" s="6" t="s">
         <v>23</v>
@@ -55233,7 +55260,7 @@
         <v>1693</v>
       </c>
       <c r="Q808" s="6">
-        <v>1310.1199999999999</v>
+        <v>40</v>
       </c>
       <c r="R808" s="6" t="s">
         <v>23</v>
@@ -56118,7 +56145,7 @@
         <v>1732</v>
       </c>
       <c r="Q823" s="6">
-        <v>911.8</v>
+        <v>912.6</v>
       </c>
       <c r="R823" s="6" t="s">
         <v>23</v>
@@ -56177,7 +56204,7 @@
         <v>1735</v>
       </c>
       <c r="Q824" s="6">
-        <v>4502.63</v>
+        <v>3436.1</v>
       </c>
       <c r="R824" s="6" t="s">
         <v>23</v>
@@ -56236,7 +56263,7 @@
         <v>1738</v>
       </c>
       <c r="Q825" s="6">
-        <v>796.4</v>
+        <v>796.2</v>
       </c>
       <c r="R825" s="6" t="s">
         <v>23</v>
@@ -56354,7 +56381,7 @@
         <v>1744</v>
       </c>
       <c r="Q827" s="6">
-        <v>576.20000000000005</v>
+        <v>555.5</v>
       </c>
       <c r="R827" s="6" t="s">
         <v>23</v>
@@ -56413,7 +56440,7 @@
         <v>1747</v>
       </c>
       <c r="Q828" s="6">
-        <v>529.6</v>
+        <v>598.6</v>
       </c>
       <c r="R828" s="6" t="s">
         <v>23</v>
@@ -56472,7 +56499,7 @@
         <v>1750</v>
       </c>
       <c r="Q829" s="6">
-        <v>3136.4</v>
+        <v>2449</v>
       </c>
       <c r="R829" s="6" t="s">
         <v>23</v>
@@ -56531,7 +56558,7 @@
         <v>1753</v>
       </c>
       <c r="Q830" s="6">
-        <v>770.3</v>
+        <v>707.8</v>
       </c>
       <c r="R830" s="6" t="s">
         <v>23</v>
@@ -56590,7 +56617,7 @@
         <v>1756</v>
       </c>
       <c r="Q831" s="6">
-        <v>2322.1</v>
+        <v>2388.1</v>
       </c>
       <c r="R831" s="6" t="s">
         <v>23</v>
@@ -56649,7 +56676,7 @@
         <v>1758</v>
       </c>
       <c r="Q832" s="6">
-        <v>1623.75</v>
+        <v>1228.0999999999999</v>
       </c>
       <c r="R832" s="6" t="s">
         <v>23</v>
@@ -56708,7 +56735,7 @@
         <v>1762</v>
       </c>
       <c r="Q833" s="6">
-        <v>6986.73</v>
+        <v>6662.7</v>
       </c>
       <c r="R833" s="6" t="s">
         <v>23</v>
@@ -56767,7 +56794,7 @@
         <v>1765</v>
       </c>
       <c r="Q834" s="6">
-        <v>4472.3999999999996</v>
+        <v>4390.6000000000004</v>
       </c>
       <c r="R834" s="6" t="s">
         <v>23</v>
@@ -56826,7 +56853,7 @@
         <v>1768</v>
       </c>
       <c r="Q835" s="6">
-        <v>4993.2</v>
+        <v>4903.5</v>
       </c>
       <c r="R835" s="6" t="s">
         <v>23</v>
@@ -56885,7 +56912,7 @@
         <v>1771</v>
       </c>
       <c r="Q836" s="6">
-        <v>245.2</v>
+        <v>259.7</v>
       </c>
       <c r="R836" s="6" t="s">
         <v>23</v>
@@ -57003,7 +57030,7 @@
         <v>1777</v>
       </c>
       <c r="Q838" s="6">
-        <v>466.46</v>
+        <v>404.3</v>
       </c>
       <c r="R838" s="6" t="s">
         <v>23</v>
@@ -57062,7 +57089,7 @@
         <v>1782</v>
       </c>
       <c r="Q839" s="6">
-        <v>136.41</v>
+        <v>123.8</v>
       </c>
       <c r="R839" s="6" t="s">
         <v>23</v>
@@ -57121,7 +57148,7 @@
         <v>1786</v>
       </c>
       <c r="Q840" s="6">
-        <v>127.43</v>
+        <v>74.8</v>
       </c>
       <c r="R840" s="6" t="s">
         <v>23</v>
@@ -57180,7 +57207,7 @@
         <v>1790</v>
       </c>
       <c r="Q841" s="6">
-        <v>4394.25</v>
+        <v>4356.5</v>
       </c>
       <c r="R841" s="6" t="s">
         <v>23</v>
@@ -57239,7 +57266,7 @@
         <v>747</v>
       </c>
       <c r="Q842" s="6">
-        <v>637.75</v>
+        <v>590.6</v>
       </c>
       <c r="R842" s="6" t="s">
         <v>23</v>
@@ -57298,7 +57325,7 @@
         <v>1797</v>
       </c>
       <c r="Q843" s="6">
-        <v>121.33</v>
+        <v>125.7</v>
       </c>
       <c r="R843" s="6" t="s">
         <v>23</v>
@@ -57357,7 +57384,7 @@
         <v>1800</v>
       </c>
       <c r="Q844" s="6">
-        <v>2071.5300000000002</v>
+        <v>2054.4</v>
       </c>
       <c r="R844" s="6" t="s">
         <v>23</v>
@@ -57416,7 +57443,7 @@
         <v>1804</v>
       </c>
       <c r="Q845" s="6">
-        <v>1511.3</v>
+        <v>1500.3</v>
       </c>
       <c r="R845" s="6" t="s">
         <v>23</v>
@@ -57475,7 +57502,7 @@
         <v>1806</v>
       </c>
       <c r="Q846" s="6">
-        <v>195.86</v>
+        <v>203.1</v>
       </c>
       <c r="R846" s="6" t="s">
         <v>23</v>
@@ -57534,7 +57561,7 @@
         <v>1809</v>
       </c>
       <c r="Q847" s="6">
-        <v>169.3</v>
+        <v>147.19999999999999</v>
       </c>
       <c r="R847" s="6" t="s">
         <v>23</v>
@@ -57593,7 +57620,7 @@
         <v>1812</v>
       </c>
       <c r="Q848" s="6">
-        <v>402.13</v>
+        <v>397.5</v>
       </c>
       <c r="R848" s="6" t="s">
         <v>23</v>
@@ -57652,7 +57679,7 @@
         <v>1817</v>
       </c>
       <c r="Q849" s="6">
-        <v>25014.5</v>
+        <v>25009.1</v>
       </c>
       <c r="R849" s="6" t="s">
         <v>23</v>
@@ -57770,7 +57797,7 @@
         <v>1822</v>
       </c>
       <c r="Q851" s="6">
-        <v>38595.01</v>
+        <v>38549.5</v>
       </c>
       <c r="R851" s="6" t="s">
         <v>23</v>
@@ -57829,7 +57856,7 @@
         <v>1825</v>
       </c>
       <c r="Q852" s="6">
-        <v>897.6</v>
+        <v>1046.5999999999999</v>
       </c>
       <c r="R852" s="6" t="s">
         <v>23</v>
@@ -58065,7 +58092,7 @@
         <v>1837</v>
       </c>
       <c r="Q856" s="6">
-        <v>144.83000000000001</v>
+        <v>161.4</v>
       </c>
       <c r="R856" s="6" t="s">
         <v>23</v>
@@ -58124,7 +58151,7 @@
         <v>1840</v>
       </c>
       <c r="Q857" s="6">
-        <v>102.34</v>
+        <v>88.7</v>
       </c>
       <c r="R857" s="6" t="s">
         <v>23</v>
@@ -58360,7 +58387,7 @@
         <v>1852</v>
       </c>
       <c r="Q861" s="6">
-        <v>334.25</v>
+        <v>285.8</v>
       </c>
       <c r="R861" s="6" t="s">
         <v>23</v>
@@ -58419,7 +58446,7 @@
         <v>1855</v>
       </c>
       <c r="Q862" s="6">
-        <v>6386.6</v>
+        <v>5950.9</v>
       </c>
       <c r="R862" s="6" t="s">
         <v>23</v>
@@ -58478,7 +58505,7 @@
         <v>1858</v>
       </c>
       <c r="Q863" s="6">
-        <v>1160.2</v>
+        <v>198</v>
       </c>
       <c r="R863" s="6" t="s">
         <v>23</v>
@@ -58537,7 +58564,7 @@
         <v>1861</v>
       </c>
       <c r="Q864" s="6">
-        <v>855.4</v>
+        <v>825.3</v>
       </c>
       <c r="R864" s="6" t="s">
         <v>23</v>
@@ -58596,7 +58623,7 @@
         <v>1864</v>
       </c>
       <c r="Q865" s="6">
-        <v>855.05</v>
+        <v>876.7</v>
       </c>
       <c r="R865" s="6" t="s">
         <v>23</v>
@@ -58655,7 +58682,7 @@
         <v>1868</v>
       </c>
       <c r="Q866" s="6">
-        <v>24.64</v>
+        <v>605.4</v>
       </c>
       <c r="R866" s="6" t="s">
         <v>23</v>
@@ -58714,7 +58741,7 @@
         <v>1871</v>
       </c>
       <c r="Q867" s="6">
-        <v>1597.7</v>
+        <v>1479.5</v>
       </c>
       <c r="R867" s="6" t="s">
         <v>23</v>
@@ -58773,7 +58800,7 @@
         <v>1874</v>
       </c>
       <c r="Q868" s="6">
-        <v>8745.32</v>
+        <v>8770.5</v>
       </c>
       <c r="R868" s="6" t="s">
         <v>23</v>
@@ -58832,7 +58859,7 @@
         <v>1877</v>
       </c>
       <c r="Q869" s="6">
-        <v>265.10000000000002</v>
+        <v>256.39999999999998</v>
       </c>
       <c r="R869" s="6" t="s">
         <v>23</v>
@@ -58891,7 +58918,7 @@
         <v>1880</v>
       </c>
       <c r="Q870" s="6">
-        <v>147.6</v>
+        <v>333.9</v>
       </c>
       <c r="R870" s="6" t="s">
         <v>23</v>
@@ -59068,7 +59095,7 @@
         <v>1889</v>
       </c>
       <c r="Q873" s="6">
-        <v>317.67</v>
+        <v>107</v>
       </c>
       <c r="R873" s="6" t="s">
         <v>23</v>
@@ -59127,7 +59154,7 @@
         <v>1892</v>
       </c>
       <c r="Q874" s="6">
-        <v>318.66000000000003</v>
+        <v>221.4</v>
       </c>
       <c r="R874" s="6" t="s">
         <v>23</v>
@@ -59186,7 +59213,7 @@
         <v>1895</v>
       </c>
       <c r="Q875" s="6">
-        <v>403.43</v>
+        <v>342.5</v>
       </c>
       <c r="R875" s="6" t="s">
         <v>23</v>
@@ -59245,7 +59272,7 @@
         <v>1898</v>
       </c>
       <c r="Q876" s="6">
-        <v>44.92</v>
+        <v>53</v>
       </c>
       <c r="R876" s="6" t="s">
         <v>23</v>
@@ -59304,7 +59331,7 @@
         <v>1901</v>
       </c>
       <c r="Q877" s="6">
-        <v>126.05</v>
+        <v>61</v>
       </c>
       <c r="R877" s="6" t="s">
         <v>23</v>
@@ -59363,7 +59390,7 @@
         <v>1904</v>
       </c>
       <c r="Q878" s="6">
-        <v>810.9</v>
+        <v>602.5</v>
       </c>
       <c r="R878" s="6" t="s">
         <v>23</v>
@@ -59422,7 +59449,7 @@
         <v>1907</v>
       </c>
       <c r="Q879" s="6">
-        <v>167.1</v>
+        <v>302.7</v>
       </c>
       <c r="R879" s="6" t="s">
         <v>23</v>
@@ -59481,7 +59508,7 @@
         <v>1910</v>
       </c>
       <c r="Q880" s="6">
-        <v>208.9</v>
+        <v>184.3</v>
       </c>
       <c r="R880" s="6" t="s">
         <v>23</v>
@@ -59540,7 +59567,7 @@
         <v>1913</v>
       </c>
       <c r="Q881" s="6">
-        <v>1880.3</v>
+        <v>1483.8</v>
       </c>
       <c r="R881" s="6" t="s">
         <v>23</v>
@@ -59599,7 +59626,7 @@
         <v>1916</v>
       </c>
       <c r="Q882" s="6">
-        <v>219.66</v>
+        <v>215.1</v>
       </c>
       <c r="R882" s="6" t="s">
         <v>23</v>
@@ -59658,7 +59685,7 @@
         <v>1919</v>
       </c>
       <c r="Q883" s="6">
-        <v>325.36</v>
+        <v>325.8</v>
       </c>
       <c r="R883" s="6" t="s">
         <v>23</v>
@@ -59717,7 +59744,7 @@
         <v>1922</v>
       </c>
       <c r="Q884" s="6">
-        <v>10052.56</v>
+        <v>9895.2999999999993</v>
       </c>
       <c r="R884" s="6" t="s">
         <v>23</v>
@@ -59776,7 +59803,7 @@
         <v>1925</v>
       </c>
       <c r="Q885" s="6">
-        <v>3037.72</v>
+        <v>3003.7</v>
       </c>
       <c r="R885" s="6" t="s">
         <v>23</v>
@@ -59894,7 +59921,7 @@
         <v>1932</v>
       </c>
       <c r="Q887" s="6">
-        <v>39.56</v>
+        <v>20</v>
       </c>
       <c r="R887" s="6" t="s">
         <v>23</v>
@@ -59953,7 +59980,7 @@
         <v>1935</v>
       </c>
       <c r="Q888" s="6">
-        <v>8.1199999999999992</v>
+        <v>0</v>
       </c>
       <c r="R888" s="6" t="s">
         <v>23</v>
@@ -60012,7 +60039,7 @@
         <v>1938</v>
       </c>
       <c r="Q889" s="6">
-        <v>30.57</v>
+        <v>252.7</v>
       </c>
       <c r="R889" s="6" t="s">
         <v>23</v>
@@ -60071,7 +60098,7 @@
         <v>1941</v>
       </c>
       <c r="Q890" s="6">
-        <v>22.72</v>
+        <v>0</v>
       </c>
       <c r="R890" s="6" t="s">
         <v>23</v>
@@ -60189,7 +60216,7 @@
         <v>1947</v>
       </c>
       <c r="Q892" s="6">
-        <v>231.17</v>
+        <v>230.9</v>
       </c>
       <c r="R892" s="6" t="s">
         <v>23</v>
@@ -60484,7 +60511,7 @@
         <v>1962</v>
       </c>
       <c r="Q897" s="6">
-        <v>0</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="R897" s="6" t="s">
         <v>23</v>
@@ -61959,7 +61986,7 @@
         <v>2038</v>
       </c>
       <c r="Q922" s="6">
-        <v>245.22</v>
+        <v>401.9</v>
       </c>
       <c r="R922" s="6" t="s">
         <v>23</v>
@@ -62003,7 +62030,7 @@
         <v>23</v>
       </c>
       <c r="L923" s="6">
-        <v>1.6</v>
+        <v>1.55</v>
       </c>
       <c r="M923" s="6">
         <v>0</v>
@@ -62018,7 +62045,7 @@
         <v>2041</v>
       </c>
       <c r="Q923" s="6">
-        <v>401.04</v>
+        <v>16635.099999999999</v>
       </c>
       <c r="R923" s="6" t="s">
         <v>23</v>
@@ -62077,7 +62104,7 @@
         <v>2044</v>
       </c>
       <c r="Q924" s="6">
-        <v>615.79999999999995</v>
+        <v>616.4</v>
       </c>
       <c r="R924" s="6" t="s">
         <v>23</v>
@@ -62136,7 +62163,7 @@
         <v>2047</v>
       </c>
       <c r="Q925" s="6">
-        <v>3973.73</v>
+        <v>3842.2</v>
       </c>
       <c r="R925" s="6" t="s">
         <v>23</v>
@@ -62195,7 +62222,7 @@
         <v>2050</v>
       </c>
       <c r="Q926" s="6">
-        <v>1544.22</v>
+        <v>1386.5</v>
       </c>
       <c r="R926" s="6" t="s">
         <v>23</v>
@@ -62254,7 +62281,7 @@
         <v>2053</v>
       </c>
       <c r="Q927" s="6">
-        <v>2429</v>
+        <v>2517</v>
       </c>
       <c r="R927" s="6" t="s">
         <v>23</v>
@@ -62313,7 +62340,7 @@
         <v>2056</v>
       </c>
       <c r="Q928" s="6">
-        <v>1373.74</v>
+        <v>662.5</v>
       </c>
       <c r="R928" s="6" t="s">
         <v>23</v>
@@ -62372,7 +62399,7 @@
         <v>2059</v>
       </c>
       <c r="Q929" s="6">
-        <v>161.83000000000001</v>
+        <v>136.4</v>
       </c>
       <c r="R929" s="6" t="s">
         <v>23</v>
@@ -62431,7 +62458,7 @@
         <v>2062</v>
       </c>
       <c r="Q930" s="6">
-        <v>419.46</v>
+        <v>239.5</v>
       </c>
       <c r="R930" s="6" t="s">
         <v>23</v>
@@ -62490,7 +62517,7 @@
         <v>2065</v>
       </c>
       <c r="Q931" s="6">
-        <v>1658.5</v>
+        <v>1127</v>
       </c>
       <c r="R931" s="6" t="s">
         <v>23</v>
@@ -62549,7 +62576,7 @@
         <v>2068</v>
       </c>
       <c r="Q932" s="6">
-        <v>673.9</v>
+        <v>683</v>
       </c>
       <c r="R932" s="6" t="s">
         <v>23</v>
@@ -62608,7 +62635,7 @@
         <v>2071</v>
       </c>
       <c r="Q933" s="6">
-        <v>189.7</v>
+        <v>6.35</v>
       </c>
       <c r="R933" s="6" t="s">
         <v>23</v>
@@ -62785,7 +62812,7 @@
         <v>2080</v>
       </c>
       <c r="Q936" s="6">
-        <v>1317</v>
+        <v>920.5</v>
       </c>
       <c r="R936" s="6" t="s">
         <v>23</v>
@@ -62844,7 +62871,7 @@
         <v>2083</v>
       </c>
       <c r="Q937" s="6">
-        <v>1002.38</v>
+        <v>3</v>
       </c>
       <c r="R937" s="6" t="s">
         <v>23</v>
@@ -62903,7 +62930,7 @@
         <v>2086</v>
       </c>
       <c r="Q938" s="6">
-        <v>473.93</v>
+        <v>474.3</v>
       </c>
       <c r="R938" s="6" t="s">
         <v>23</v>
@@ -63021,7 +63048,7 @@
         <v>2092</v>
       </c>
       <c r="Q940" s="6">
-        <v>175.97</v>
+        <v>190.7</v>
       </c>
       <c r="R940" s="6" t="s">
         <v>23</v>
@@ -63080,7 +63107,7 @@
         <v>2095</v>
       </c>
       <c r="Q941" s="6">
-        <v>1108.6300000000001</v>
+        <v>1092.8</v>
       </c>
       <c r="R941" s="6" t="s">
         <v>23</v>
@@ -63198,7 +63225,7 @@
         <v>2101</v>
       </c>
       <c r="Q943" s="6">
-        <v>108.9</v>
+        <v>176.4</v>
       </c>
       <c r="R943" s="6" t="s">
         <v>23</v>
@@ -63257,7 +63284,7 @@
         <v>2104</v>
       </c>
       <c r="Q944" s="6">
-        <v>2649.24</v>
+        <v>2630</v>
       </c>
       <c r="R944" s="6" t="s">
         <v>23</v>
@@ -63316,7 +63343,7 @@
         <v>2107</v>
       </c>
       <c r="Q945" s="6">
-        <v>1523.45</v>
+        <v>5468.3</v>
       </c>
       <c r="R945" s="6" t="s">
         <v>23</v>
@@ -63360,7 +63387,7 @@
         <v>23</v>
       </c>
       <c r="L946" s="6">
-        <v>3.48</v>
+        <v>3.13</v>
       </c>
       <c r="M946" s="6">
         <v>0</v>
@@ -63375,7 +63402,7 @@
         <v>2110</v>
       </c>
       <c r="Q946" s="6">
-        <v>212.67</v>
+        <v>10144.5</v>
       </c>
       <c r="R946" s="6" t="s">
         <v>23</v>
@@ -63552,7 +63579,7 @@
         <v>2119</v>
       </c>
       <c r="Q949" s="6">
-        <v>611.88</v>
+        <v>2162.6</v>
       </c>
       <c r="R949" s="6" t="s">
         <v>23</v>
@@ -63611,7 +63638,7 @@
         <v>2122</v>
       </c>
       <c r="Q950" s="6">
-        <v>364.1</v>
+        <v>368.2</v>
       </c>
       <c r="R950" s="6" t="s">
         <v>23</v>
@@ -63670,7 +63697,7 @@
         <v>2125</v>
       </c>
       <c r="Q951" s="6">
-        <v>-18.03</v>
+        <v>0</v>
       </c>
       <c r="R951" s="6" t="s">
         <v>23</v>
@@ -63729,7 +63756,7 @@
         <v>2128</v>
       </c>
       <c r="Q952" s="6">
-        <v>281.14999999999998</v>
+        <v>299.5</v>
       </c>
       <c r="R952" s="6" t="s">
         <v>23</v>
@@ -63788,7 +63815,7 @@
         <v>2131</v>
       </c>
       <c r="Q953" s="6">
-        <v>243.7</v>
+        <v>247.8</v>
       </c>
       <c r="R953" s="6" t="s">
         <v>23</v>
@@ -63847,7 +63874,7 @@
         <v>2134</v>
       </c>
       <c r="Q954" s="6">
-        <v>157.05000000000001</v>
+        <v>127.2</v>
       </c>
       <c r="R954" s="6" t="s">
         <v>23</v>
@@ -63906,7 +63933,7 @@
         <v>2137</v>
       </c>
       <c r="Q955" s="6">
-        <v>394.1</v>
+        <v>300.60000000000002</v>
       </c>
       <c r="R955" s="6" t="s">
         <v>23</v>
@@ -63965,7 +63992,7 @@
         <v>2140</v>
       </c>
       <c r="Q956" s="6">
-        <v>365.55</v>
+        <v>357.9</v>
       </c>
       <c r="R956" s="6" t="s">
         <v>23</v>
@@ -64006,7 +64033,7 @@
         <v>21</v>
       </c>
       <c r="K957" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L957" s="6">
         <v>0</v>
@@ -64024,7 +64051,7 @@
         <v>2143</v>
       </c>
       <c r="Q957" s="6">
-        <v>0</v>
+        <v>2413.5</v>
       </c>
       <c r="R957" s="6" t="s">
         <v>23</v>
@@ -64083,7 +64110,7 @@
         <v>2146</v>
       </c>
       <c r="Q958" s="6">
-        <v>301.05</v>
+        <v>1098.3</v>
       </c>
       <c r="R958" s="6" t="s">
         <v>23</v>
@@ -64142,7 +64169,7 @@
         <v>2149</v>
       </c>
       <c r="Q959" s="6">
-        <v>7955</v>
+        <v>5796.5</v>
       </c>
       <c r="R959" s="6" t="s">
         <v>23</v>
@@ -64201,7 +64228,7 @@
         <v>2151</v>
       </c>
       <c r="Q960" s="6">
-        <v>609.85</v>
+        <v>1723.4</v>
       </c>
       <c r="R960" s="6" t="s">
         <v>23</v>
@@ -64260,7 +64287,7 @@
         <v>2154</v>
       </c>
       <c r="Q961" s="6">
-        <v>3994.35</v>
+        <v>3957.92</v>
       </c>
       <c r="R961" s="6" t="s">
         <v>23</v>
@@ -64319,7 +64346,7 @@
         <v>2157</v>
       </c>
       <c r="Q962" s="6">
-        <v>2483.65</v>
+        <v>2283.6999999999998</v>
       </c>
       <c r="R962" s="6" t="s">
         <v>23</v>
@@ -64717,7 +64744,7 @@
         <v>23</v>
       </c>
       <c r="L969" s="6">
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="M969" s="6">
         <v>0</v>
@@ -64732,7 +64759,7 @@
         <v>2198</v>
       </c>
       <c r="Q969" s="6">
-        <v>50.47</v>
+        <v>37.5</v>
       </c>
       <c r="R969" s="6" t="s">
         <v>23</v>
@@ -65204,7 +65231,7 @@
         <v>2222</v>
       </c>
       <c r="Q977" s="6">
-        <v>28.26</v>
+        <v>0</v>
       </c>
       <c r="R977" s="6" t="s">
         <v>23</v>
@@ -65322,7 +65349,7 @@
         <v>2228</v>
       </c>
       <c r="Q979" s="6">
-        <v>152.44999999999999</v>
+        <v>1043.8</v>
       </c>
       <c r="R979" s="6" t="s">
         <v>23</v>
@@ -65381,7 +65408,7 @@
         <v>2230</v>
       </c>
       <c r="Q980" s="6">
-        <v>1974.27</v>
+        <v>1912.4</v>
       </c>
       <c r="R980" s="6" t="s">
         <v>23</v>
@@ -65440,7 +65467,7 @@
         <v>2233</v>
       </c>
       <c r="Q981" s="6">
-        <v>13237.03</v>
+        <v>9699.9</v>
       </c>
       <c r="R981" s="6" t="s">
         <v>23</v>
@@ -65499,7 +65526,7 @@
         <v>2236</v>
       </c>
       <c r="Q982" s="6">
-        <v>10896.35</v>
+        <v>8662.2999999999993</v>
       </c>
       <c r="R982" s="6" t="s">
         <v>23</v>
@@ -65558,7 +65585,7 @@
         <v>2239</v>
       </c>
       <c r="Q983" s="6">
-        <v>2815.1</v>
+        <v>2782.8</v>
       </c>
       <c r="R983" s="6" t="s">
         <v>23</v>
@@ -65617,7 +65644,7 @@
         <v>2242</v>
       </c>
       <c r="Q984" s="6">
-        <v>2831.3</v>
+        <v>2374.6999999999998</v>
       </c>
       <c r="R984" s="6" t="s">
         <v>23</v>
@@ -65735,7 +65762,7 @@
         <v>2248</v>
       </c>
       <c r="Q986" s="6">
-        <v>359.4</v>
+        <v>315.2</v>
       </c>
       <c r="R986" s="6" t="s">
         <v>23</v>
@@ -65794,7 +65821,7 @@
         <v>2251</v>
       </c>
       <c r="Q987" s="6">
-        <v>505.8</v>
+        <v>463.6</v>
       </c>
       <c r="R987" s="6" t="s">
         <v>23</v>
@@ -65853,7 +65880,7 @@
         <v>2254</v>
       </c>
       <c r="Q988" s="6">
-        <v>304</v>
+        <v>255</v>
       </c>
       <c r="R988" s="6" t="s">
         <v>23</v>
@@ -65912,7 +65939,7 @@
         <v>2257</v>
       </c>
       <c r="Q989" s="6">
-        <v>5707.35</v>
+        <v>5633.5</v>
       </c>
       <c r="R989" s="6" t="s">
         <v>23</v>
@@ -66089,7 +66116,7 @@
         <v>2266</v>
       </c>
       <c r="Q992" s="6">
-        <v>55.5</v>
+        <v>50.5</v>
       </c>
       <c r="R992" s="6" t="s">
         <v>23</v>
@@ -66148,7 +66175,7 @@
         <v>2269</v>
       </c>
       <c r="Q993" s="6">
-        <v>138.9</v>
+        <v>132.9</v>
       </c>
       <c r="R993" s="6" t="s">
         <v>23</v>
@@ -66207,7 +66234,7 @@
         <v>2275</v>
       </c>
       <c r="Q994" s="6">
-        <v>1180.57</v>
+        <v>235.2</v>
       </c>
       <c r="R994" s="6" t="s">
         <v>23</v>
@@ -66266,7 +66293,7 @@
         <v>2278</v>
       </c>
       <c r="Q995" s="6">
-        <v>1862.64</v>
+        <v>1539</v>
       </c>
       <c r="R995" s="6" t="s">
         <v>23</v>
@@ -66325,7 +66352,7 @@
         <v>2281</v>
       </c>
       <c r="Q996" s="6">
-        <v>555.01</v>
+        <v>385.4</v>
       </c>
       <c r="R996" s="6" t="s">
         <v>23</v>
@@ -66384,7 +66411,7 @@
         <v>2284</v>
       </c>
       <c r="Q997" s="6">
-        <v>24705.55</v>
+        <v>12593.3</v>
       </c>
       <c r="R997" s="6" t="s">
         <v>23</v>
@@ -66443,7 +66470,7 @@
         <v>2287</v>
       </c>
       <c r="Q998" s="6">
-        <v>43240.025970000002</v>
+        <v>48779.6</v>
       </c>
       <c r="R998" s="6" t="s">
         <v>23</v>
@@ -66502,7 +66529,7 @@
         <v>2290</v>
       </c>
       <c r="Q999" s="6">
-        <v>162.68</v>
+        <v>194.4</v>
       </c>
       <c r="R999" s="6" t="s">
         <v>23</v>
@@ -66561,7 +66588,7 @@
         <v>2293</v>
       </c>
       <c r="Q1000" s="6">
-        <v>13112.83</v>
+        <v>8026</v>
       </c>
       <c r="R1000" s="6" t="s">
         <v>23</v>
@@ -66620,7 +66647,7 @@
         <v>2296</v>
       </c>
       <c r="Q1001" s="6">
-        <v>113.09</v>
+        <v>9</v>
       </c>
       <c r="R1001" s="6" t="s">
         <v>23</v>
@@ -66679,7 +66706,7 @@
         <v>2299</v>
       </c>
       <c r="Q1002" s="6">
-        <v>2559.7399999999998</v>
+        <v>197</v>
       </c>
       <c r="R1002" s="6" t="s">
         <v>23</v>
@@ -66738,7 +66765,7 @@
         <v>2302</v>
       </c>
       <c r="Q1003" s="6">
-        <v>7103.55</v>
+        <v>3451</v>
       </c>
       <c r="R1003" s="6" t="s">
         <v>23</v>
@@ -66797,7 +66824,7 @@
         <v>2305</v>
       </c>
       <c r="Q1004" s="6">
-        <v>15.97</v>
+        <v>487.5</v>
       </c>
       <c r="R1004" s="6" t="s">
         <v>23</v>
@@ -66974,7 +67001,7 @@
         <v>2314</v>
       </c>
       <c r="Q1007" s="6">
-        <v>796.7</v>
+        <v>770.1</v>
       </c>
       <c r="R1007" s="6" t="s">
         <v>23</v>
@@ -67033,7 +67060,7 @@
         <v>2317</v>
       </c>
       <c r="Q1008" s="6">
-        <v>1014.84</v>
+        <v>88.2</v>
       </c>
       <c r="R1008" s="6" t="s">
         <v>23</v>
@@ -67092,7 +67119,7 @@
         <v>2320</v>
       </c>
       <c r="Q1009" s="6">
-        <v>22.06</v>
+        <v>24</v>
       </c>
       <c r="R1009" s="6" t="s">
         <v>23</v>
@@ -67210,7 +67237,7 @@
         <v>2332</v>
       </c>
       <c r="Q1011" s="6">
-        <v>264.02999999999997</v>
+        <v>232.6</v>
       </c>
       <c r="R1011" s="6" t="s">
         <v>23</v>
@@ -67251,7 +67278,7 @@
         <v>21</v>
       </c>
       <c r="K1012" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1012" s="6">
         <v>0</v>
@@ -67269,7 +67296,7 @@
         <v>2335</v>
       </c>
       <c r="Q1012" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R1012" s="6" t="s">
         <v>23</v>
@@ -67328,7 +67355,7 @@
         <v>2338</v>
       </c>
       <c r="Q1013" s="6">
-        <v>63.92</v>
+        <v>792.4</v>
       </c>
       <c r="R1013" s="6" t="s">
         <v>23</v>
@@ -67428,10 +67455,10 @@
         <v>21</v>
       </c>
       <c r="K1015" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1015" s="6">
-        <v>0</v>
+        <v>1.58</v>
       </c>
       <c r="M1015" s="6">
         <v>0</v>
@@ -67446,7 +67473,7 @@
         <v>2344</v>
       </c>
       <c r="Q1015" s="6">
-        <v>0</v>
+        <v>2145</v>
       </c>
       <c r="R1015" s="6" t="s">
         <v>23</v>
@@ -67490,7 +67517,7 @@
         <v>23</v>
       </c>
       <c r="L1016" s="6">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M1016" s="6">
         <v>0</v>
@@ -67505,7 +67532,7 @@
         <v>2347</v>
       </c>
       <c r="Q1016" s="6">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="R1016" s="6" t="s">
         <v>23</v>
@@ -67623,7 +67650,7 @@
         <v>2352</v>
       </c>
       <c r="Q1018" s="6">
-        <v>393.72</v>
+        <v>385.2</v>
       </c>
       <c r="R1018" s="6" t="s">
         <v>23</v>
@@ -67682,7 +67709,7 @@
         <v>2363</v>
       </c>
       <c r="Q1019" s="6">
-        <v>27.14</v>
+        <v>27</v>
       </c>
       <c r="R1019" s="6" t="s">
         <v>23</v>
@@ -67741,7 +67768,7 @@
         <v>2366</v>
       </c>
       <c r="Q1020" s="6">
-        <v>11.54</v>
+        <v>4</v>
       </c>
       <c r="R1020" s="6" t="s">
         <v>23</v>
@@ -67800,7 +67827,7 @@
         <v>2369</v>
       </c>
       <c r="Q1021" s="6">
-        <v>44.1</v>
+        <v>40</v>
       </c>
       <c r="R1021" s="6" t="s">
         <v>23</v>
@@ -67859,7 +67886,7 @@
         <v>2372</v>
       </c>
       <c r="Q1022" s="6">
-        <v>100.51</v>
+        <v>0</v>
       </c>
       <c r="R1022" s="6" t="s">
         <v>23</v>
@@ -67918,7 +67945,7 @@
         <v>2375</v>
       </c>
       <c r="Q1023" s="6">
-        <v>252.77</v>
+        <v>1149.4000000000001</v>
       </c>
       <c r="R1023" s="6" t="s">
         <v>23</v>
@@ -67929,16 +67956,16 @@
     </row>
     <row r="1024" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1024" s="5" t="s">
-        <v>2165</v>
+        <v>2377</v>
       </c>
       <c r="B1024" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1024" s="5" t="s">
-        <v>2166</v>
+        <v>2378</v>
       </c>
       <c r="D1024" s="5" t="s">
-        <v>2167</v>
+        <v>2379</v>
       </c>
       <c r="E1024" s="6" t="s">
         <v>23</v>
@@ -67959,10 +67986,10 @@
         <v>21</v>
       </c>
       <c r="K1024" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L1024" s="6">
-        <v>1.98</v>
+        <v>0</v>
       </c>
       <c r="M1024" s="6">
         <v>0</v>
@@ -67974,10 +68001,10 @@
         <v>21</v>
       </c>
       <c r="P1024" s="5" t="s">
-        <v>2166</v>
+        <v>2378</v>
       </c>
       <c r="Q1024" s="6">
-        <v>560.70000000000005</v>
+        <v>0</v>
       </c>
       <c r="R1024" s="6" t="s">
         <v>23</v>
@@ -67988,16 +68015,16 @@
     </row>
     <row r="1025" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1025" s="5" t="s">
-        <v>2168</v>
+        <v>2380</v>
       </c>
       <c r="B1025" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1025" s="5" t="s">
-        <v>2169</v>
+        <v>2381</v>
       </c>
       <c r="D1025" s="5" t="s">
-        <v>2170</v>
+        <v>2382</v>
       </c>
       <c r="E1025" s="6" t="s">
         <v>23</v>
@@ -68018,10 +68045,10 @@
         <v>21</v>
       </c>
       <c r="K1025" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L1025" s="6">
-        <v>3.02</v>
+        <v>0</v>
       </c>
       <c r="M1025" s="6">
         <v>0</v>
@@ -68033,10 +68060,10 @@
         <v>21</v>
       </c>
       <c r="P1025" s="5" t="s">
-        <v>2169</v>
+        <v>2381</v>
       </c>
       <c r="Q1025" s="6">
-        <v>60.4</v>
+        <v>0</v>
       </c>
       <c r="R1025" s="6" t="s">
         <v>23</v>
@@ -68047,16 +68074,16 @@
     </row>
     <row r="1026" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1026" s="5" t="s">
-        <v>2171</v>
+        <v>2383</v>
       </c>
       <c r="B1026" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1026" s="5" t="s">
-        <v>2172</v>
+        <v>2384</v>
       </c>
       <c r="D1026" s="5" t="s">
-        <v>2173</v>
+        <v>2385</v>
       </c>
       <c r="E1026" s="6" t="s">
         <v>23</v>
@@ -68077,10 +68104,10 @@
         <v>21</v>
       </c>
       <c r="K1026" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L1026" s="6">
-        <v>2.65</v>
+        <v>0</v>
       </c>
       <c r="M1026" s="6">
         <v>0</v>
@@ -68092,10 +68119,10 @@
         <v>21</v>
       </c>
       <c r="P1026" s="5" t="s">
-        <v>2172</v>
+        <v>2384</v>
       </c>
       <c r="Q1026" s="6">
-        <v>1022.9</v>
+        <v>0</v>
       </c>
       <c r="R1026" s="6" t="s">
         <v>23</v>
@@ -68106,16 +68133,16 @@
     </row>
     <row r="1027" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1027" s="5" t="s">
-        <v>2189</v>
+        <v>2165</v>
       </c>
       <c r="B1027" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1027" s="5" t="s">
-        <v>2190</v>
+        <v>2166</v>
       </c>
       <c r="D1027" s="5" t="s">
-        <v>2191</v>
+        <v>2167</v>
       </c>
       <c r="E1027" s="6" t="s">
         <v>23</v>
@@ -68136,10 +68163,10 @@
         <v>21</v>
       </c>
       <c r="K1027" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1027" s="6">
-        <v>0</v>
+        <v>1.98</v>
       </c>
       <c r="M1027" s="6">
         <v>0</v>
@@ -68151,10 +68178,10 @@
         <v>21</v>
       </c>
       <c r="P1027" s="5" t="s">
-        <v>2190</v>
+        <v>2166</v>
       </c>
       <c r="Q1027" s="6">
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="R1027" s="6" t="s">
         <v>23</v>
@@ -68165,16 +68192,16 @@
     </row>
     <row r="1028" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1028" s="5" t="s">
-        <v>2192</v>
+        <v>2168</v>
       </c>
       <c r="B1028" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1028" s="5" t="s">
-        <v>2193</v>
+        <v>2169</v>
       </c>
       <c r="D1028" s="5" t="s">
-        <v>2194</v>
+        <v>2170</v>
       </c>
       <c r="E1028" s="6" t="s">
         <v>23</v>
@@ -68195,10 +68222,10 @@
         <v>21</v>
       </c>
       <c r="K1028" s="6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="L1028" s="6">
-        <v>0</v>
+        <v>3.02</v>
       </c>
       <c r="M1028" s="6">
         <v>0</v>
@@ -68210,10 +68237,10 @@
         <v>21</v>
       </c>
       <c r="P1028" s="5" t="s">
-        <v>2193</v>
+        <v>2169</v>
       </c>
       <c r="Q1028" s="6">
-        <v>0</v>
+        <v>49.4</v>
       </c>
       <c r="R1028" s="6" t="s">
         <v>23</v>
@@ -68224,16 +68251,16 @@
     </row>
     <row r="1029" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1029" s="5" t="s">
-        <v>2322</v>
+        <v>2171</v>
       </c>
       <c r="B1029" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1029" s="5" t="s">
-        <v>2323</v>
+        <v>2172</v>
       </c>
       <c r="D1029" s="5" t="s">
-        <v>2324</v>
+        <v>2173</v>
       </c>
       <c r="E1029" s="6" t="s">
         <v>23</v>
@@ -68269,10 +68296,10 @@
         <v>21</v>
       </c>
       <c r="P1029" s="5" t="s">
-        <v>2323</v>
+        <v>2172</v>
       </c>
       <c r="Q1029" s="6">
-        <v>239.08</v>
+        <v>1024.9000000000001</v>
       </c>
       <c r="R1029" s="6" t="s">
         <v>23</v>
@@ -68283,16 +68310,16 @@
     </row>
     <row r="1030" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1030" s="5" t="s">
-        <v>2325</v>
+        <v>2189</v>
       </c>
       <c r="B1030" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C1030" s="5" t="s">
-        <v>2326</v>
+        <v>2190</v>
       </c>
       <c r="D1030" s="5" t="s">
-        <v>2327</v>
+        <v>2191</v>
       </c>
       <c r="E1030" s="6" t="s">
         <v>23</v>
@@ -68313,10 +68340,10 @@
         <v>21</v>
       </c>
       <c r="K1030" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="L1030" s="6">
-        <v>4.1500000000000004</v>
+        <v>0</v>
       </c>
       <c r="M1030" s="6">
         <v>0</v>
@@ -68328,10 +68355,10 @@
         <v>21</v>
       </c>
       <c r="P1030" s="5" t="s">
-        <v>2326</v>
+        <v>2190</v>
       </c>
       <c r="Q1030" s="6">
-        <v>156.21</v>
+        <v>0</v>
       </c>
       <c r="R1030" s="6" t="s">
         <v>23</v>
@@ -68342,60 +68369,237 @@
     </row>
     <row r="1031" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1031" s="5" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B1031" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1031" s="5" t="s">
+        <v>2193</v>
+      </c>
+      <c r="D1031" s="5" t="s">
+        <v>2194</v>
+      </c>
+      <c r="E1031" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1031" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1031" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1031" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1031" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1031" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1031" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1031" s="6">
+        <v>0</v>
+      </c>
+      <c r="M1031" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1031" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1031" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1031" s="5" t="s">
+        <v>2193</v>
+      </c>
+      <c r="Q1031" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1031" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1031" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1032" s="5" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B1032" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1032" s="5" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D1032" s="5" t="s">
+        <v>2324</v>
+      </c>
+      <c r="E1032" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1032" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1032" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1032" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1032" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1032" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1032" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1032" s="6">
+        <v>2.65</v>
+      </c>
+      <c r="M1032" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1032" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1032" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1032" s="5" t="s">
+        <v>2323</v>
+      </c>
+      <c r="Q1032" s="6">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="R1032" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1032" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1033" s="5" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B1033" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1033" s="5" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D1033" s="5" t="s">
+        <v>2327</v>
+      </c>
+      <c r="E1033" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1033" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1033" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1033" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1033" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1033" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1033" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1033" s="6">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="M1033" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1033" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1033" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1033" s="5" t="s">
+        <v>2326</v>
+      </c>
+      <c r="Q1033" s="6">
+        <v>153.30000000000001</v>
+      </c>
+      <c r="R1033" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1033" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1034" s="5" t="s">
         <v>2354</v>
       </c>
-      <c r="B1031" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1031" s="5" t="s">
+      <c r="B1034" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1034" s="5" t="s">
         <v>2355</v>
       </c>
-      <c r="D1031" s="5" t="s">
+      <c r="D1034" s="5" t="s">
         <v>2356</v>
       </c>
-      <c r="E1031" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1031" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1031" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1031" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1031" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1031" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1031" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1031" s="6">
+      <c r="E1034" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1034" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1034" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1034" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1034" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1034" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1034" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1034" s="6">
         <v>4.2</v>
       </c>
-      <c r="M1031" s="6">
-        <v>0</v>
-      </c>
-      <c r="N1031" s="6">
-        <v>0</v>
-      </c>
-      <c r="O1031" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1031" s="5" t="s">
+      <c r="M1034" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1034" s="6">
+        <v>0</v>
+      </c>
+      <c r="O1034" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1034" s="5" t="s">
         <v>2355</v>
       </c>
-      <c r="Q1031" s="6">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="R1031" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1031" s="5" t="s">
+      <c r="Q1034" s="6">
+        <v>0</v>
+      </c>
+      <c r="R1034" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1034" s="5" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>